<commit_message>
it currently works and creates an excel with the data we're looking for.
</commit_message>
<xml_diff>
--- a/combined_dataframes.xlsx
+++ b/combined_dataframes.xlsx
@@ -10,13 +10,15 @@
     <sheet name="Materials" sheetId="1" r:id="rId1"/>
     <sheet name="Samples" sheetId="2" r:id="rId2"/>
     <sheet name="Standard Deviations" sheetId="3" r:id="rId3"/>
+    <sheet name="Absorbance Material" sheetId="4" r:id="rId4"/>
+    <sheet name="Absorbance Sample" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="146">
   <si>
     <t>Wavelength</t>
   </si>
@@ -3996,4 +3998,2485 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:AC7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:29">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0.1091032787514837</v>
+      </c>
+      <c r="C2">
+        <v>0.1101816761276027</v>
+      </c>
+      <c r="D2">
+        <v>0.02741273299404127</v>
+      </c>
+      <c r="E2">
+        <v>0.1180603826647182</v>
+      </c>
+      <c r="F2">
+        <v>0.1971650202481618</v>
+      </c>
+      <c r="G2">
+        <v>0.2568725770218377</v>
+      </c>
+      <c r="H2">
+        <v>0.1527637526862227</v>
+      </c>
+      <c r="I2">
+        <v>0.3310160310405767</v>
+      </c>
+      <c r="J2">
+        <v>0.4226856392910123</v>
+      </c>
+      <c r="K2">
+        <v>0.5406774829821425</v>
+      </c>
+      <c r="L2">
+        <v>0.6199774313573367</v>
+      </c>
+      <c r="M2">
+        <v>0.9667226091397561</v>
+      </c>
+      <c r="N2">
+        <v>1.071864830461241</v>
+      </c>
+      <c r="O2">
+        <v>0.6623277337807519</v>
+      </c>
+      <c r="P2">
+        <v>1.103874344692192</v>
+      </c>
+      <c r="Q2">
+        <v>1.08185466692754</v>
+      </c>
+      <c r="R2">
+        <v>1.132474218027037</v>
+      </c>
+      <c r="S2">
+        <v>0.6776275958351473</v>
+      </c>
+      <c r="T2">
+        <v>1.102915602939393</v>
+      </c>
+      <c r="U2">
+        <v>1.257876888228906</v>
+      </c>
+      <c r="V2">
+        <v>1.524035159648379</v>
+      </c>
+      <c r="W2">
+        <v>0.947323714538376</v>
+      </c>
+      <c r="X2">
+        <v>1.623776114922772</v>
+      </c>
+      <c r="Y2">
+        <v>1.673470685028914</v>
+      </c>
+      <c r="Z2">
+        <v>0.7745266666654831</v>
+      </c>
+      <c r="AA2">
+        <v>1.789368583984428</v>
+      </c>
+      <c r="AB2">
+        <v>1.868469770158993</v>
+      </c>
+      <c r="AC2">
+        <v>0.3496328657293818</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>0.1065248613707963</v>
+      </c>
+      <c r="C3">
+        <v>0.1141159770063213</v>
+      </c>
+      <c r="D3">
+        <v>0.0262091357323121</v>
+      </c>
+      <c r="E3">
+        <v>0.1105868532978474</v>
+      </c>
+      <c r="F3">
+        <v>0.1842595514100371</v>
+      </c>
+      <c r="G3">
+        <v>0.2409665056731912</v>
+      </c>
+      <c r="H3">
+        <v>0.1559882252553818</v>
+      </c>
+      <c r="I3">
+        <v>0.3100647834838206</v>
+      </c>
+      <c r="J3">
+        <v>0.3967371912363383</v>
+      </c>
+      <c r="K3">
+        <v>0.5261091306312111</v>
+      </c>
+      <c r="L3">
+        <v>0.6086500885306875</v>
+      </c>
+      <c r="M3">
+        <v>0.9317318787692025</v>
+      </c>
+      <c r="N3">
+        <v>1.060054965353013</v>
+      </c>
+      <c r="O3">
+        <v>0.6428777725291057</v>
+      </c>
+      <c r="P3">
+        <v>1.063555030082388</v>
+      </c>
+      <c r="Q3">
+        <v>1.047930608081077</v>
+      </c>
+      <c r="R3">
+        <v>1.091167185846077</v>
+      </c>
+      <c r="S3">
+        <v>0.6580900111495951</v>
+      </c>
+      <c r="T3">
+        <v>1.062500997870782</v>
+      </c>
+      <c r="U3">
+        <v>1.231580949784416</v>
+      </c>
+      <c r="V3">
+        <v>1.471728759625167</v>
+      </c>
+      <c r="W3">
+        <v>0.9186556038780315</v>
+      </c>
+      <c r="X3">
+        <v>1.591855118739844</v>
+      </c>
+      <c r="Y3">
+        <v>1.633544391150927</v>
+      </c>
+      <c r="Z3">
+        <v>0.7552838139763814</v>
+      </c>
+      <c r="AA3">
+        <v>1.744549079472522</v>
+      </c>
+      <c r="AB3">
+        <v>1.825834434720153</v>
+      </c>
+      <c r="AC3">
+        <v>0.3280596922560227</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>0.1020898253374901</v>
+      </c>
+      <c r="C4">
+        <v>0.1160811511517312</v>
+      </c>
+      <c r="D4">
+        <v>0.03309911453127855</v>
+      </c>
+      <c r="E4">
+        <v>0.1106021758022038</v>
+      </c>
+      <c r="F4">
+        <v>0.1856046420871866</v>
+      </c>
+      <c r="G4">
+        <v>0.2385857584304371</v>
+      </c>
+      <c r="H4">
+        <v>0.1701105787892694</v>
+      </c>
+      <c r="I4">
+        <v>0.3175301142925238</v>
+      </c>
+      <c r="J4">
+        <v>0.4127586454760483</v>
+      </c>
+      <c r="K4">
+        <v>0.5536811362301561</v>
+      </c>
+      <c r="L4">
+        <v>0.6262907492598118</v>
+      </c>
+      <c r="M4">
+        <v>0.9451956914934021</v>
+      </c>
+      <c r="N4">
+        <v>1.075420750105125</v>
+      </c>
+      <c r="O4">
+        <v>0.6764117477818518</v>
+      </c>
+      <c r="P4">
+        <v>1.119956499461221</v>
+      </c>
+      <c r="Q4">
+        <v>1.106178038515265</v>
+      </c>
+      <c r="R4">
+        <v>1.13245424365302</v>
+      </c>
+      <c r="S4">
+        <v>0.6788729504973916</v>
+      </c>
+      <c r="T4">
+        <v>1.115583639000869</v>
+      </c>
+      <c r="U4">
+        <v>1.289063642109349</v>
+      </c>
+      <c r="V4">
+        <v>1.556285665468272</v>
+      </c>
+      <c r="W4">
+        <v>0.9540318256533921</v>
+      </c>
+      <c r="X4">
+        <v>1.691181858761334</v>
+      </c>
+      <c r="Y4">
+        <v>1.749800362682512</v>
+      </c>
+      <c r="Z4">
+        <v>0.7769723148426648</v>
+      </c>
+      <c r="AA4">
+        <v>1.854703786777249</v>
+      </c>
+      <c r="AB4">
+        <v>1.953347187822582</v>
+      </c>
+      <c r="AC4">
+        <v>0.3536839970022914</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29">
+      <c r="A5">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>0.1599624977141008</v>
+      </c>
+      <c r="C5">
+        <v>0.1549443537356876</v>
+      </c>
+      <c r="D5">
+        <v>0.04228221841153366</v>
+      </c>
+      <c r="E5">
+        <v>0.1582341396406156</v>
+      </c>
+      <c r="F5">
+        <v>0.2417216944401548</v>
+      </c>
+      <c r="G5">
+        <v>0.3129857256943832</v>
+      </c>
+      <c r="H5">
+        <v>0.1623589290157654</v>
+      </c>
+      <c r="I5">
+        <v>0.3841300182971971</v>
+      </c>
+      <c r="J5">
+        <v>0.4637459682559456</v>
+      </c>
+      <c r="K5">
+        <v>0.5978837406411646</v>
+      </c>
+      <c r="L5">
+        <v>0.610313468099947</v>
+      </c>
+      <c r="M5">
+        <v>1.0250397916582</v>
+      </c>
+      <c r="N5">
+        <v>1.122005416909158</v>
+      </c>
+      <c r="O5">
+        <v>0.6694403468784057</v>
+      </c>
+      <c r="P5">
+        <v>1.172737239856142</v>
+      </c>
+      <c r="Q5">
+        <v>1.15173315119782</v>
+      </c>
+      <c r="R5">
+        <v>1.162216719192099</v>
+      </c>
+      <c r="S5">
+        <v>0.6756797871111998</v>
+      </c>
+      <c r="T5">
+        <v>1.15412976740858</v>
+      </c>
+      <c r="U5">
+        <v>1.301905632800824</v>
+      </c>
+      <c r="V5">
+        <v>1.596075283413903</v>
+      </c>
+      <c r="W5">
+        <v>1.015285035601363</v>
+      </c>
+      <c r="X5">
+        <v>1.709077309482693</v>
+      </c>
+      <c r="Y5">
+        <v>1.781046231835997</v>
+      </c>
+      <c r="Z5">
+        <v>0.8355139900344872</v>
+      </c>
+      <c r="AA5">
+        <v>1.909531034931402</v>
+      </c>
+      <c r="AB5">
+        <v>2.010729426263379</v>
+      </c>
+      <c r="AC5">
+        <v>0.3987581227923139</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29">
+      <c r="A6">
+        <v>0</v>
+      </c>
+      <c r="B6">
+        <v>0.09885921131259251</v>
+      </c>
+      <c r="C6">
+        <v>0.1078691868591891</v>
+      </c>
+      <c r="D6">
+        <v>0.04677974162968777</v>
+      </c>
+      <c r="E6">
+        <v>0.1203978287893512</v>
+      </c>
+      <c r="F6">
+        <v>0.1723363178817414</v>
+      </c>
+      <c r="G6">
+        <v>0.2395157272837175</v>
+      </c>
+      <c r="H6">
+        <v>0.1666955948467023</v>
+      </c>
+      <c r="I6">
+        <v>0.3228584220772007</v>
+      </c>
+      <c r="J6">
+        <v>0.3975796067863022</v>
+      </c>
+      <c r="K6">
+        <v>0.5518114607652178</v>
+      </c>
+      <c r="L6">
+        <v>0.6079345442989547</v>
+      </c>
+      <c r="M6">
+        <v>0.9057516722434528</v>
+      </c>
+      <c r="N6">
+        <v>0.9902980475907769</v>
+      </c>
+      <c r="O6">
+        <v>0.6390556885676887</v>
+      </c>
+      <c r="P6">
+        <v>1.02600371494347</v>
+      </c>
+      <c r="Q6">
+        <v>1.005215255941397</v>
+      </c>
+      <c r="R6">
+        <v>1.021519532261951</v>
+      </c>
+      <c r="S6">
+        <v>0.6531380872264289</v>
+      </c>
+      <c r="T6">
+        <v>1.031185390078135</v>
+      </c>
+      <c r="U6">
+        <v>1.168228170104673</v>
+      </c>
+      <c r="V6">
+        <v>1.462199316919897</v>
+      </c>
+      <c r="W6">
+        <v>0.9255202102402511</v>
+      </c>
+      <c r="X6">
+        <v>1.483586743380633</v>
+      </c>
+      <c r="Y6">
+        <v>1.622920436767506</v>
+      </c>
+      <c r="Z6">
+        <v>0.7517312001947793</v>
+      </c>
+      <c r="AA6">
+        <v>1.724830633510442</v>
+      </c>
+      <c r="AB6">
+        <v>1.74616002108639</v>
+      </c>
+      <c r="AC6">
+        <v>0.3449175146224282</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29">
+      <c r="A7">
+        <v>0</v>
+      </c>
+      <c r="B7">
+        <v>0.1461600070381094</v>
+      </c>
+      <c r="C7">
+        <v>0.1417556465953067</v>
+      </c>
+      <c r="D7">
+        <v>0.04642783725400321</v>
+      </c>
+      <c r="E7">
+        <v>0.1640492833022129</v>
+      </c>
+      <c r="F7">
+        <v>0.2478341141480356</v>
+      </c>
+      <c r="G7">
+        <v>0.2719387859520953</v>
+      </c>
+      <c r="H7">
+        <v>0.2087689465084316</v>
+      </c>
+      <c r="I7">
+        <v>0.4002275820371259</v>
+      </c>
+      <c r="J7">
+        <v>0.5091136356686438</v>
+      </c>
+      <c r="K7">
+        <v>0.6156866824518425</v>
+      </c>
+      <c r="L7">
+        <v>0.7799711349839066</v>
+      </c>
+      <c r="M7">
+        <v>1.179799416265034</v>
+      </c>
+      <c r="N7">
+        <v>1.452354802479325</v>
+      </c>
+      <c r="O7">
+        <v>0.8551849957880159</v>
+      </c>
+      <c r="P7">
+        <v>1.450847554321722</v>
+      </c>
+      <c r="Q7">
+        <v>1.450527234440926</v>
+      </c>
+      <c r="R7">
+        <v>1.428536083645852</v>
+      </c>
+      <c r="S7">
+        <v>0.8406045818969866</v>
+      </c>
+      <c r="T7">
+        <v>1.444643536698521</v>
+      </c>
+      <c r="U7">
+        <v>1.733011419134605</v>
+      </c>
+      <c r="V7">
+        <v>2.38870893597383</v>
+      </c>
+      <c r="W7">
+        <v>1.285816317118114</v>
+      </c>
+      <c r="X7">
+        <v>2.417209374242582</v>
+      </c>
+      <c r="Y7">
+        <v>2.740654052592297</v>
+      </c>
+      <c r="Z7">
+        <v>1.00776014472243</v>
+      </c>
+      <c r="AA7">
+        <v>3.21325846353809</v>
+      </c>
+      <c r="AB7">
+        <v>3.732407623899116</v>
+      </c>
+      <c r="AC7">
+        <v>0.4325244194631127</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:CI7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:87">
+      <c r="A1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AT1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AU1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AV1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AW1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AX1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AY1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AZ1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="BA1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="BB1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="BC1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="BD1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="BE1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="BF1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="BG1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="BH1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="BI1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="BJ1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="BK1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="BL1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="BM1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="BN1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="BO1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="BP1" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="BQ1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="BR1" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="BS1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="BT1" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="BU1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="BV1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="BW1" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="BX1" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="BY1" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="BZ1" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="CA1" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="CB1" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="CC1" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="CD1" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="CE1" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="CF1" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="CG1" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="CH1" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="CI1" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="2" spans="1:87">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0.06795099732174277</v>
+      </c>
+      <c r="C2">
+        <v>0.08185805465480191</v>
+      </c>
+      <c r="D2">
+        <v>0.1545338928394538</v>
+      </c>
+      <c r="E2">
+        <v>0.1595285979578524</v>
+      </c>
+      <c r="F2">
+        <v>0.1611356300105169</v>
+      </c>
+      <c r="G2">
+        <v>0.1657440760914083</v>
+      </c>
+      <c r="H2">
+        <v>0.1522321958209901</v>
+      </c>
+      <c r="I2">
+        <v>0.1604916017349513</v>
+      </c>
+      <c r="J2">
+        <v>0.1120118472991535</v>
+      </c>
+      <c r="K2">
+        <v>0.1194300125897388</v>
+      </c>
+      <c r="L2">
+        <v>0.002974758985301182</v>
+      </c>
+      <c r="M2">
+        <v>0.1121004179217738</v>
+      </c>
+      <c r="N2">
+        <v>0.1913025001408202</v>
+      </c>
+      <c r="O2">
+        <v>0.2010557087478083</v>
+      </c>
+      <c r="P2">
+        <v>0.1945269807809258</v>
+      </c>
+      <c r="Q2">
+        <v>0.2779525147030378</v>
+      </c>
+      <c r="R2">
+        <v>0.2690071736811264</v>
+      </c>
+      <c r="S2">
+        <v>0.2716118830993711</v>
+      </c>
+      <c r="T2">
+        <v>0.3176560953365489</v>
+      </c>
+      <c r="U2">
+        <v>0.3301819559422958</v>
+      </c>
+      <c r="V2">
+        <v>0.3131392511907007</v>
+      </c>
+      <c r="W2">
+        <v>0.001330261400455145</v>
+      </c>
+      <c r="X2">
+        <v>0.3266598543948022</v>
+      </c>
+      <c r="Y2">
+        <v>0.3319231269399354</v>
+      </c>
+      <c r="Z2">
+        <v>0.33346493110568</v>
+      </c>
+      <c r="AA2">
+        <v>0.4829306993669014</v>
+      </c>
+      <c r="AB2">
+        <v>0.4898524009478926</v>
+      </c>
+      <c r="AC2">
+        <v>0.4896019436102285</v>
+      </c>
+      <c r="AD2">
+        <v>0.4373970654521983</v>
+      </c>
+      <c r="AE2">
+        <v>0.4306792180796415</v>
+      </c>
+      <c r="AF2">
+        <v>0.4277006167351722</v>
+      </c>
+      <c r="AG2">
+        <v>1.01899263158486</v>
+      </c>
+      <c r="AH2">
+        <v>0.1995119506017013</v>
+      </c>
+      <c r="AI2">
+        <v>1.026949115133777</v>
+      </c>
+      <c r="AJ2">
+        <v>1.024379418627245</v>
+      </c>
+      <c r="AK2">
+        <v>1.013984726349174</v>
+      </c>
+      <c r="AL2">
+        <v>1.016103755226842</v>
+      </c>
+      <c r="AM2">
+        <v>1.017959728441051</v>
+      </c>
+      <c r="AN2">
+        <v>1.12178981811764</v>
+      </c>
+      <c r="AO2">
+        <v>1.128846836013933</v>
+      </c>
+      <c r="AP2">
+        <v>1.112898153439635</v>
+      </c>
+      <c r="AQ2">
+        <v>1.108901319659735</v>
+      </c>
+      <c r="AR2">
+        <v>1.107784533644136</v>
+      </c>
+      <c r="AS2">
+        <v>0.2078434700802005</v>
+      </c>
+      <c r="AT2">
+        <v>1.126976540244029</v>
+      </c>
+      <c r="AU2">
+        <v>1.15642433072145</v>
+      </c>
+      <c r="AV2">
+        <v>1.176725201038425</v>
+      </c>
+      <c r="AW2">
+        <v>1.144612984295044</v>
+      </c>
+      <c r="AX2">
+        <v>1.131278282202457</v>
+      </c>
+      <c r="AY2">
+        <v>1.117729844113085</v>
+      </c>
+      <c r="AZ2">
+        <v>1.116643994309363</v>
+      </c>
+      <c r="BA2">
+        <v>1.212702435619046</v>
+      </c>
+      <c r="BB2">
+        <v>1.21928876747057</v>
+      </c>
+      <c r="BC2">
+        <v>1.210609183259514</v>
+      </c>
+      <c r="BD2">
+        <v>0.204715584709188</v>
+      </c>
+      <c r="BE2">
+        <v>1.086805281829825</v>
+      </c>
+      <c r="BF2">
+        <v>1.084310676819978</v>
+      </c>
+      <c r="BG2">
+        <v>1.076349440387174</v>
+      </c>
+      <c r="BH2">
+        <v>1.313627091948996</v>
+      </c>
+      <c r="BI2">
+        <v>1.306779881285925</v>
+      </c>
+      <c r="BJ2">
+        <v>1.313414825429418</v>
+      </c>
+      <c r="BK2">
+        <v>1.301348894529031</v>
+      </c>
+      <c r="BL2">
+        <v>1.3051761215023</v>
+      </c>
+      <c r="BM2">
+        <v>1.317076515764124</v>
+      </c>
+      <c r="BN2">
+        <v>2.488672286634736</v>
+      </c>
+      <c r="BO2">
+        <v>0.06283595561770416</v>
+      </c>
+      <c r="BP2">
+        <v>2.474974116374596</v>
+      </c>
+      <c r="BQ2">
+        <v>2.475548528763476</v>
+      </c>
+      <c r="BR2">
+        <v>1.677426607305108</v>
+      </c>
+      <c r="BS2">
+        <v>1.681449415043503</v>
+      </c>
+      <c r="BT2">
+        <v>1.660453162689851</v>
+      </c>
+      <c r="BU2">
+        <v>1.714476497547774</v>
+      </c>
+      <c r="BV2">
+        <v>1.765027021071516</v>
+      </c>
+      <c r="BW2">
+        <v>1.690234886541741</v>
+      </c>
+      <c r="BX2">
+        <v>1.701908530833132</v>
+      </c>
+      <c r="BY2">
+        <v>1.704198085567938</v>
+      </c>
+      <c r="BZ2">
+        <v>0.04918456893420017</v>
+      </c>
+      <c r="CA2">
+        <v>1.687194530989987</v>
+      </c>
+      <c r="CB2">
+        <v>1.919785367810857</v>
+      </c>
+      <c r="CC2">
+        <v>1.928167274677659</v>
+      </c>
+      <c r="CD2">
+        <v>1.907916940354473</v>
+      </c>
+      <c r="CE2">
+        <v>1.919215747486826</v>
+      </c>
+      <c r="CF2">
+        <v>1.926238552017087</v>
+      </c>
+      <c r="CG2">
+        <v>1.912777983247811</v>
+      </c>
+      <c r="CH2">
+        <v>0.0614402292893785</v>
+      </c>
+      <c r="CI2">
+        <v>0.07791362787603238</v>
+      </c>
+    </row>
+    <row r="3" spans="1:87">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>0.06254309411229172</v>
+      </c>
+      <c r="C3">
+        <v>0.05785678103512904</v>
+      </c>
+      <c r="D3">
+        <v>0.1433899630497707</v>
+      </c>
+      <c r="E3">
+        <v>0.1483169813843757</v>
+      </c>
+      <c r="F3">
+        <v>0.1470527193014075</v>
+      </c>
+      <c r="G3">
+        <v>0.1496672710642195</v>
+      </c>
+      <c r="H3">
+        <v>0.1540524273499986</v>
+      </c>
+      <c r="I3">
+        <v>0.1578234254181533</v>
+      </c>
+      <c r="J3">
+        <v>0.1037213976898729</v>
+      </c>
+      <c r="K3">
+        <v>0.09495811317170584</v>
+      </c>
+      <c r="L3">
+        <v>0.002315853507733548</v>
+      </c>
+      <c r="M3">
+        <v>0.1011536916548215</v>
+      </c>
+      <c r="N3">
+        <v>0.1789797946206727</v>
+      </c>
+      <c r="O3">
+        <v>0.1726894573919343</v>
+      </c>
+      <c r="P3">
+        <v>0.1738728165946373</v>
+      </c>
+      <c r="Q3">
+        <v>0.2525142444596454</v>
+      </c>
+      <c r="R3">
+        <v>0.2475249976218991</v>
+      </c>
+      <c r="S3">
+        <v>0.255713639650946</v>
+      </c>
+      <c r="T3">
+        <v>0.2928322070710072</v>
+      </c>
+      <c r="U3">
+        <v>0.2940084387592624</v>
+      </c>
+      <c r="V3">
+        <v>0.3137637401213069</v>
+      </c>
+      <c r="W3">
+        <v>0.001869700701004347</v>
+      </c>
+      <c r="X3">
+        <v>0.3039233660583848</v>
+      </c>
+      <c r="Y3">
+        <v>0.3002289262914682</v>
+      </c>
+      <c r="Z3">
+        <v>0.3078415998742265</v>
+      </c>
+      <c r="AA3">
+        <v>0.4481233899072491</v>
+      </c>
+      <c r="AB3">
+        <v>0.4463180747955694</v>
+      </c>
+      <c r="AC3">
+        <v>0.4585852651378226</v>
+      </c>
+      <c r="AD3">
+        <v>0.4052696777173711</v>
+      </c>
+      <c r="AE3">
+        <v>0.4086558333297102</v>
+      </c>
+      <c r="AF3">
+        <v>0.4067019442358616</v>
+      </c>
+      <c r="AG3">
+        <v>0.985449928045534</v>
+      </c>
+      <c r="AH3">
+        <v>0.1928535557583117</v>
+      </c>
+      <c r="AI3">
+        <v>0.9940083474749077</v>
+      </c>
+      <c r="AJ3">
+        <v>0.9835278215611972</v>
+      </c>
+      <c r="AK3">
+        <v>0.953755380326761</v>
+      </c>
+      <c r="AL3">
+        <v>0.9819740242282641</v>
+      </c>
+      <c r="AM3">
+        <v>0.9788849928641112</v>
+      </c>
+      <c r="AN3">
+        <v>1.10425467251388</v>
+      </c>
+      <c r="AO3">
+        <v>1.098594181794953</v>
+      </c>
+      <c r="AP3">
+        <v>1.096510620778534</v>
+      </c>
+      <c r="AQ3">
+        <v>1.065805080491945</v>
+      </c>
+      <c r="AR3">
+        <v>1.065646616280369</v>
+      </c>
+      <c r="AS3">
+        <v>0.1900194398218211</v>
+      </c>
+      <c r="AT3">
+        <v>1.074111195167979</v>
+      </c>
+      <c r="AU3">
+        <v>1.123957093707858</v>
+      </c>
+      <c r="AV3">
+        <v>1.11245921217335</v>
+      </c>
+      <c r="AW3">
+        <v>1.105008508231081</v>
+      </c>
+      <c r="AX3">
+        <v>1.075295965202646</v>
+      </c>
+      <c r="AY3">
+        <v>1.082903579075164</v>
+      </c>
+      <c r="AZ3">
+        <v>1.083910664160616</v>
+      </c>
+      <c r="BA3">
+        <v>1.156531424687362</v>
+      </c>
+      <c r="BB3">
+        <v>1.153948784082036</v>
+      </c>
+      <c r="BC3">
+        <v>1.174401777410012</v>
+      </c>
+      <c r="BD3">
+        <v>0.1833590955163211</v>
+      </c>
+      <c r="BE3">
+        <v>1.045432144962698</v>
+      </c>
+      <c r="BF3">
+        <v>1.029427607496673</v>
+      </c>
+      <c r="BG3">
+        <v>1.037962699501496</v>
+      </c>
+      <c r="BH3">
+        <v>1.255249383946394</v>
+      </c>
+      <c r="BI3">
+        <v>1.288895485521961</v>
+      </c>
+      <c r="BJ3">
+        <v>1.265233471629128</v>
+      </c>
+      <c r="BK3">
+        <v>1.260028518855096</v>
+      </c>
+      <c r="BL3">
+        <v>1.254994352563541</v>
+      </c>
+      <c r="BM3">
+        <v>1.245648968037489</v>
+      </c>
+      <c r="BN3">
+        <v>2.419851279703033</v>
+      </c>
+      <c r="BO3">
+        <v>0.0320701584753309</v>
+      </c>
+      <c r="BP3">
+        <v>2.389803366704771</v>
+      </c>
+      <c r="BQ3">
+        <v>2.402928895117701</v>
+      </c>
+      <c r="BR3">
+        <v>1.63023505717894</v>
+      </c>
+      <c r="BS3">
+        <v>1.651122404539787</v>
+      </c>
+      <c r="BT3">
+        <v>1.613737177433537</v>
+      </c>
+      <c r="BU3">
+        <v>1.660786902927901</v>
+      </c>
+      <c r="BV3">
+        <v>1.683014039654155</v>
+      </c>
+      <c r="BW3">
+        <v>1.676140434024832</v>
+      </c>
+      <c r="BX3">
+        <v>1.660140996320911</v>
+      </c>
+      <c r="BY3">
+        <v>1.634348831846555</v>
+      </c>
+      <c r="BZ3">
+        <v>0.03093495153954072</v>
+      </c>
+      <c r="CA3">
+        <v>1.628704209351442</v>
+      </c>
+      <c r="CB3">
+        <v>1.876055044353057</v>
+      </c>
+      <c r="CC3">
+        <v>1.868342932769132</v>
+      </c>
+      <c r="CD3">
+        <v>1.875966400268557</v>
+      </c>
+      <c r="CE3">
+        <v>1.860660744604795</v>
+      </c>
+      <c r="CF3">
+        <v>1.860135408236272</v>
+      </c>
+      <c r="CG3">
+        <v>1.8299393991325</v>
+      </c>
+      <c r="CH3">
+        <v>0.03044318140292155</v>
+      </c>
+      <c r="CI3">
+        <v>0.05513501163719099</v>
+      </c>
+    </row>
+    <row r="4" spans="1:87">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>0.03833920716397395</v>
+      </c>
+      <c r="C4">
+        <v>0.04367385821915429</v>
+      </c>
+      <c r="D4">
+        <v>0.1297175473504567</v>
+      </c>
+      <c r="E4">
+        <v>0.1314549432236708</v>
+      </c>
+      <c r="F4">
+        <v>0.126546191620998</v>
+      </c>
+      <c r="G4">
+        <v>0.1408241820141943</v>
+      </c>
+      <c r="H4">
+        <v>0.14193599480132</v>
+      </c>
+      <c r="I4">
+        <v>0.1469368819771829</v>
+      </c>
+      <c r="J4">
+        <v>0.09187943693942219</v>
+      </c>
+      <c r="K4">
+        <v>0.09279983223092153</v>
+      </c>
+      <c r="L4">
+        <v>-0.001004910967455668</v>
+      </c>
+      <c r="M4">
+        <v>0.1031102377321041</v>
+      </c>
+      <c r="N4">
+        <v>0.1557520307000901</v>
+      </c>
+      <c r="O4">
+        <v>0.1553085342176607</v>
+      </c>
+      <c r="P4">
+        <v>0.1525362433194694</v>
+      </c>
+      <c r="Q4">
+        <v>0.2528441489259688</v>
+      </c>
+      <c r="R4">
+        <v>0.2357826949753737</v>
+      </c>
+      <c r="S4">
+        <v>0.2358582630510093</v>
+      </c>
+      <c r="T4">
+        <v>0.2796335062737026</v>
+      </c>
+      <c r="U4">
+        <v>0.2823934259153261</v>
+      </c>
+      <c r="V4">
+        <v>0.3132074683489514</v>
+      </c>
+      <c r="W4">
+        <v>0.01151183258022224</v>
+      </c>
+      <c r="X4">
+        <v>0.2966779126958042</v>
+      </c>
+      <c r="Y4">
+        <v>0.285126218778282</v>
+      </c>
+      <c r="Z4">
+        <v>0.3017339166970138</v>
+      </c>
+      <c r="AA4">
+        <v>0.4558772986221947</v>
+      </c>
+      <c r="AB4">
+        <v>0.4528359006649535</v>
+      </c>
+      <c r="AC4">
+        <v>0.4573808235033963</v>
+      </c>
+      <c r="AD4">
+        <v>0.4101833791173501</v>
+      </c>
+      <c r="AE4">
+        <v>0.4229486839812581</v>
+      </c>
+      <c r="AF4">
+        <v>0.4091607952057537</v>
+      </c>
+      <c r="AG4">
+        <v>1.024477842413456</v>
+      </c>
+      <c r="AH4">
+        <v>0.188325535155088</v>
+      </c>
+      <c r="AI4">
+        <v>1.004498740112759</v>
+      </c>
+      <c r="AJ4">
+        <v>1.00460740855161</v>
+      </c>
+      <c r="AK4">
+        <v>0.9748877903160449</v>
+      </c>
+      <c r="AL4">
+        <v>0.9741640868250526</v>
+      </c>
+      <c r="AM4">
+        <v>0.9679925760233756</v>
+      </c>
+      <c r="AN4">
+        <v>1.099505350093428</v>
+      </c>
+      <c r="AO4">
+        <v>1.122928633549595</v>
+      </c>
+      <c r="AP4">
+        <v>1.085626175492969</v>
+      </c>
+      <c r="AQ4">
+        <v>1.092988516261982</v>
+      </c>
+      <c r="AR4">
+        <v>1.103531673330121</v>
+      </c>
+      <c r="AS4">
+        <v>0.2014408876085131</v>
+      </c>
+      <c r="AT4">
+        <v>1.103110674663337</v>
+      </c>
+      <c r="AU4">
+        <v>1.172028554412571</v>
+      </c>
+      <c r="AV4">
+        <v>1.167673494442184</v>
+      </c>
+      <c r="AW4">
+        <v>1.168423750731289</v>
+      </c>
+      <c r="AX4">
+        <v>1.125860318784975</v>
+      </c>
+      <c r="AY4">
+        <v>1.106687745906473</v>
+      </c>
+      <c r="AZ4">
+        <v>1.117439128134247</v>
+      </c>
+      <c r="BA4">
+        <v>1.187103285661931</v>
+      </c>
+      <c r="BB4">
+        <v>1.17566789098289</v>
+      </c>
+      <c r="BC4">
+        <v>1.168209155089518</v>
+      </c>
+      <c r="BD4">
+        <v>0.1905223314708753</v>
+      </c>
+      <c r="BE4">
+        <v>1.068966952670205</v>
+      </c>
+      <c r="BF4">
+        <v>1.060162313290766</v>
+      </c>
+      <c r="BG4">
+        <v>1.084601906465271</v>
+      </c>
+      <c r="BH4">
+        <v>1.300468441429387</v>
+      </c>
+      <c r="BI4">
+        <v>1.318199809783778</v>
+      </c>
+      <c r="BJ4">
+        <v>1.31284049392728</v>
+      </c>
+      <c r="BK4">
+        <v>1.317602262333849</v>
+      </c>
+      <c r="BL4">
+        <v>1.282926373557593</v>
+      </c>
+      <c r="BM4">
+        <v>1.320491286496821</v>
+      </c>
+      <c r="BN4">
+        <v>2.636961302139714</v>
+      </c>
+      <c r="BO4">
+        <v>0.02138087320821584</v>
+      </c>
+      <c r="BP4">
+        <v>2.587155235745727</v>
+      </c>
+      <c r="BQ4">
+        <v>2.651770855926393</v>
+      </c>
+      <c r="BR4">
+        <v>1.720932236206869</v>
+      </c>
+      <c r="BS4">
+        <v>1.722383544002407</v>
+      </c>
+      <c r="BT4">
+        <v>1.711706377621188</v>
+      </c>
+      <c r="BU4">
+        <v>1.781260444724237</v>
+      </c>
+      <c r="BV4">
+        <v>1.785818006532374</v>
+      </c>
+      <c r="BW4">
+        <v>1.763899655059693</v>
+      </c>
+      <c r="BX4">
+        <v>1.719517875086779</v>
+      </c>
+      <c r="BY4">
+        <v>1.74203260405706</v>
+      </c>
+      <c r="BZ4">
+        <v>0.01194290195077402</v>
+      </c>
+      <c r="CA4">
+        <v>1.714476042920863</v>
+      </c>
+      <c r="CB4">
+        <v>1.953065676662382</v>
+      </c>
+      <c r="CC4">
+        <v>2.002280908260923</v>
+      </c>
+      <c r="CD4">
+        <v>2.009111662658423</v>
+      </c>
+      <c r="CE4">
+        <v>1.949364643123308</v>
+      </c>
+      <c r="CF4">
+        <v>1.983909284890204</v>
+      </c>
+      <c r="CG4">
+        <v>1.994716192448075</v>
+      </c>
+      <c r="CH4">
+        <v>0.03445170658732304</v>
+      </c>
+      <c r="CI4">
+        <v>0.05372631012837377</v>
+      </c>
+    </row>
+    <row r="5" spans="1:87">
+      <c r="A5">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>0.1881966511082789</v>
+      </c>
+      <c r="C5">
+        <v>0.1750716187995824</v>
+      </c>
+      <c r="D5">
+        <v>0.2890848398746892</v>
+      </c>
+      <c r="E5">
+        <v>0.2744378742829458</v>
+      </c>
+      <c r="F5">
+        <v>0.2684965519858511</v>
+      </c>
+      <c r="G5">
+        <v>0.2684043977114589</v>
+      </c>
+      <c r="H5">
+        <v>0.288873363867502</v>
+      </c>
+      <c r="I5">
+        <v>0.2597976009690804</v>
+      </c>
+      <c r="J5">
+        <v>0.251693458605665</v>
+      </c>
+      <c r="K5">
+        <v>0.2344350474374066</v>
+      </c>
+      <c r="L5">
+        <v>0.01116511243619821</v>
+      </c>
+      <c r="M5">
+        <v>0.2396414284772545</v>
+      </c>
+      <c r="N5">
+        <v>0.290984635207768</v>
+      </c>
+      <c r="O5">
+        <v>0.2970974855986788</v>
+      </c>
+      <c r="P5">
+        <v>0.312706114360255</v>
+      </c>
+      <c r="Q5">
+        <v>0.3780815766488732</v>
+      </c>
+      <c r="R5">
+        <v>0.3880851187727803</v>
+      </c>
+      <c r="S5">
+        <v>0.3838628446330425</v>
+      </c>
+      <c r="T5">
+        <v>0.4585419539298044</v>
+      </c>
+      <c r="U5">
+        <v>0.4502600664085776</v>
+      </c>
+      <c r="V5">
+        <v>0.4242212189429646</v>
+      </c>
+      <c r="W5">
+        <v>0.01402748021711575</v>
+      </c>
+      <c r="X5">
+        <v>0.4657173727026709</v>
+      </c>
+      <c r="Y5">
+        <v>0.4383928731107648</v>
+      </c>
+      <c r="Z5">
+        <v>0.459513729384551</v>
+      </c>
+      <c r="AA5">
+        <v>0.615711562080528</v>
+      </c>
+      <c r="AB5">
+        <v>0.6186077384473645</v>
+      </c>
+      <c r="AC5">
+        <v>0.6116104683614789</v>
+      </c>
+      <c r="AD5">
+        <v>0.5163378661859894</v>
+      </c>
+      <c r="AE5">
+        <v>0.5576603121359391</v>
+      </c>
+      <c r="AF5">
+        <v>0.5445327039376731</v>
+      </c>
+      <c r="AG5">
+        <v>1.156490453635927</v>
+      </c>
+      <c r="AH5">
+        <v>0.2203103574328929</v>
+      </c>
+      <c r="AI5">
+        <v>1.131146284779263</v>
+      </c>
+      <c r="AJ5">
+        <v>1.126423594408779</v>
+      </c>
+      <c r="AK5">
+        <v>1.154344624684555</v>
+      </c>
+      <c r="AL5">
+        <v>1.133051205281654</v>
+      </c>
+      <c r="AM5">
+        <v>1.1398612996056</v>
+      </c>
+      <c r="AN5">
+        <v>1.217134182410509</v>
+      </c>
+      <c r="AO5">
+        <v>1.240710215406989</v>
+      </c>
+      <c r="AP5">
+        <v>1.260666619418507</v>
+      </c>
+      <c r="AQ5">
+        <v>1.256218792504037</v>
+      </c>
+      <c r="AR5">
+        <v>1.236803485493025</v>
+      </c>
+      <c r="AS5">
+        <v>0.2346015030006579</v>
+      </c>
+      <c r="AT5">
+        <v>1.262991623145054</v>
+      </c>
+      <c r="AU5">
+        <v>1.310891289812208</v>
+      </c>
+      <c r="AV5">
+        <v>1.296957326823001</v>
+      </c>
+      <c r="AW5">
+        <v>1.30972061749532</v>
+      </c>
+      <c r="AX5">
+        <v>1.250929662137866</v>
+      </c>
+      <c r="AY5">
+        <v>1.247777798863432</v>
+      </c>
+      <c r="AZ5">
+        <v>1.240194597507536</v>
+      </c>
+      <c r="BA5">
+        <v>1.319130365972271</v>
+      </c>
+      <c r="BB5">
+        <v>1.280903502793044</v>
+      </c>
+      <c r="BC5">
+        <v>1.296603695419857</v>
+      </c>
+      <c r="BD5">
+        <v>0.2429821024350673</v>
+      </c>
+      <c r="BE5">
+        <v>1.205024395054442</v>
+      </c>
+      <c r="BF5">
+        <v>1.215268634878065</v>
+      </c>
+      <c r="BG5">
+        <v>1.176498204519787</v>
+      </c>
+      <c r="BH5">
+        <v>1.442777376863091</v>
+      </c>
+      <c r="BI5">
+        <v>1.414179171950821</v>
+      </c>
+      <c r="BJ5">
+        <v>1.430777682913397</v>
+      </c>
+      <c r="BK5">
+        <v>1.4128790881607</v>
+      </c>
+      <c r="BL5">
+        <v>1.443968741246742</v>
+      </c>
+      <c r="BM5">
+        <v>1.420988286948955</v>
+      </c>
+      <c r="BN5">
+        <v>2.760139961080261</v>
+      </c>
+      <c r="BO5">
+        <v>0.1666897062290194</v>
+      </c>
+      <c r="BP5">
+        <v>2.813553185329114</v>
+      </c>
+      <c r="BQ5">
+        <v>2.811651848682326</v>
+      </c>
+      <c r="BR5">
+        <v>1.872951504573724</v>
+      </c>
+      <c r="BS5">
+        <v>1.803617547774103</v>
+      </c>
+      <c r="BT5">
+        <v>1.80425787564384</v>
+      </c>
+      <c r="BU5">
+        <v>1.873694755090048</v>
+      </c>
+      <c r="BV5">
+        <v>1.933464435466854</v>
+      </c>
+      <c r="BW5">
+        <v>1.888959187164408</v>
+      </c>
+      <c r="BX5">
+        <v>1.886639177835629</v>
+      </c>
+      <c r="BY5">
+        <v>1.887277238153974</v>
+      </c>
+      <c r="BZ5">
+        <v>0.1579967294129387</v>
+      </c>
+      <c r="CA5">
+        <v>1.858323361054042</v>
+      </c>
+      <c r="CB5">
+        <v>2.108191897831868</v>
+      </c>
+      <c r="CC5">
+        <v>2.138341436207218</v>
+      </c>
+      <c r="CD5">
+        <v>2.137896413905129</v>
+      </c>
+      <c r="CE5">
+        <v>2.08964915364912</v>
+      </c>
+      <c r="CF5">
+        <v>2.157898578671151</v>
+      </c>
+      <c r="CG5">
+        <v>2.093914529399436</v>
+      </c>
+      <c r="CH5">
+        <v>0.1788430909872715</v>
+      </c>
+      <c r="CI5">
+        <v>0.1850127532138407</v>
+      </c>
+    </row>
+    <row r="6" spans="1:87">
+      <c r="A6">
+        <v>0</v>
+      </c>
+      <c r="B6">
+        <v>0.04618049010047671</v>
+      </c>
+      <c r="C6">
+        <v>0.05660105263717474</v>
+      </c>
+      <c r="D6">
+        <v>0.1404435861315483</v>
+      </c>
+      <c r="E6">
+        <v>0.1129972831565304</v>
+      </c>
+      <c r="F6">
+        <v>0.1453107775944028</v>
+      </c>
+      <c r="G6">
+        <v>0.1334810937770101</v>
+      </c>
+      <c r="H6">
+        <v>0.1566303143704205</v>
+      </c>
+      <c r="I6">
+        <v>0.1355295441204163</v>
+      </c>
+      <c r="J6">
+        <v>0.1241187209410544</v>
+      </c>
+      <c r="K6">
+        <v>0.1276196893336042</v>
+      </c>
+      <c r="L6">
+        <v>-0.003840402552067633</v>
+      </c>
+      <c r="M6">
+        <v>0.1004957451604708</v>
+      </c>
+      <c r="N6">
+        <v>0.1720559465402511</v>
+      </c>
+      <c r="O6">
+        <v>0.1928764199905353</v>
+      </c>
+      <c r="P6">
+        <v>0.1727895077115985</v>
+      </c>
+      <c r="Q6">
+        <v>0.2238226611154495</v>
+      </c>
+      <c r="R6">
+        <v>0.2231275742656919</v>
+      </c>
+      <c r="S6">
+        <v>0.2389180156830674</v>
+      </c>
+      <c r="T6">
+        <v>0.2865781466545998</v>
+      </c>
+      <c r="U6">
+        <v>0.295858746089077</v>
+      </c>
+      <c r="V6">
+        <v>0.3009615773636864</v>
+      </c>
+      <c r="W6">
+        <v>0.007001353599929366</v>
+      </c>
+      <c r="X6">
+        <v>0.326475918346098</v>
+      </c>
+      <c r="Y6">
+        <v>0.3104874623196898</v>
+      </c>
+      <c r="Z6">
+        <v>0.341622288261455</v>
+      </c>
+      <c r="AA6">
+        <v>0.4215945782691212</v>
+      </c>
+      <c r="AB6">
+        <v>0.4294688744584179</v>
+      </c>
+      <c r="AC6">
+        <v>0.4548608398447015</v>
+      </c>
+      <c r="AD6">
+        <v>0.4107678897983407</v>
+      </c>
+      <c r="AE6">
+        <v>0.4202462873998518</v>
+      </c>
+      <c r="AF6">
+        <v>0.4400534671698642</v>
+      </c>
+      <c r="AG6">
+        <v>0.9965589039232278</v>
+      </c>
+      <c r="AH6">
+        <v>0.2085729231489898</v>
+      </c>
+      <c r="AI6">
+        <v>0.9775627895942107</v>
+      </c>
+      <c r="AJ6">
+        <v>0.9392526006422522</v>
+      </c>
+      <c r="AK6">
+        <v>0.9384632591771854</v>
+      </c>
+      <c r="AL6">
+        <v>0.9400950463767029</v>
+      </c>
+      <c r="AM6">
+        <v>0.9405674968129348</v>
+      </c>
+      <c r="AN6">
+        <v>1.011214820888098</v>
+      </c>
+      <c r="AO6">
+        <v>1.016319263455206</v>
+      </c>
+      <c r="AP6">
+        <v>1.045572195712293</v>
+      </c>
+      <c r="AQ6">
+        <v>1.016489194633488</v>
+      </c>
+      <c r="AR6">
+        <v>1.025402628562557</v>
+      </c>
+      <c r="AS6">
+        <v>0.2107291892734859</v>
+      </c>
+      <c r="AT6">
+        <v>1.015296954046005</v>
+      </c>
+      <c r="AU6">
+        <v>1.08998575457769</v>
+      </c>
+      <c r="AV6">
+        <v>1.076187666963908</v>
+      </c>
+      <c r="AW6">
+        <v>1.070350577039326</v>
+      </c>
+      <c r="AX6">
+        <v>1.01762947982831</v>
+      </c>
+      <c r="AY6">
+        <v>1.030289597858286</v>
+      </c>
+      <c r="AZ6">
+        <v>1.024942126674597</v>
+      </c>
+      <c r="BA6">
+        <v>1.050383162557839</v>
+      </c>
+      <c r="BB6">
+        <v>1.092254933154031</v>
+      </c>
+      <c r="BC6">
+        <v>1.09822167779114</v>
+      </c>
+      <c r="BD6">
+        <v>0.2359426421017406</v>
+      </c>
+      <c r="BE6">
+        <v>0.9523925047341975</v>
+      </c>
+      <c r="BF6">
+        <v>1.035088531458818</v>
+      </c>
+      <c r="BG6">
+        <v>0.9807408297827257</v>
+      </c>
+      <c r="BH6">
+        <v>1.191356993940401</v>
+      </c>
+      <c r="BI6">
+        <v>1.201910560472023</v>
+      </c>
+      <c r="BJ6">
+        <v>1.2184766318359</v>
+      </c>
+      <c r="BK6">
+        <v>1.186423776242012</v>
+      </c>
+      <c r="BL6">
+        <v>1.304553440054293</v>
+      </c>
+      <c r="BM6">
+        <v>1.222382950648558</v>
+      </c>
+      <c r="BN6">
+        <v>2.242925312456034</v>
+      </c>
+      <c r="BO6">
+        <v>0.07211756104950118</v>
+      </c>
+      <c r="BP6">
+        <v>2.173834750663177</v>
+      </c>
+      <c r="BQ6">
+        <v>2.252674025538894</v>
+      </c>
+      <c r="BR6">
+        <v>1.489589958837439</v>
+      </c>
+      <c r="BS6">
+        <v>1.512023919696251</v>
+      </c>
+      <c r="BT6">
+        <v>1.552012845938398</v>
+      </c>
+      <c r="BU6">
+        <v>1.670492050770646</v>
+      </c>
+      <c r="BV6">
+        <v>1.625057732931408</v>
+      </c>
+      <c r="BW6">
+        <v>1.675864123836584</v>
+      </c>
+      <c r="BX6">
+        <v>1.56561358516818</v>
+      </c>
+      <c r="BY6">
+        <v>1.649281507369268</v>
+      </c>
+      <c r="BZ6">
+        <v>0.03431128333213561</v>
+      </c>
+      <c r="CA6">
+        <v>1.612388089464998</v>
+      </c>
+      <c r="CB6">
+        <v>1.801793873707485</v>
+      </c>
+      <c r="CC6">
+        <v>1.881591187463184</v>
+      </c>
+      <c r="CD6">
+        <v>1.769034225942265</v>
+      </c>
+      <c r="CE6">
+        <v>1.820545299080496</v>
+      </c>
+      <c r="CF6">
+        <v>1.752036053586298</v>
+      </c>
+      <c r="CG6">
+        <v>1.790508605933244</v>
+      </c>
+      <c r="CH6">
+        <v>0.05008895685144273</v>
+      </c>
+      <c r="CI6">
+        <v>0.06627287461984564</v>
+      </c>
+    </row>
+    <row r="7" spans="1:87">
+      <c r="A7">
+        <v>0</v>
+      </c>
+      <c r="B7">
+        <v>0.08139561075577238</v>
+      </c>
+      <c r="C7">
+        <v>0.08580789983117487</v>
+      </c>
+      <c r="D7">
+        <v>0.2188236736177796</v>
+      </c>
+      <c r="E7">
+        <v>0.2033783344532896</v>
+      </c>
+      <c r="F7">
+        <v>0.1814783696929212</v>
+      </c>
+      <c r="G7">
+        <v>0.1877154390448533</v>
+      </c>
+      <c r="H7">
+        <v>0.2104282265880995</v>
+      </c>
+      <c r="I7">
+        <v>0.1921159350891234</v>
+      </c>
+      <c r="J7">
+        <v>0.1624031750507396</v>
+      </c>
+      <c r="K7">
+        <v>0.1358949407699438</v>
+      </c>
+      <c r="L7">
+        <v>0.01233184694713855</v>
+      </c>
+      <c r="M7">
+        <v>0.1938904951474605</v>
+      </c>
+      <c r="N7">
+        <v>0.2463740684337486</v>
+      </c>
+      <c r="O7">
+        <v>0.2174215592437918</v>
+      </c>
+      <c r="P7">
+        <v>0.2132178736942696</v>
+      </c>
+      <c r="Q7">
+        <v>0.3349426784622033</v>
+      </c>
+      <c r="R7">
+        <v>0.3668434489370849</v>
+      </c>
+      <c r="S7">
+        <v>0.2760251502098539</v>
+      </c>
+      <c r="T7">
+        <v>0.3640708838821</v>
+      </c>
+      <c r="U7">
+        <v>0.342690909572162</v>
+      </c>
+      <c r="V7">
+        <v>0.4456181228603575</v>
+      </c>
+      <c r="W7">
+        <v>0.03589530866177911</v>
+      </c>
+      <c r="X7">
+        <v>0.3575320177480512</v>
+      </c>
+      <c r="Y7">
+        <v>0.3617844519202073</v>
+      </c>
+      <c r="Z7">
+        <v>0.4090053258879582</v>
+      </c>
+      <c r="AA7">
+        <v>0.6120020618939226</v>
+      </c>
+      <c r="AB7">
+        <v>0.614626782827309</v>
+      </c>
+      <c r="AC7">
+        <v>0.5791489688119996</v>
+      </c>
+      <c r="AD7">
+        <v>0.5017647710425769</v>
+      </c>
+      <c r="AE7">
+        <v>0.489678767677242</v>
+      </c>
+      <c r="AF7">
+        <v>0.4631440780117863</v>
+      </c>
+      <c r="AG7">
+        <v>1.23091731600297</v>
+      </c>
+      <c r="AH7">
+        <v>0.2217959432978147</v>
+      </c>
+      <c r="AI7">
+        <v>1.389517363312149</v>
+      </c>
+      <c r="AJ7">
+        <v>1.380500487476161</v>
+      </c>
+      <c r="AK7">
+        <v>1.292199369509935</v>
+      </c>
+      <c r="AL7">
+        <v>1.117573344985812</v>
+      </c>
+      <c r="AM7">
+        <v>1.305691723231708</v>
+      </c>
+      <c r="AN7">
+        <v>1.602930376760634</v>
+      </c>
+      <c r="AO7">
+        <v>1.403550978622442</v>
+      </c>
+      <c r="AP7">
+        <v>1.525600570811129</v>
+      </c>
+      <c r="AQ7">
+        <v>1.484894420512529</v>
+      </c>
+      <c r="AR7">
+        <v>1.525600570811129</v>
+      </c>
+      <c r="AS7">
+        <v>0.2699811624978711</v>
+      </c>
+      <c r="AT7">
+        <v>1.516983793421944</v>
+      </c>
+      <c r="AU7">
+        <v>1.601896105798979</v>
+      </c>
+      <c r="AV7">
+        <v>1.407989077527697</v>
+      </c>
+      <c r="AW7">
+        <v>1.596922238622056</v>
+      </c>
+      <c r="AX7">
+        <v>1.550518291839777</v>
+      </c>
+      <c r="AY7">
+        <v>1.38199278486653</v>
+      </c>
+      <c r="AZ7">
+        <v>1.382500478386768</v>
+      </c>
+      <c r="BA7">
+        <v>1.473513180848214</v>
+      </c>
+      <c r="BB7">
+        <v>1.607102640956338</v>
+      </c>
+      <c r="BC7">
+        <v>1.556055712444142</v>
+      </c>
+      <c r="BD7">
+        <v>0.2710764792454293</v>
+      </c>
+      <c r="BE7">
+        <v>1.37983795834449</v>
+      </c>
+      <c r="BF7">
+        <v>1.416399336047944</v>
+      </c>
+      <c r="BG7">
+        <v>1.44083032705779</v>
+      </c>
+      <c r="BH7">
+        <v>1.658911452186672</v>
+      </c>
+      <c r="BI7">
+        <v>1.773067063912149</v>
+      </c>
+      <c r="BJ7">
+        <v>1.926080660151839</v>
+      </c>
+      <c r="BK7">
+        <v>1.680002939679785</v>
+      </c>
+      <c r="BL7">
+        <v>1.888063179885118</v>
+      </c>
+      <c r="BM7">
+        <v>1.789964692695393</v>
+      </c>
+      <c r="BO7">
+        <v>0.1062020160298224</v>
+      </c>
+      <c r="BR7">
+        <v>2.684462882471138</v>
+      </c>
+      <c r="BS7">
+        <v>2.498777989999738</v>
+      </c>
+      <c r="BT7">
+        <v>2.275318400961112</v>
+      </c>
+      <c r="BU7">
+        <v>2.714938376468172</v>
+      </c>
+      <c r="BV7">
+        <v>2.790374078712237</v>
+      </c>
+      <c r="BW7">
+        <v>2.889090844672491</v>
+      </c>
+      <c r="BX7">
+        <v>3.031002863128569</v>
+      </c>
+      <c r="BY7">
+        <v>2.858717110926029</v>
+      </c>
+      <c r="BZ7">
+        <v>0.0715543656274555</v>
+      </c>
+      <c r="CA7">
+        <v>2.892091199905992</v>
+      </c>
+      <c r="CB7">
+        <v>3.346224959460505</v>
+      </c>
+      <c r="CC7">
+        <v>3.748771574773756</v>
+      </c>
+      <c r="CD7">
+        <v>3.826215663449488</v>
+      </c>
+      <c r="CE7">
+        <v>3.670235156945154</v>
+      </c>
+      <c r="CF7">
+        <v>3.877437932587533</v>
+      </c>
+      <c r="CG7">
+        <v>3.69005895255929</v>
+      </c>
+      <c r="CH7">
+        <v>0.1090431169904558</v>
+      </c>
+      <c r="CI7">
+        <v>0.08244096957791737</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
everything works right now holy
</commit_message>
<xml_diff>
--- a/combined_dataframes.xlsx
+++ b/combined_dataframes.xlsx
@@ -10,8 +10,8 @@
     <sheet name="Materials" sheetId="1" r:id="rId1"/>
     <sheet name="Samples" sheetId="2" r:id="rId2"/>
     <sheet name="Standard Deviations" sheetId="3" r:id="rId3"/>
-    <sheet name="Absorbance Material" sheetId="4" r:id="rId4"/>
-    <sheet name="Absorbance Sample" sheetId="5" r:id="rId5"/>
+    <sheet name="Absorbance Sample" sheetId="4" r:id="rId4"/>
+    <sheet name="Absorbance Material" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -3448,91 +3448,91 @@
         <v>630.188</v>
       </c>
       <c r="B2">
-        <v>1419.887194542227</v>
+        <v>0.04380160840378852</v>
       </c>
       <c r="C2">
-        <v>99.05847704765242</v>
+        <v>0.003442687054076699</v>
       </c>
       <c r="D2">
-        <v>195.7745563779936</v>
+        <v>0.006811475382995633</v>
       </c>
       <c r="E2">
-        <v>2070.413381785143</v>
+        <v>0.06519961898701958</v>
       </c>
       <c r="F2">
-        <v>1408.361502997367</v>
+        <v>0.04878718867337409</v>
       </c>
       <c r="G2">
-        <v>1220.732856719685</v>
+        <v>0.04580236160330386</v>
       </c>
       <c r="H2">
-        <v>770.4099195233662</v>
+        <v>0.0308421251356063</v>
       </c>
       <c r="I2">
-        <v>5301.100484434812</v>
+        <v>0.1840502634711886</v>
       </c>
       <c r="J2">
-        <v>1945.319110171901</v>
+        <v>0.08674260772758295</v>
       </c>
       <c r="K2">
-        <v>640.2927184694516</v>
+        <v>0.03021306079148173</v>
       </c>
       <c r="L2">
-        <v>5641.822046127917</v>
+        <v>0.3405260125651525</v>
       </c>
       <c r="M2">
-        <v>8957.658443523342</v>
+        <v>0.4769809927023454</v>
       </c>
       <c r="N2">
-        <v>24.25827023923989</v>
+        <v>0.001988951213859676</v>
       </c>
       <c r="O2">
-        <v>87.77881877195649</v>
+        <v>0.007991909223191256</v>
       </c>
       <c r="P2">
-        <v>9378.847055512741</v>
+        <v>0.5199039035226427</v>
       </c>
       <c r="Q2">
-        <v>266.544544448016</v>
+        <v>0.02501408586664908</v>
       </c>
       <c r="R2">
-        <v>146.108056502713</v>
+        <v>0.01344171170029101</v>
       </c>
       <c r="S2">
-        <v>603.0421972797592</v>
+        <v>0.05745513230834962</v>
       </c>
       <c r="T2">
-        <v>9693.111451395522</v>
+        <v>0.5485179382329738</v>
       </c>
       <c r="U2">
-        <v>1374.686445694072</v>
+        <v>0.1347529118200271</v>
       </c>
       <c r="V2">
-        <v>55.06540815248692</v>
+        <v>0.006042968219808958</v>
       </c>
       <c r="W2">
-        <v>3627.652272586224</v>
+        <v>0.6798825195807328</v>
       </c>
       <c r="X2">
-        <v>16628.01501992721</v>
+        <v>1.392814464621002</v>
       </c>
       <c r="Y2">
-        <v>70.64415120871634</v>
+        <v>0.01114393270727403</v>
       </c>
       <c r="Z2">
-        <v>228.0724046766727</v>
+        <v>0.0381594778969615</v>
       </c>
       <c r="AA2">
-        <v>14973.34164723009</v>
+        <v>0.9548622480525796</v>
       </c>
       <c r="AB2">
-        <v>759.0125262965033</v>
+        <v>0.1367702556211942</v>
       </c>
       <c r="AC2">
-        <v>45.80075081262309</v>
+        <v>0.009243594899532774</v>
       </c>
       <c r="AD2">
-        <v>15270.73806152473</v>
+        <v>1.064146767345145</v>
       </c>
     </row>
     <row r="3" spans="1:30">
@@ -3540,91 +3540,91 @@
         <v>710.104</v>
       </c>
       <c r="B3">
-        <v>1099.331746300907</v>
+        <v>0.03483534427164225</v>
       </c>
       <c r="C3">
-        <v>71.94060883812479</v>
+        <v>0.002558959803086337</v>
       </c>
       <c r="D3">
-        <v>113.8440719800559</v>
+        <v>0.004081929199245724</v>
       </c>
       <c r="E3">
-        <v>1736.869309987079</v>
+        <v>0.05618788099176582</v>
       </c>
       <c r="F3">
-        <v>1224.15532498944</v>
+        <v>0.04323161733596066</v>
       </c>
       <c r="G3">
-        <v>1158.699064392908</v>
+        <v>0.04403409764172868</v>
       </c>
       <c r="H3">
-        <v>538.2490216201052</v>
+        <v>0.02177790626241956</v>
       </c>
       <c r="I3">
-        <v>4955.343318005322</v>
+        <v>0.1772997187173177</v>
       </c>
       <c r="J3">
-        <v>1861.457320730186</v>
+        <v>0.0832763529682408</v>
       </c>
       <c r="K3">
-        <v>590.5938603854595</v>
+        <v>0.02792253189203511</v>
       </c>
       <c r="L3">
-        <v>5481.518246437296</v>
+        <v>0.3335776956336156</v>
       </c>
       <c r="M3">
-        <v>8498.114045608883</v>
+        <v>0.4595513457559852</v>
       </c>
       <c r="N3">
-        <v>191.3502014631812</v>
+        <v>0.01547757197089769</v>
       </c>
       <c r="O3">
-        <v>43.35752616328579</v>
+        <v>0.004007341574491936</v>
       </c>
       <c r="P3">
-        <v>9059.362543489195</v>
+        <v>0.5055893369240256</v>
       </c>
       <c r="Q3">
-        <v>283.2762250878102</v>
+        <v>0.02610040002654425</v>
       </c>
       <c r="R3">
-        <v>168.6101000088663</v>
+        <v>0.01543447923232249</v>
       </c>
       <c r="S3">
-        <v>437.4825471090245</v>
+        <v>0.04120231209957874</v>
       </c>
       <c r="T3">
-        <v>9455.209979884106</v>
+        <v>0.5388210441959386</v>
       </c>
       <c r="U3">
-        <v>1328.25525273759</v>
+        <v>0.127985562826109</v>
       </c>
       <c r="V3">
-        <v>139.7911567303171</v>
+        <v>0.01538551374611017</v>
       </c>
       <c r="W3">
-        <v>3708.400449213246</v>
+        <v>0.6752444082993834</v>
       </c>
       <c r="X3">
-        <v>16474.9364618145</v>
+        <v>1.365042692238199</v>
       </c>
       <c r="Y3">
-        <v>119.0632633308865</v>
+        <v>0.01873551227683343</v>
       </c>
       <c r="Z3">
-        <v>69.58191808940026</v>
+        <v>0.01137997494534088</v>
       </c>
       <c r="AA3">
-        <v>14589.05861003033</v>
+        <v>0.9332660967146171</v>
       </c>
       <c r="AB3">
-        <v>796.338581069635</v>
+        <v>0.1406346507813414</v>
       </c>
       <c r="AC3">
-        <v>45.15707115170318</v>
+        <v>0.008992213134374078</v>
       </c>
       <c r="AD3">
-        <v>14984.72196267669</v>
+        <v>1.03188556681252</v>
       </c>
     </row>
     <row r="4" spans="1:30">
@@ -3632,91 +3632,91 @@
         <v>800.131</v>
       </c>
       <c r="B4">
-        <v>517.9768438839717</v>
+        <v>0.02382491412922419</v>
       </c>
       <c r="C4">
-        <v>48.56834694531019</v>
+        <v>0.002489038766263462</v>
       </c>
       <c r="D4">
-        <v>62.57876396989686</v>
+        <v>0.003256022651867537</v>
       </c>
       <c r="E4">
-        <v>1143.315439642534</v>
+        <v>0.05389446332121701</v>
       </c>
       <c r="F4">
-        <v>590.38253380753</v>
+        <v>0.03026553929253614</v>
       </c>
       <c r="G4">
-        <v>975.8023503379167</v>
+        <v>0.05366988735372546</v>
       </c>
       <c r="H4">
-        <v>447.5254831012426</v>
+        <v>0.02610686518409367</v>
       </c>
       <c r="I4">
-        <v>3224.207520632009</v>
+        <v>0.1696138634764636</v>
       </c>
       <c r="J4">
-        <v>1439.813380207658</v>
+        <v>0.09415583632941925</v>
       </c>
       <c r="K4">
-        <v>374.9131151346941</v>
+        <v>0.0260368094389145</v>
       </c>
       <c r="L4">
-        <v>3854.661960639349</v>
+        <v>0.3513408845422157</v>
       </c>
       <c r="M4">
-        <v>5922.555016468821</v>
+        <v>0.4712491925962035</v>
       </c>
       <c r="N4">
-        <v>31.84458352687387</v>
+        <v>0.003789355100363839</v>
       </c>
       <c r="O4">
-        <v>138.6201828739236</v>
+        <v>0.01885362508256829</v>
       </c>
       <c r="P4">
-        <v>6204.105199388144</v>
+        <v>0.5178056453281826</v>
       </c>
       <c r="Q4">
-        <v>274.9621646245166</v>
+        <v>0.03859403752367153</v>
       </c>
       <c r="R4">
-        <v>224.5478507467841</v>
+        <v>0.03159791021982255</v>
       </c>
       <c r="S4">
-        <v>262.5247989714492</v>
+        <v>0.03735963043712377</v>
       </c>
       <c r="T4">
-        <v>6410.02173960237</v>
+        <v>0.5381117437132337</v>
       </c>
       <c r="U4">
-        <v>899.5069212212877</v>
+        <v>0.1322514586264388</v>
       </c>
       <c r="V4">
-        <v>17.49531080032566</v>
+        <v>0.002936941940250607</v>
       </c>
       <c r="W4">
-        <v>2572.489757574362</v>
+        <v>0.7711371486957126</v>
       </c>
       <c r="X4">
-        <v>11610.60755610037</v>
+        <v>1.50035133213359</v>
       </c>
       <c r="Y4">
-        <v>23.09273424694432</v>
+        <v>0.00579115191322902</v>
       </c>
       <c r="Z4">
-        <v>43.54516304941364</v>
+        <v>0.01156562808995899</v>
       </c>
       <c r="AA4">
-        <v>10393.1517719951</v>
+        <v>0.9924321621850073</v>
       </c>
       <c r="AB4">
-        <v>538.7827786084113</v>
+        <v>0.1539365631592119</v>
       </c>
       <c r="AC4">
-        <v>92.08353530897894</v>
+        <v>0.02999499531395346</v>
       </c>
       <c r="AD4">
-        <v>10521.80885319749</v>
+        <v>1.12623636418945</v>
       </c>
     </row>
     <row r="5" spans="1:30">
@@ -3724,91 +3724,91 @@
         <v>905.029</v>
       </c>
       <c r="B5">
-        <v>1617.237696869264</v>
+        <v>0.1050716562403819</v>
       </c>
       <c r="C5">
-        <v>134.9491873817697</v>
+        <v>0.01059646568340399</v>
       </c>
       <c r="D5">
-        <v>191.0223093646392</v>
+        <v>0.01493572626170266</v>
       </c>
       <c r="E5">
-        <v>1992.863283613555</v>
+        <v>0.1341648252104573</v>
       </c>
       <c r="F5">
-        <v>406.8421118505303</v>
+        <v>0.03155600924603286</v>
       </c>
       <c r="G5">
-        <v>486.5924956521623</v>
+        <v>0.04093901201930097</v>
       </c>
       <c r="H5">
-        <v>453.1896434441105</v>
+        <v>0.04093521321507429</v>
       </c>
       <c r="I5">
-        <v>3362.461336733107</v>
+        <v>0.2496679772018402</v>
       </c>
       <c r="J5">
-        <v>960.2326586171707</v>
+        <v>0.0968553655084167</v>
       </c>
       <c r="K5">
-        <v>546.5012838274034</v>
+        <v>0.05713282373309569</v>
       </c>
       <c r="L5">
-        <v>2545.484674119057</v>
+        <v>0.349585983672509</v>
       </c>
       <c r="M5">
-        <v>4655.392763505567</v>
+        <v>0.5245133599461783</v>
       </c>
       <c r="N5">
-        <v>58.31970057364849</v>
+        <v>0.0108746938647454</v>
       </c>
       <c r="O5">
-        <v>106.3481353856286</v>
+        <v>0.02179128443811644</v>
       </c>
       <c r="P5">
-        <v>4894.020681065826</v>
+        <v>0.5843069475983483</v>
       </c>
       <c r="Q5">
-        <v>114.7170149759836</v>
+        <v>0.02463805463690635</v>
       </c>
       <c r="R5">
-        <v>163.459649378677</v>
+        <v>0.03488844950697861</v>
       </c>
       <c r="S5">
-        <v>184.9770231677437</v>
+        <v>0.03947438743705833</v>
       </c>
       <c r="T5">
-        <v>4843.87549605427</v>
+        <v>0.5836709407202497</v>
       </c>
       <c r="U5">
-        <v>651.3537478014542</v>
+        <v>0.1438563934239109</v>
       </c>
       <c r="V5">
-        <v>40.53507092629809</v>
+        <v>0.009979649945074659</v>
       </c>
       <c r="W5">
-        <v>1706.367763108235</v>
+        <v>0.766611808275704</v>
       </c>
       <c r="X5">
-        <v>7645.620060431658</v>
+        <v>1.527618769364381</v>
       </c>
       <c r="Y5">
-        <v>106.7511907427736</v>
+        <v>0.0398464181594551</v>
       </c>
       <c r="Z5">
-        <v>77.81258397585832</v>
+        <v>0.03105407838314926</v>
       </c>
       <c r="AA5">
-        <v>6828.055048527729</v>
+        <v>0.9982164260587829</v>
       </c>
       <c r="AB5">
-        <v>354.0251785890376</v>
+        <v>0.1537061063351251</v>
       </c>
       <c r="AC5">
-        <v>70.79426247938447</v>
+        <v>0.03508529780733404</v>
       </c>
       <c r="AD5">
-        <v>6907.338253699829</v>
+        <v>1.103890292713196</v>
       </c>
     </row>
     <row r="6" spans="1:30">
@@ -3816,91 +3816,91 @@
         <v>940.061</v>
       </c>
       <c r="B6">
-        <v>210.6778496306622</v>
+        <v>0.03012447772476088</v>
       </c>
       <c r="C6">
-        <v>110.0603535565826</v>
+        <v>0.01742197378082713</v>
       </c>
       <c r="D6">
-        <v>79.57772159970415</v>
+        <v>0.01281486810983787</v>
       </c>
       <c r="E6">
-        <v>506.4813220642988</v>
+        <v>0.07490833267334479</v>
       </c>
       <c r="F6">
-        <v>301.4548240201174</v>
+        <v>0.04845710064628785</v>
       </c>
       <c r="G6">
-        <v>172.4240555288039</v>
+        <v>0.02926541427599602</v>
       </c>
       <c r="H6">
-        <v>168.2092126638729</v>
+        <v>0.03055013472217077</v>
       </c>
       <c r="I6">
-        <v>1089.44424607228</v>
+        <v>0.1775422918024317</v>
       </c>
       <c r="J6">
-        <v>284.7379709048301</v>
+        <v>0.05731453534385886</v>
       </c>
       <c r="K6">
-        <v>103.0589087609603</v>
+        <v>0.02213092473299724</v>
       </c>
       <c r="L6">
-        <v>1167.322104787278</v>
+        <v>0.3271663331982967</v>
       </c>
       <c r="M6">
-        <v>1776.201337412232</v>
+        <v>0.4333408735961855</v>
       </c>
       <c r="N6">
-        <v>3.099141010021867</v>
+        <v>0.001104064831045499</v>
       </c>
       <c r="O6">
-        <v>47.57223796501476</v>
+        <v>0.01853923130539162</v>
       </c>
       <c r="P6">
-        <v>1864.883150541878</v>
+        <v>0.4678000727207514</v>
       </c>
       <c r="Q6">
-        <v>99.84919917054916</v>
+        <v>0.03974183997231336</v>
       </c>
       <c r="R6">
-        <v>69.48829092012555</v>
+        <v>0.02752173302625305</v>
       </c>
       <c r="S6">
-        <v>84.60393622639553</v>
+        <v>0.03398898202802981</v>
       </c>
       <c r="T6">
-        <v>1793.662295479559</v>
+        <v>0.4615357856782757</v>
       </c>
       <c r="U6">
-        <v>263.9985089446528</v>
+        <v>0.1093409603399115</v>
       </c>
       <c r="V6">
-        <v>34.58852157869713</v>
+        <v>0.01602945600003627</v>
       </c>
       <c r="W6">
-        <v>737.6883344102712</v>
+        <v>0.5669803748054993</v>
       </c>
       <c r="X6">
-        <v>3404.418322125676</v>
+        <v>1.236814272718895</v>
       </c>
       <c r="Y6">
-        <v>49.57330657722958</v>
+        <v>0.03162017724975023</v>
       </c>
       <c r="Z6">
-        <v>38.52545035427882</v>
+        <v>0.02791184265788797</v>
       </c>
       <c r="AA6">
-        <v>3175.563690957088</v>
+        <v>0.9092135690933091</v>
       </c>
       <c r="AB6">
-        <v>174.9189866052282</v>
+        <v>0.1382705502260923</v>
       </c>
       <c r="AC6">
-        <v>42.86010761769037</v>
+        <v>0.03567409246096202</v>
       </c>
       <c r="AD6">
-        <v>3220.814277892316</v>
+        <v>1.000192592390936</v>
       </c>
     </row>
     <row r="7" spans="1:30">
@@ -3908,91 +3908,88 @@
         <v>1000.111</v>
       </c>
       <c r="B7">
-        <v>163.7820485431781</v>
+        <v>0.04831788733417309</v>
       </c>
       <c r="C7">
-        <v>54.31535441290982</v>
+        <v>0.01876538783528313</v>
       </c>
       <c r="D7">
-        <v>34.8606780628261</v>
+        <v>0.01204557389918076</v>
       </c>
       <c r="E7">
-        <v>260.6715787633934</v>
+        <v>0.08009570125640078</v>
       </c>
       <c r="F7">
-        <v>74.51864246616418</v>
+        <v>0.02628841389534355</v>
       </c>
       <c r="G7">
-        <v>215.5227931681473</v>
+        <v>0.08107137248680792</v>
       </c>
       <c r="H7">
-        <v>118.1741394087557</v>
+        <v>0.04592290276599627</v>
       </c>
       <c r="I7">
-        <v>610.4654347094518</v>
+        <v>0.2156703190135762</v>
       </c>
       <c r="J7">
-        <v>287.4266014567893</v>
+        <v>0.132945062656417</v>
       </c>
       <c r="K7">
-        <v>117.1104819177174</v>
+        <v>0.05771311672953128</v>
       </c>
       <c r="L7">
-        <v>671.9361065793385</v>
+        <v>0.4358161730697819</v>
       </c>
       <c r="M7">
-        <v>1123.659577129568</v>
+        <v>0.6715964611170515</v>
       </c>
       <c r="N7">
-        <v>110.8659357061491</v>
+        <v>0.1049323720973965</v>
       </c>
       <c r="O7">
-        <v>79.43571237170346</v>
+        <v>0.1005220923011128</v>
       </c>
       <c r="P7">
-        <v>1104.65287571481</v>
+        <v>0.7134717132567179</v>
       </c>
       <c r="Q7">
-        <v>76.56200575350677</v>
+        <v>0.09720243866889566</v>
       </c>
       <c r="R7">
-        <v>90.86119509999854</v>
+        <v>0.1130993979273773</v>
       </c>
       <c r="S7">
-        <v>89.46722486475144</v>
+        <v>0.1129716684927707</v>
       </c>
       <c r="T7">
-        <v>1086.267377214284</v>
+        <v>0.6966080131783599</v>
       </c>
       <c r="U7">
-        <v>101.137932176805</v>
+        <v>0.1335217690948347</v>
       </c>
       <c r="V7">
-        <v>72.24213157846326</v>
+        <v>0.1242499740885699</v>
       </c>
       <c r="W7">
-        <v>443.5174599437997</v>
-      </c>
-      <c r="X7">
-        <v>1951.269757593757</v>
+        <v>0.0693661055159956</v>
       </c>
       <c r="Y7">
-        <v>61.34456964556847</v>
+        <v>0.2048626669973225</v>
       </c>
       <c r="Z7">
-        <v>18.72315344700247</v>
+        <v>0.08733520408590827</v>
       </c>
       <c r="AA7">
-        <v>1791.659251664501</v>
+        <v>1.661138864281263</v>
       </c>
       <c r="AB7">
-        <v>57.06101208355843</v>
+        <v>0.4285989799627858</v>
       </c>
       <c r="AC7">
-        <v>8.826920470923028</v>
+        <v>0.1079248422892098</v>
       </c>
       <c r="AD7">
-        <v>1803.655806771347</v>
+        <v>2.07522246196933</v>
       </c>
     </row>
   </sheetData>
@@ -4001,6 +3998,1851 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:CI7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:87">
+      <c r="A1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AT1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AU1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AV1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AW1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AX1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AY1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AZ1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="BA1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="BB1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="BC1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="BD1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="BE1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="BF1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="BG1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="BH1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="BI1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="BJ1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="BK1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="BL1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="BM1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="BN1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="BO1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="BP1" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="BQ1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="BR1" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="BS1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="BT1" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="BU1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="BV1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="BW1" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="BX1" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="BY1" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="BZ1" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="CA1" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="CB1" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="CC1" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="CD1" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="CE1" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="CF1" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="CG1" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="CH1" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="CI1" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="2" spans="1:87">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0.06795099732174277</v>
+      </c>
+      <c r="C2">
+        <v>0.08185805465480191</v>
+      </c>
+      <c r="D2">
+        <v>0.1545338928394538</v>
+      </c>
+      <c r="E2">
+        <v>0.1595285979578524</v>
+      </c>
+      <c r="F2">
+        <v>0.1611356300105169</v>
+      </c>
+      <c r="G2">
+        <v>0.1657440760914083</v>
+      </c>
+      <c r="H2">
+        <v>0.1522321958209901</v>
+      </c>
+      <c r="I2">
+        <v>0.1604916017349513</v>
+      </c>
+      <c r="J2">
+        <v>0.1120118472991535</v>
+      </c>
+      <c r="K2">
+        <v>0.1194300125897388</v>
+      </c>
+      <c r="L2">
+        <v>0.002974758985301182</v>
+      </c>
+      <c r="M2">
+        <v>0.1121004179217738</v>
+      </c>
+      <c r="N2">
+        <v>0.1913025001408202</v>
+      </c>
+      <c r="O2">
+        <v>0.2010557087478083</v>
+      </c>
+      <c r="P2">
+        <v>0.1945269807809258</v>
+      </c>
+      <c r="Q2">
+        <v>0.2779525147030378</v>
+      </c>
+      <c r="R2">
+        <v>0.2690071736811264</v>
+      </c>
+      <c r="S2">
+        <v>0.2716118830993711</v>
+      </c>
+      <c r="T2">
+        <v>0.3176560953365489</v>
+      </c>
+      <c r="U2">
+        <v>0.3301819559422958</v>
+      </c>
+      <c r="V2">
+        <v>0.3131392511907007</v>
+      </c>
+      <c r="W2">
+        <v>0.001330261400455145</v>
+      </c>
+      <c r="X2">
+        <v>0.3266598543948022</v>
+      </c>
+      <c r="Y2">
+        <v>0.3319231269399354</v>
+      </c>
+      <c r="Z2">
+        <v>0.33346493110568</v>
+      </c>
+      <c r="AA2">
+        <v>0.4829306993669014</v>
+      </c>
+      <c r="AB2">
+        <v>0.4898524009478926</v>
+      </c>
+      <c r="AC2">
+        <v>0.4896019436102285</v>
+      </c>
+      <c r="AD2">
+        <v>0.4373970654521983</v>
+      </c>
+      <c r="AE2">
+        <v>0.4306792180796415</v>
+      </c>
+      <c r="AF2">
+        <v>0.4277006167351722</v>
+      </c>
+      <c r="AG2">
+        <v>1.01899263158486</v>
+      </c>
+      <c r="AH2">
+        <v>0.1995119506017013</v>
+      </c>
+      <c r="AI2">
+        <v>1.026949115133777</v>
+      </c>
+      <c r="AJ2">
+        <v>1.024379418627245</v>
+      </c>
+      <c r="AK2">
+        <v>1.013984726349174</v>
+      </c>
+      <c r="AL2">
+        <v>1.016103755226842</v>
+      </c>
+      <c r="AM2">
+        <v>1.017959728441051</v>
+      </c>
+      <c r="AN2">
+        <v>1.12178981811764</v>
+      </c>
+      <c r="AO2">
+        <v>1.128846836013933</v>
+      </c>
+      <c r="AP2">
+        <v>1.112898153439635</v>
+      </c>
+      <c r="AQ2">
+        <v>1.108901319659735</v>
+      </c>
+      <c r="AR2">
+        <v>1.107784533644136</v>
+      </c>
+      <c r="AS2">
+        <v>0.2078434700802005</v>
+      </c>
+      <c r="AT2">
+        <v>1.126976540244029</v>
+      </c>
+      <c r="AU2">
+        <v>1.15642433072145</v>
+      </c>
+      <c r="AV2">
+        <v>1.176725201038425</v>
+      </c>
+      <c r="AW2">
+        <v>1.144612984295044</v>
+      </c>
+      <c r="AX2">
+        <v>1.131278282202457</v>
+      </c>
+      <c r="AY2">
+        <v>1.117729844113085</v>
+      </c>
+      <c r="AZ2">
+        <v>1.116643994309363</v>
+      </c>
+      <c r="BA2">
+        <v>1.212702435619046</v>
+      </c>
+      <c r="BB2">
+        <v>1.21928876747057</v>
+      </c>
+      <c r="BC2">
+        <v>1.210609183259514</v>
+      </c>
+      <c r="BD2">
+        <v>0.204715584709188</v>
+      </c>
+      <c r="BE2">
+        <v>1.086805281829825</v>
+      </c>
+      <c r="BF2">
+        <v>1.084310676819978</v>
+      </c>
+      <c r="BG2">
+        <v>1.076349440387174</v>
+      </c>
+      <c r="BH2">
+        <v>1.313627091948996</v>
+      </c>
+      <c r="BI2">
+        <v>1.306779881285925</v>
+      </c>
+      <c r="BJ2">
+        <v>1.313414825429418</v>
+      </c>
+      <c r="BK2">
+        <v>1.301348894529031</v>
+      </c>
+      <c r="BL2">
+        <v>1.3051761215023</v>
+      </c>
+      <c r="BM2">
+        <v>1.317076515764124</v>
+      </c>
+      <c r="BN2">
+        <v>2.488672286634736</v>
+      </c>
+      <c r="BO2">
+        <v>0.06283595561770416</v>
+      </c>
+      <c r="BP2">
+        <v>2.474974116374596</v>
+      </c>
+      <c r="BQ2">
+        <v>2.475548528763476</v>
+      </c>
+      <c r="BR2">
+        <v>1.677426607305108</v>
+      </c>
+      <c r="BS2">
+        <v>1.681449415043503</v>
+      </c>
+      <c r="BT2">
+        <v>1.660453162689851</v>
+      </c>
+      <c r="BU2">
+        <v>1.714476497547774</v>
+      </c>
+      <c r="BV2">
+        <v>1.765027021071516</v>
+      </c>
+      <c r="BW2">
+        <v>1.690234886541741</v>
+      </c>
+      <c r="BX2">
+        <v>1.701908530833132</v>
+      </c>
+      <c r="BY2">
+        <v>1.704198085567938</v>
+      </c>
+      <c r="BZ2">
+        <v>0.04918456893420017</v>
+      </c>
+      <c r="CA2">
+        <v>1.687194530989987</v>
+      </c>
+      <c r="CB2">
+        <v>1.919785367810857</v>
+      </c>
+      <c r="CC2">
+        <v>1.928167274677659</v>
+      </c>
+      <c r="CD2">
+        <v>1.907916940354473</v>
+      </c>
+      <c r="CE2">
+        <v>1.919215747486826</v>
+      </c>
+      <c r="CF2">
+        <v>1.926238552017087</v>
+      </c>
+      <c r="CG2">
+        <v>1.912777983247811</v>
+      </c>
+      <c r="CH2">
+        <v>0.0614402292893785</v>
+      </c>
+      <c r="CI2">
+        <v>0.07791362787603238</v>
+      </c>
+    </row>
+    <row r="3" spans="1:87">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>0.06254309411229172</v>
+      </c>
+      <c r="C3">
+        <v>0.05785678103512904</v>
+      </c>
+      <c r="D3">
+        <v>0.1433899630497707</v>
+      </c>
+      <c r="E3">
+        <v>0.1483169813843757</v>
+      </c>
+      <c r="F3">
+        <v>0.1470527193014075</v>
+      </c>
+      <c r="G3">
+        <v>0.1496672710642195</v>
+      </c>
+      <c r="H3">
+        <v>0.1540524273499986</v>
+      </c>
+      <c r="I3">
+        <v>0.1578234254181533</v>
+      </c>
+      <c r="J3">
+        <v>0.1037213976898729</v>
+      </c>
+      <c r="K3">
+        <v>0.09495811317170584</v>
+      </c>
+      <c r="L3">
+        <v>0.002315853507733548</v>
+      </c>
+      <c r="M3">
+        <v>0.1011536916548215</v>
+      </c>
+      <c r="N3">
+        <v>0.1789797946206727</v>
+      </c>
+      <c r="O3">
+        <v>0.1726894573919343</v>
+      </c>
+      <c r="P3">
+        <v>0.1738728165946373</v>
+      </c>
+      <c r="Q3">
+        <v>0.2525142444596454</v>
+      </c>
+      <c r="R3">
+        <v>0.2475249976218991</v>
+      </c>
+      <c r="S3">
+        <v>0.255713639650946</v>
+      </c>
+      <c r="T3">
+        <v>0.2928322070710072</v>
+      </c>
+      <c r="U3">
+        <v>0.2940084387592624</v>
+      </c>
+      <c r="V3">
+        <v>0.3137637401213069</v>
+      </c>
+      <c r="W3">
+        <v>0.001869700701004347</v>
+      </c>
+      <c r="X3">
+        <v>0.3039233660583848</v>
+      </c>
+      <c r="Y3">
+        <v>0.3002289262914682</v>
+      </c>
+      <c r="Z3">
+        <v>0.3078415998742265</v>
+      </c>
+      <c r="AA3">
+        <v>0.4481233899072491</v>
+      </c>
+      <c r="AB3">
+        <v>0.4463180747955694</v>
+      </c>
+      <c r="AC3">
+        <v>0.4585852651378226</v>
+      </c>
+      <c r="AD3">
+        <v>0.4052696777173711</v>
+      </c>
+      <c r="AE3">
+        <v>0.4086558333297102</v>
+      </c>
+      <c r="AF3">
+        <v>0.4067019442358616</v>
+      </c>
+      <c r="AG3">
+        <v>0.985449928045534</v>
+      </c>
+      <c r="AH3">
+        <v>0.1928535557583117</v>
+      </c>
+      <c r="AI3">
+        <v>0.9940083474749077</v>
+      </c>
+      <c r="AJ3">
+        <v>0.9835278215611972</v>
+      </c>
+      <c r="AK3">
+        <v>0.953755380326761</v>
+      </c>
+      <c r="AL3">
+        <v>0.9819740242282641</v>
+      </c>
+      <c r="AM3">
+        <v>0.9788849928641112</v>
+      </c>
+      <c r="AN3">
+        <v>1.10425467251388</v>
+      </c>
+      <c r="AO3">
+        <v>1.098594181794953</v>
+      </c>
+      <c r="AP3">
+        <v>1.096510620778534</v>
+      </c>
+      <c r="AQ3">
+        <v>1.065805080491945</v>
+      </c>
+      <c r="AR3">
+        <v>1.065646616280369</v>
+      </c>
+      <c r="AS3">
+        <v>0.1900194398218211</v>
+      </c>
+      <c r="AT3">
+        <v>1.074111195167979</v>
+      </c>
+      <c r="AU3">
+        <v>1.123957093707858</v>
+      </c>
+      <c r="AV3">
+        <v>1.11245921217335</v>
+      </c>
+      <c r="AW3">
+        <v>1.105008508231081</v>
+      </c>
+      <c r="AX3">
+        <v>1.075295965202646</v>
+      </c>
+      <c r="AY3">
+        <v>1.082903579075164</v>
+      </c>
+      <c r="AZ3">
+        <v>1.083910664160616</v>
+      </c>
+      <c r="BA3">
+        <v>1.156531424687362</v>
+      </c>
+      <c r="BB3">
+        <v>1.153948784082036</v>
+      </c>
+      <c r="BC3">
+        <v>1.174401777410012</v>
+      </c>
+      <c r="BD3">
+        <v>0.1833590955163211</v>
+      </c>
+      <c r="BE3">
+        <v>1.045432144962698</v>
+      </c>
+      <c r="BF3">
+        <v>1.029427607496673</v>
+      </c>
+      <c r="BG3">
+        <v>1.037962699501496</v>
+      </c>
+      <c r="BH3">
+        <v>1.255249383946394</v>
+      </c>
+      <c r="BI3">
+        <v>1.288895485521961</v>
+      </c>
+      <c r="BJ3">
+        <v>1.265233471629128</v>
+      </c>
+      <c r="BK3">
+        <v>1.260028518855096</v>
+      </c>
+      <c r="BL3">
+        <v>1.254994352563541</v>
+      </c>
+      <c r="BM3">
+        <v>1.245648968037489</v>
+      </c>
+      <c r="BN3">
+        <v>2.419851279703033</v>
+      </c>
+      <c r="BO3">
+        <v>0.0320701584753309</v>
+      </c>
+      <c r="BP3">
+        <v>2.389803366704771</v>
+      </c>
+      <c r="BQ3">
+        <v>2.402928895117701</v>
+      </c>
+      <c r="BR3">
+        <v>1.63023505717894</v>
+      </c>
+      <c r="BS3">
+        <v>1.651122404539787</v>
+      </c>
+      <c r="BT3">
+        <v>1.613737177433537</v>
+      </c>
+      <c r="BU3">
+        <v>1.660786902927901</v>
+      </c>
+      <c r="BV3">
+        <v>1.683014039654155</v>
+      </c>
+      <c r="BW3">
+        <v>1.676140434024832</v>
+      </c>
+      <c r="BX3">
+        <v>1.660140996320911</v>
+      </c>
+      <c r="BY3">
+        <v>1.634348831846555</v>
+      </c>
+      <c r="BZ3">
+        <v>0.03093495153954072</v>
+      </c>
+      <c r="CA3">
+        <v>1.628704209351442</v>
+      </c>
+      <c r="CB3">
+        <v>1.876055044353057</v>
+      </c>
+      <c r="CC3">
+        <v>1.868342932769132</v>
+      </c>
+      <c r="CD3">
+        <v>1.875966400268557</v>
+      </c>
+      <c r="CE3">
+        <v>1.860660744604795</v>
+      </c>
+      <c r="CF3">
+        <v>1.860135408236272</v>
+      </c>
+      <c r="CG3">
+        <v>1.8299393991325</v>
+      </c>
+      <c r="CH3">
+        <v>0.03044318140292155</v>
+      </c>
+      <c r="CI3">
+        <v>0.05513501163719099</v>
+      </c>
+    </row>
+    <row r="4" spans="1:87">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>0.03833920716397395</v>
+      </c>
+      <c r="C4">
+        <v>0.04367385821915429</v>
+      </c>
+      <c r="D4">
+        <v>0.1297175473504567</v>
+      </c>
+      <c r="E4">
+        <v>0.1314549432236708</v>
+      </c>
+      <c r="F4">
+        <v>0.126546191620998</v>
+      </c>
+      <c r="G4">
+        <v>0.1408241820141943</v>
+      </c>
+      <c r="H4">
+        <v>0.14193599480132</v>
+      </c>
+      <c r="I4">
+        <v>0.1469368819771829</v>
+      </c>
+      <c r="J4">
+        <v>0.09187943693942219</v>
+      </c>
+      <c r="K4">
+        <v>0.09279983223092153</v>
+      </c>
+      <c r="L4">
+        <v>-0.001004910967455668</v>
+      </c>
+      <c r="M4">
+        <v>0.1031102377321041</v>
+      </c>
+      <c r="N4">
+        <v>0.1557520307000901</v>
+      </c>
+      <c r="O4">
+        <v>0.1553085342176607</v>
+      </c>
+      <c r="P4">
+        <v>0.1525362433194694</v>
+      </c>
+      <c r="Q4">
+        <v>0.2528441489259688</v>
+      </c>
+      <c r="R4">
+        <v>0.2357826949753737</v>
+      </c>
+      <c r="S4">
+        <v>0.2358582630510093</v>
+      </c>
+      <c r="T4">
+        <v>0.2796335062737026</v>
+      </c>
+      <c r="U4">
+        <v>0.2823934259153261</v>
+      </c>
+      <c r="V4">
+        <v>0.3132074683489514</v>
+      </c>
+      <c r="W4">
+        <v>0.01151183258022224</v>
+      </c>
+      <c r="X4">
+        <v>0.2966779126958042</v>
+      </c>
+      <c r="Y4">
+        <v>0.285126218778282</v>
+      </c>
+      <c r="Z4">
+        <v>0.3017339166970138</v>
+      </c>
+      <c r="AA4">
+        <v>0.4558772986221947</v>
+      </c>
+      <c r="AB4">
+        <v>0.4528359006649535</v>
+      </c>
+      <c r="AC4">
+        <v>0.4573808235033963</v>
+      </c>
+      <c r="AD4">
+        <v>0.4101833791173501</v>
+      </c>
+      <c r="AE4">
+        <v>0.4229486839812581</v>
+      </c>
+      <c r="AF4">
+        <v>0.4091607952057537</v>
+      </c>
+      <c r="AG4">
+        <v>1.024477842413456</v>
+      </c>
+      <c r="AH4">
+        <v>0.188325535155088</v>
+      </c>
+      <c r="AI4">
+        <v>1.004498740112759</v>
+      </c>
+      <c r="AJ4">
+        <v>1.00460740855161</v>
+      </c>
+      <c r="AK4">
+        <v>0.9748877903160449</v>
+      </c>
+      <c r="AL4">
+        <v>0.9741640868250526</v>
+      </c>
+      <c r="AM4">
+        <v>0.9679925760233756</v>
+      </c>
+      <c r="AN4">
+        <v>1.099505350093428</v>
+      </c>
+      <c r="AO4">
+        <v>1.122928633549595</v>
+      </c>
+      <c r="AP4">
+        <v>1.085626175492969</v>
+      </c>
+      <c r="AQ4">
+        <v>1.092988516261982</v>
+      </c>
+      <c r="AR4">
+        <v>1.103531673330121</v>
+      </c>
+      <c r="AS4">
+        <v>0.2014408876085131</v>
+      </c>
+      <c r="AT4">
+        <v>1.103110674663337</v>
+      </c>
+      <c r="AU4">
+        <v>1.172028554412571</v>
+      </c>
+      <c r="AV4">
+        <v>1.167673494442184</v>
+      </c>
+      <c r="AW4">
+        <v>1.168423750731289</v>
+      </c>
+      <c r="AX4">
+        <v>1.125860318784975</v>
+      </c>
+      <c r="AY4">
+        <v>1.106687745906473</v>
+      </c>
+      <c r="AZ4">
+        <v>1.117439128134247</v>
+      </c>
+      <c r="BA4">
+        <v>1.187103285661931</v>
+      </c>
+      <c r="BB4">
+        <v>1.17566789098289</v>
+      </c>
+      <c r="BC4">
+        <v>1.168209155089518</v>
+      </c>
+      <c r="BD4">
+        <v>0.1905223314708753</v>
+      </c>
+      <c r="BE4">
+        <v>1.068966952670205</v>
+      </c>
+      <c r="BF4">
+        <v>1.060162313290766</v>
+      </c>
+      <c r="BG4">
+        <v>1.084601906465271</v>
+      </c>
+      <c r="BH4">
+        <v>1.300468441429387</v>
+      </c>
+      <c r="BI4">
+        <v>1.318199809783778</v>
+      </c>
+      <c r="BJ4">
+        <v>1.31284049392728</v>
+      </c>
+      <c r="BK4">
+        <v>1.317602262333849</v>
+      </c>
+      <c r="BL4">
+        <v>1.282926373557593</v>
+      </c>
+      <c r="BM4">
+        <v>1.320491286496821</v>
+      </c>
+      <c r="BN4">
+        <v>2.636961302139714</v>
+      </c>
+      <c r="BO4">
+        <v>0.02138087320821584</v>
+      </c>
+      <c r="BP4">
+        <v>2.587155235745727</v>
+      </c>
+      <c r="BQ4">
+        <v>2.651770855926393</v>
+      </c>
+      <c r="BR4">
+        <v>1.720932236206869</v>
+      </c>
+      <c r="BS4">
+        <v>1.722383544002407</v>
+      </c>
+      <c r="BT4">
+        <v>1.711706377621188</v>
+      </c>
+      <c r="BU4">
+        <v>1.781260444724237</v>
+      </c>
+      <c r="BV4">
+        <v>1.785818006532374</v>
+      </c>
+      <c r="BW4">
+        <v>1.763899655059693</v>
+      </c>
+      <c r="BX4">
+        <v>1.719517875086779</v>
+      </c>
+      <c r="BY4">
+        <v>1.74203260405706</v>
+      </c>
+      <c r="BZ4">
+        <v>0.01194290195077402</v>
+      </c>
+      <c r="CA4">
+        <v>1.714476042920863</v>
+      </c>
+      <c r="CB4">
+        <v>1.953065676662382</v>
+      </c>
+      <c r="CC4">
+        <v>2.002280908260923</v>
+      </c>
+      <c r="CD4">
+        <v>2.009111662658423</v>
+      </c>
+      <c r="CE4">
+        <v>1.949364643123308</v>
+      </c>
+      <c r="CF4">
+        <v>1.983909284890204</v>
+      </c>
+      <c r="CG4">
+        <v>1.994716192448075</v>
+      </c>
+      <c r="CH4">
+        <v>0.03445170658732304</v>
+      </c>
+      <c r="CI4">
+        <v>0.05372631012837377</v>
+      </c>
+    </row>
+    <row r="5" spans="1:87">
+      <c r="A5">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>0.1881966511082789</v>
+      </c>
+      <c r="C5">
+        <v>0.1750716187995824</v>
+      </c>
+      <c r="D5">
+        <v>0.2890848398746892</v>
+      </c>
+      <c r="E5">
+        <v>0.2744378742829458</v>
+      </c>
+      <c r="F5">
+        <v>0.2684965519858511</v>
+      </c>
+      <c r="G5">
+        <v>0.2684043977114589</v>
+      </c>
+      <c r="H5">
+        <v>0.288873363867502</v>
+      </c>
+      <c r="I5">
+        <v>0.2597976009690804</v>
+      </c>
+      <c r="J5">
+        <v>0.251693458605665</v>
+      </c>
+      <c r="K5">
+        <v>0.2344350474374066</v>
+      </c>
+      <c r="L5">
+        <v>0.01116511243619821</v>
+      </c>
+      <c r="M5">
+        <v>0.2396414284772545</v>
+      </c>
+      <c r="N5">
+        <v>0.290984635207768</v>
+      </c>
+      <c r="O5">
+        <v>0.2970974855986788</v>
+      </c>
+      <c r="P5">
+        <v>0.312706114360255</v>
+      </c>
+      <c r="Q5">
+        <v>0.3780815766488732</v>
+      </c>
+      <c r="R5">
+        <v>0.3880851187727803</v>
+      </c>
+      <c r="S5">
+        <v>0.3838628446330425</v>
+      </c>
+      <c r="T5">
+        <v>0.4585419539298044</v>
+      </c>
+      <c r="U5">
+        <v>0.4502600664085776</v>
+      </c>
+      <c r="V5">
+        <v>0.4242212189429646</v>
+      </c>
+      <c r="W5">
+        <v>0.01402748021711575</v>
+      </c>
+      <c r="X5">
+        <v>0.4657173727026709</v>
+      </c>
+      <c r="Y5">
+        <v>0.4383928731107648</v>
+      </c>
+      <c r="Z5">
+        <v>0.459513729384551</v>
+      </c>
+      <c r="AA5">
+        <v>0.615711562080528</v>
+      </c>
+      <c r="AB5">
+        <v>0.6186077384473645</v>
+      </c>
+      <c r="AC5">
+        <v>0.6116104683614789</v>
+      </c>
+      <c r="AD5">
+        <v>0.5163378661859894</v>
+      </c>
+      <c r="AE5">
+        <v>0.5576603121359391</v>
+      </c>
+      <c r="AF5">
+        <v>0.5445327039376731</v>
+      </c>
+      <c r="AG5">
+        <v>1.156490453635927</v>
+      </c>
+      <c r="AH5">
+        <v>0.2203103574328929</v>
+      </c>
+      <c r="AI5">
+        <v>1.131146284779263</v>
+      </c>
+      <c r="AJ5">
+        <v>1.126423594408779</v>
+      </c>
+      <c r="AK5">
+        <v>1.154344624684555</v>
+      </c>
+      <c r="AL5">
+        <v>1.133051205281654</v>
+      </c>
+      <c r="AM5">
+        <v>1.1398612996056</v>
+      </c>
+      <c r="AN5">
+        <v>1.217134182410509</v>
+      </c>
+      <c r="AO5">
+        <v>1.240710215406989</v>
+      </c>
+      <c r="AP5">
+        <v>1.260666619418507</v>
+      </c>
+      <c r="AQ5">
+        <v>1.256218792504037</v>
+      </c>
+      <c r="AR5">
+        <v>1.236803485493025</v>
+      </c>
+      <c r="AS5">
+        <v>0.2346015030006579</v>
+      </c>
+      <c r="AT5">
+        <v>1.262991623145054</v>
+      </c>
+      <c r="AU5">
+        <v>1.310891289812208</v>
+      </c>
+      <c r="AV5">
+        <v>1.296957326823001</v>
+      </c>
+      <c r="AW5">
+        <v>1.30972061749532</v>
+      </c>
+      <c r="AX5">
+        <v>1.250929662137866</v>
+      </c>
+      <c r="AY5">
+        <v>1.247777798863432</v>
+      </c>
+      <c r="AZ5">
+        <v>1.240194597507536</v>
+      </c>
+      <c r="BA5">
+        <v>1.319130365972271</v>
+      </c>
+      <c r="BB5">
+        <v>1.280903502793044</v>
+      </c>
+      <c r="BC5">
+        <v>1.296603695419857</v>
+      </c>
+      <c r="BD5">
+        <v>0.2429821024350673</v>
+      </c>
+      <c r="BE5">
+        <v>1.205024395054442</v>
+      </c>
+      <c r="BF5">
+        <v>1.215268634878065</v>
+      </c>
+      <c r="BG5">
+        <v>1.176498204519787</v>
+      </c>
+      <c r="BH5">
+        <v>1.442777376863091</v>
+      </c>
+      <c r="BI5">
+        <v>1.414179171950821</v>
+      </c>
+      <c r="BJ5">
+        <v>1.430777682913397</v>
+      </c>
+      <c r="BK5">
+        <v>1.4128790881607</v>
+      </c>
+      <c r="BL5">
+        <v>1.443968741246742</v>
+      </c>
+      <c r="BM5">
+        <v>1.420988286948955</v>
+      </c>
+      <c r="BN5">
+        <v>2.760139961080261</v>
+      </c>
+      <c r="BO5">
+        <v>0.1666897062290194</v>
+      </c>
+      <c r="BP5">
+        <v>2.813553185329114</v>
+      </c>
+      <c r="BQ5">
+        <v>2.811651848682326</v>
+      </c>
+      <c r="BR5">
+        <v>1.872951504573724</v>
+      </c>
+      <c r="BS5">
+        <v>1.803617547774103</v>
+      </c>
+      <c r="BT5">
+        <v>1.80425787564384</v>
+      </c>
+      <c r="BU5">
+        <v>1.873694755090048</v>
+      </c>
+      <c r="BV5">
+        <v>1.933464435466854</v>
+      </c>
+      <c r="BW5">
+        <v>1.888959187164408</v>
+      </c>
+      <c r="BX5">
+        <v>1.886639177835629</v>
+      </c>
+      <c r="BY5">
+        <v>1.887277238153974</v>
+      </c>
+      <c r="BZ5">
+        <v>0.1579967294129387</v>
+      </c>
+      <c r="CA5">
+        <v>1.858323361054042</v>
+      </c>
+      <c r="CB5">
+        <v>2.108191897831868</v>
+      </c>
+      <c r="CC5">
+        <v>2.138341436207218</v>
+      </c>
+      <c r="CD5">
+        <v>2.137896413905129</v>
+      </c>
+      <c r="CE5">
+        <v>2.08964915364912</v>
+      </c>
+      <c r="CF5">
+        <v>2.157898578671151</v>
+      </c>
+      <c r="CG5">
+        <v>2.093914529399436</v>
+      </c>
+      <c r="CH5">
+        <v>0.1788430909872715</v>
+      </c>
+      <c r="CI5">
+        <v>0.1850127532138407</v>
+      </c>
+    </row>
+    <row r="6" spans="1:87">
+      <c r="A6">
+        <v>0</v>
+      </c>
+      <c r="B6">
+        <v>0.04618049010047671</v>
+      </c>
+      <c r="C6">
+        <v>0.05660105263717474</v>
+      </c>
+      <c r="D6">
+        <v>0.1404435861315483</v>
+      </c>
+      <c r="E6">
+        <v>0.1129972831565304</v>
+      </c>
+      <c r="F6">
+        <v>0.1453107775944028</v>
+      </c>
+      <c r="G6">
+        <v>0.1334810937770101</v>
+      </c>
+      <c r="H6">
+        <v>0.1566303143704205</v>
+      </c>
+      <c r="I6">
+        <v>0.1355295441204163</v>
+      </c>
+      <c r="J6">
+        <v>0.1241187209410544</v>
+      </c>
+      <c r="K6">
+        <v>0.1276196893336042</v>
+      </c>
+      <c r="L6">
+        <v>-0.003840402552067633</v>
+      </c>
+      <c r="M6">
+        <v>0.1004957451604708</v>
+      </c>
+      <c r="N6">
+        <v>0.1720559465402511</v>
+      </c>
+      <c r="O6">
+        <v>0.1928764199905353</v>
+      </c>
+      <c r="P6">
+        <v>0.1727895077115985</v>
+      </c>
+      <c r="Q6">
+        <v>0.2238226611154495</v>
+      </c>
+      <c r="R6">
+        <v>0.2231275742656919</v>
+      </c>
+      <c r="S6">
+        <v>0.2389180156830674</v>
+      </c>
+      <c r="T6">
+        <v>0.2865781466545998</v>
+      </c>
+      <c r="U6">
+        <v>0.295858746089077</v>
+      </c>
+      <c r="V6">
+        <v>0.3009615773636864</v>
+      </c>
+      <c r="W6">
+        <v>0.007001353599929366</v>
+      </c>
+      <c r="X6">
+        <v>0.326475918346098</v>
+      </c>
+      <c r="Y6">
+        <v>0.3104874623196898</v>
+      </c>
+      <c r="Z6">
+        <v>0.341622288261455</v>
+      </c>
+      <c r="AA6">
+        <v>0.4215945782691212</v>
+      </c>
+      <c r="AB6">
+        <v>0.4294688744584179</v>
+      </c>
+      <c r="AC6">
+        <v>0.4548608398447015</v>
+      </c>
+      <c r="AD6">
+        <v>0.4107678897983407</v>
+      </c>
+      <c r="AE6">
+        <v>0.4202462873998518</v>
+      </c>
+      <c r="AF6">
+        <v>0.4400534671698642</v>
+      </c>
+      <c r="AG6">
+        <v>0.9965589039232278</v>
+      </c>
+      <c r="AH6">
+        <v>0.2085729231489898</v>
+      </c>
+      <c r="AI6">
+        <v>0.9775627895942107</v>
+      </c>
+      <c r="AJ6">
+        <v>0.9392526006422522</v>
+      </c>
+      <c r="AK6">
+        <v>0.9384632591771854</v>
+      </c>
+      <c r="AL6">
+        <v>0.9400950463767029</v>
+      </c>
+      <c r="AM6">
+        <v>0.9405674968129348</v>
+      </c>
+      <c r="AN6">
+        <v>1.011214820888098</v>
+      </c>
+      <c r="AO6">
+        <v>1.016319263455206</v>
+      </c>
+      <c r="AP6">
+        <v>1.045572195712293</v>
+      </c>
+      <c r="AQ6">
+        <v>1.016489194633488</v>
+      </c>
+      <c r="AR6">
+        <v>1.025402628562557</v>
+      </c>
+      <c r="AS6">
+        <v>0.2107291892734859</v>
+      </c>
+      <c r="AT6">
+        <v>1.015296954046005</v>
+      </c>
+      <c r="AU6">
+        <v>1.08998575457769</v>
+      </c>
+      <c r="AV6">
+        <v>1.076187666963908</v>
+      </c>
+      <c r="AW6">
+        <v>1.070350577039326</v>
+      </c>
+      <c r="AX6">
+        <v>1.01762947982831</v>
+      </c>
+      <c r="AY6">
+        <v>1.030289597858286</v>
+      </c>
+      <c r="AZ6">
+        <v>1.024942126674597</v>
+      </c>
+      <c r="BA6">
+        <v>1.050383162557839</v>
+      </c>
+      <c r="BB6">
+        <v>1.092254933154031</v>
+      </c>
+      <c r="BC6">
+        <v>1.09822167779114</v>
+      </c>
+      <c r="BD6">
+        <v>0.2359426421017406</v>
+      </c>
+      <c r="BE6">
+        <v>0.9523925047341975</v>
+      </c>
+      <c r="BF6">
+        <v>1.035088531458818</v>
+      </c>
+      <c r="BG6">
+        <v>0.9807408297827257</v>
+      </c>
+      <c r="BH6">
+        <v>1.191356993940401</v>
+      </c>
+      <c r="BI6">
+        <v>1.201910560472023</v>
+      </c>
+      <c r="BJ6">
+        <v>1.2184766318359</v>
+      </c>
+      <c r="BK6">
+        <v>1.186423776242012</v>
+      </c>
+      <c r="BL6">
+        <v>1.304553440054293</v>
+      </c>
+      <c r="BM6">
+        <v>1.222382950648558</v>
+      </c>
+      <c r="BN6">
+        <v>2.242925312456034</v>
+      </c>
+      <c r="BO6">
+        <v>0.07211756104950118</v>
+      </c>
+      <c r="BP6">
+        <v>2.173834750663177</v>
+      </c>
+      <c r="BQ6">
+        <v>2.252674025538894</v>
+      </c>
+      <c r="BR6">
+        <v>1.489589958837439</v>
+      </c>
+      <c r="BS6">
+        <v>1.512023919696251</v>
+      </c>
+      <c r="BT6">
+        <v>1.552012845938398</v>
+      </c>
+      <c r="BU6">
+        <v>1.670492050770646</v>
+      </c>
+      <c r="BV6">
+        <v>1.625057732931408</v>
+      </c>
+      <c r="BW6">
+        <v>1.675864123836584</v>
+      </c>
+      <c r="BX6">
+        <v>1.56561358516818</v>
+      </c>
+      <c r="BY6">
+        <v>1.649281507369268</v>
+      </c>
+      <c r="BZ6">
+        <v>0.03431128333213561</v>
+      </c>
+      <c r="CA6">
+        <v>1.612388089464998</v>
+      </c>
+      <c r="CB6">
+        <v>1.801793873707485</v>
+      </c>
+      <c r="CC6">
+        <v>1.881591187463184</v>
+      </c>
+      <c r="CD6">
+        <v>1.769034225942265</v>
+      </c>
+      <c r="CE6">
+        <v>1.820545299080496</v>
+      </c>
+      <c r="CF6">
+        <v>1.752036053586298</v>
+      </c>
+      <c r="CG6">
+        <v>1.790508605933244</v>
+      </c>
+      <c r="CH6">
+        <v>0.05008895685144273</v>
+      </c>
+      <c r="CI6">
+        <v>0.06627287461984564</v>
+      </c>
+    </row>
+    <row r="7" spans="1:87">
+      <c r="A7">
+        <v>0</v>
+      </c>
+      <c r="B7">
+        <v>0.08139561075577238</v>
+      </c>
+      <c r="C7">
+        <v>0.08580789983117487</v>
+      </c>
+      <c r="D7">
+        <v>0.2188236736177796</v>
+      </c>
+      <c r="E7">
+        <v>0.2033783344532896</v>
+      </c>
+      <c r="F7">
+        <v>0.1814783696929212</v>
+      </c>
+      <c r="G7">
+        <v>0.1877154390448533</v>
+      </c>
+      <c r="H7">
+        <v>0.2104282265880995</v>
+      </c>
+      <c r="I7">
+        <v>0.1921159350891234</v>
+      </c>
+      <c r="J7">
+        <v>0.1624031750507396</v>
+      </c>
+      <c r="K7">
+        <v>0.1358949407699438</v>
+      </c>
+      <c r="L7">
+        <v>0.01233184694713855</v>
+      </c>
+      <c r="M7">
+        <v>0.1938904951474605</v>
+      </c>
+      <c r="N7">
+        <v>0.2463740684337486</v>
+      </c>
+      <c r="O7">
+        <v>0.2174215592437918</v>
+      </c>
+      <c r="P7">
+        <v>0.2132178736942696</v>
+      </c>
+      <c r="Q7">
+        <v>0.3349426784622033</v>
+      </c>
+      <c r="R7">
+        <v>0.3668434489370849</v>
+      </c>
+      <c r="S7">
+        <v>0.2760251502098539</v>
+      </c>
+      <c r="T7">
+        <v>0.3640708838821</v>
+      </c>
+      <c r="U7">
+        <v>0.342690909572162</v>
+      </c>
+      <c r="V7">
+        <v>0.4456181228603575</v>
+      </c>
+      <c r="W7">
+        <v>0.03589530866177911</v>
+      </c>
+      <c r="X7">
+        <v>0.3575320177480512</v>
+      </c>
+      <c r="Y7">
+        <v>0.3617844519202073</v>
+      </c>
+      <c r="Z7">
+        <v>0.4090053258879582</v>
+      </c>
+      <c r="AA7">
+        <v>0.6120020618939226</v>
+      </c>
+      <c r="AB7">
+        <v>0.614626782827309</v>
+      </c>
+      <c r="AC7">
+        <v>0.5791489688119996</v>
+      </c>
+      <c r="AD7">
+        <v>0.5017647710425769</v>
+      </c>
+      <c r="AE7">
+        <v>0.489678767677242</v>
+      </c>
+      <c r="AF7">
+        <v>0.4631440780117863</v>
+      </c>
+      <c r="AG7">
+        <v>1.23091731600297</v>
+      </c>
+      <c r="AH7">
+        <v>0.2217959432978147</v>
+      </c>
+      <c r="AI7">
+        <v>1.389517363312149</v>
+      </c>
+      <c r="AJ7">
+        <v>1.380500487476161</v>
+      </c>
+      <c r="AK7">
+        <v>1.292199369509935</v>
+      </c>
+      <c r="AL7">
+        <v>1.117573344985812</v>
+      </c>
+      <c r="AM7">
+        <v>1.305691723231708</v>
+      </c>
+      <c r="AN7">
+        <v>1.602930376760634</v>
+      </c>
+      <c r="AO7">
+        <v>1.403550978622442</v>
+      </c>
+      <c r="AP7">
+        <v>1.525600570811129</v>
+      </c>
+      <c r="AQ7">
+        <v>1.484894420512529</v>
+      </c>
+      <c r="AR7">
+        <v>1.525600570811129</v>
+      </c>
+      <c r="AS7">
+        <v>0.2699811624978711</v>
+      </c>
+      <c r="AT7">
+        <v>1.516983793421944</v>
+      </c>
+      <c r="AU7">
+        <v>1.601896105798979</v>
+      </c>
+      <c r="AV7">
+        <v>1.407989077527697</v>
+      </c>
+      <c r="AW7">
+        <v>1.596922238622056</v>
+      </c>
+      <c r="AX7">
+        <v>1.550518291839777</v>
+      </c>
+      <c r="AY7">
+        <v>1.38199278486653</v>
+      </c>
+      <c r="AZ7">
+        <v>1.382500478386768</v>
+      </c>
+      <c r="BA7">
+        <v>1.473513180848214</v>
+      </c>
+      <c r="BB7">
+        <v>1.607102640956338</v>
+      </c>
+      <c r="BC7">
+        <v>1.556055712444142</v>
+      </c>
+      <c r="BD7">
+        <v>0.2710764792454293</v>
+      </c>
+      <c r="BE7">
+        <v>1.37983795834449</v>
+      </c>
+      <c r="BF7">
+        <v>1.416399336047944</v>
+      </c>
+      <c r="BG7">
+        <v>1.44083032705779</v>
+      </c>
+      <c r="BH7">
+        <v>1.658911452186672</v>
+      </c>
+      <c r="BI7">
+        <v>1.773067063912149</v>
+      </c>
+      <c r="BJ7">
+        <v>1.926080660151839</v>
+      </c>
+      <c r="BK7">
+        <v>1.680002939679785</v>
+      </c>
+      <c r="BL7">
+        <v>1.888063179885118</v>
+      </c>
+      <c r="BM7">
+        <v>1.789964692695393</v>
+      </c>
+      <c r="BO7">
+        <v>0.1062020160298224</v>
+      </c>
+      <c r="BR7">
+        <v>2.684462882471138</v>
+      </c>
+      <c r="BS7">
+        <v>2.498777989999738</v>
+      </c>
+      <c r="BT7">
+        <v>2.275318400961112</v>
+      </c>
+      <c r="BU7">
+        <v>2.714938376468172</v>
+      </c>
+      <c r="BV7">
+        <v>2.790374078712237</v>
+      </c>
+      <c r="BW7">
+        <v>2.889090844672491</v>
+      </c>
+      <c r="BX7">
+        <v>3.031002863128569</v>
+      </c>
+      <c r="BY7">
+        <v>2.858717110926029</v>
+      </c>
+      <c r="BZ7">
+        <v>0.0715543656274555</v>
+      </c>
+      <c r="CA7">
+        <v>2.892091199905992</v>
+      </c>
+      <c r="CB7">
+        <v>3.346224959460505</v>
+      </c>
+      <c r="CC7">
+        <v>3.748771574773756</v>
+      </c>
+      <c r="CD7">
+        <v>3.826215663449488</v>
+      </c>
+      <c r="CE7">
+        <v>3.670235156945154</v>
+      </c>
+      <c r="CF7">
+        <v>3.877437932587533</v>
+      </c>
+      <c r="CG7">
+        <v>3.69005895255929</v>
+      </c>
+      <c r="CH7">
+        <v>0.1090431169904558</v>
+      </c>
+      <c r="CI7">
+        <v>0.08244096957791737</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AC7"/>
   <sheetViews>
@@ -4634,1849 +6476,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:CI7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:87">
-      <c r="A1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="AG1" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="AH1" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="AI1" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="AJ1" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="AK1" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="AL1" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="AM1" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="AN1" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="AO1" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="AP1" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="AQ1" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="AR1" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="AS1" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="AT1" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="AU1" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="AV1" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="AW1" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="AX1" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="AY1" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="AZ1" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="BA1" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="BB1" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="BC1" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="BD1" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="BE1" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="BF1" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="BG1" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="BH1" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="BI1" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="BJ1" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="BK1" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="BL1" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="BM1" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="BN1" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="BO1" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="BP1" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="BQ1" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="BR1" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="BS1" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="BT1" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="BU1" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="BV1" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="BW1" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="BX1" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="BY1" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="BZ1" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="CA1" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="CB1" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="CC1" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="CD1" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="CE1" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="CF1" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="CG1" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="CH1" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="CI1" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="2" spans="1:87">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>0.06795099732174277</v>
-      </c>
-      <c r="C2">
-        <v>0.08185805465480191</v>
-      </c>
-      <c r="D2">
-        <v>0.1545338928394538</v>
-      </c>
-      <c r="E2">
-        <v>0.1595285979578524</v>
-      </c>
-      <c r="F2">
-        <v>0.1611356300105169</v>
-      </c>
-      <c r="G2">
-        <v>0.1657440760914083</v>
-      </c>
-      <c r="H2">
-        <v>0.1522321958209901</v>
-      </c>
-      <c r="I2">
-        <v>0.1604916017349513</v>
-      </c>
-      <c r="J2">
-        <v>0.1120118472991535</v>
-      </c>
-      <c r="K2">
-        <v>0.1194300125897388</v>
-      </c>
-      <c r="L2">
-        <v>0.002974758985301182</v>
-      </c>
-      <c r="M2">
-        <v>0.1121004179217738</v>
-      </c>
-      <c r="N2">
-        <v>0.1913025001408202</v>
-      </c>
-      <c r="O2">
-        <v>0.2010557087478083</v>
-      </c>
-      <c r="P2">
-        <v>0.1945269807809258</v>
-      </c>
-      <c r="Q2">
-        <v>0.2779525147030378</v>
-      </c>
-      <c r="R2">
-        <v>0.2690071736811264</v>
-      </c>
-      <c r="S2">
-        <v>0.2716118830993711</v>
-      </c>
-      <c r="T2">
-        <v>0.3176560953365489</v>
-      </c>
-      <c r="U2">
-        <v>0.3301819559422958</v>
-      </c>
-      <c r="V2">
-        <v>0.3131392511907007</v>
-      </c>
-      <c r="W2">
-        <v>0.001330261400455145</v>
-      </c>
-      <c r="X2">
-        <v>0.3266598543948022</v>
-      </c>
-      <c r="Y2">
-        <v>0.3319231269399354</v>
-      </c>
-      <c r="Z2">
-        <v>0.33346493110568</v>
-      </c>
-      <c r="AA2">
-        <v>0.4829306993669014</v>
-      </c>
-      <c r="AB2">
-        <v>0.4898524009478926</v>
-      </c>
-      <c r="AC2">
-        <v>0.4896019436102285</v>
-      </c>
-      <c r="AD2">
-        <v>0.4373970654521983</v>
-      </c>
-      <c r="AE2">
-        <v>0.4306792180796415</v>
-      </c>
-      <c r="AF2">
-        <v>0.4277006167351722</v>
-      </c>
-      <c r="AG2">
-        <v>1.01899263158486</v>
-      </c>
-      <c r="AH2">
-        <v>0.1995119506017013</v>
-      </c>
-      <c r="AI2">
-        <v>1.026949115133777</v>
-      </c>
-      <c r="AJ2">
-        <v>1.024379418627245</v>
-      </c>
-      <c r="AK2">
-        <v>1.013984726349174</v>
-      </c>
-      <c r="AL2">
-        <v>1.016103755226842</v>
-      </c>
-      <c r="AM2">
-        <v>1.017959728441051</v>
-      </c>
-      <c r="AN2">
-        <v>1.12178981811764</v>
-      </c>
-      <c r="AO2">
-        <v>1.128846836013933</v>
-      </c>
-      <c r="AP2">
-        <v>1.112898153439635</v>
-      </c>
-      <c r="AQ2">
-        <v>1.108901319659735</v>
-      </c>
-      <c r="AR2">
-        <v>1.107784533644136</v>
-      </c>
-      <c r="AS2">
-        <v>0.2078434700802005</v>
-      </c>
-      <c r="AT2">
-        <v>1.126976540244029</v>
-      </c>
-      <c r="AU2">
-        <v>1.15642433072145</v>
-      </c>
-      <c r="AV2">
-        <v>1.176725201038425</v>
-      </c>
-      <c r="AW2">
-        <v>1.144612984295044</v>
-      </c>
-      <c r="AX2">
-        <v>1.131278282202457</v>
-      </c>
-      <c r="AY2">
-        <v>1.117729844113085</v>
-      </c>
-      <c r="AZ2">
-        <v>1.116643994309363</v>
-      </c>
-      <c r="BA2">
-        <v>1.212702435619046</v>
-      </c>
-      <c r="BB2">
-        <v>1.21928876747057</v>
-      </c>
-      <c r="BC2">
-        <v>1.210609183259514</v>
-      </c>
-      <c r="BD2">
-        <v>0.204715584709188</v>
-      </c>
-      <c r="BE2">
-        <v>1.086805281829825</v>
-      </c>
-      <c r="BF2">
-        <v>1.084310676819978</v>
-      </c>
-      <c r="BG2">
-        <v>1.076349440387174</v>
-      </c>
-      <c r="BH2">
-        <v>1.313627091948996</v>
-      </c>
-      <c r="BI2">
-        <v>1.306779881285925</v>
-      </c>
-      <c r="BJ2">
-        <v>1.313414825429418</v>
-      </c>
-      <c r="BK2">
-        <v>1.301348894529031</v>
-      </c>
-      <c r="BL2">
-        <v>1.3051761215023</v>
-      </c>
-      <c r="BM2">
-        <v>1.317076515764124</v>
-      </c>
-      <c r="BN2">
-        <v>2.488672286634736</v>
-      </c>
-      <c r="BO2">
-        <v>0.06283595561770416</v>
-      </c>
-      <c r="BP2">
-        <v>2.474974116374596</v>
-      </c>
-      <c r="BQ2">
-        <v>2.475548528763476</v>
-      </c>
-      <c r="BR2">
-        <v>1.677426607305108</v>
-      </c>
-      <c r="BS2">
-        <v>1.681449415043503</v>
-      </c>
-      <c r="BT2">
-        <v>1.660453162689851</v>
-      </c>
-      <c r="BU2">
-        <v>1.714476497547774</v>
-      </c>
-      <c r="BV2">
-        <v>1.765027021071516</v>
-      </c>
-      <c r="BW2">
-        <v>1.690234886541741</v>
-      </c>
-      <c r="BX2">
-        <v>1.701908530833132</v>
-      </c>
-      <c r="BY2">
-        <v>1.704198085567938</v>
-      </c>
-      <c r="BZ2">
-        <v>0.04918456893420017</v>
-      </c>
-      <c r="CA2">
-        <v>1.687194530989987</v>
-      </c>
-      <c r="CB2">
-        <v>1.919785367810857</v>
-      </c>
-      <c r="CC2">
-        <v>1.928167274677659</v>
-      </c>
-      <c r="CD2">
-        <v>1.907916940354473</v>
-      </c>
-      <c r="CE2">
-        <v>1.919215747486826</v>
-      </c>
-      <c r="CF2">
-        <v>1.926238552017087</v>
-      </c>
-      <c r="CG2">
-        <v>1.912777983247811</v>
-      </c>
-      <c r="CH2">
-        <v>0.0614402292893785</v>
-      </c>
-      <c r="CI2">
-        <v>0.07791362787603238</v>
-      </c>
-    </row>
-    <row r="3" spans="1:87">
-      <c r="A3">
-        <v>0</v>
-      </c>
-      <c r="B3">
-        <v>0.06254309411229172</v>
-      </c>
-      <c r="C3">
-        <v>0.05785678103512904</v>
-      </c>
-      <c r="D3">
-        <v>0.1433899630497707</v>
-      </c>
-      <c r="E3">
-        <v>0.1483169813843757</v>
-      </c>
-      <c r="F3">
-        <v>0.1470527193014075</v>
-      </c>
-      <c r="G3">
-        <v>0.1496672710642195</v>
-      </c>
-      <c r="H3">
-        <v>0.1540524273499986</v>
-      </c>
-      <c r="I3">
-        <v>0.1578234254181533</v>
-      </c>
-      <c r="J3">
-        <v>0.1037213976898729</v>
-      </c>
-      <c r="K3">
-        <v>0.09495811317170584</v>
-      </c>
-      <c r="L3">
-        <v>0.002315853507733548</v>
-      </c>
-      <c r="M3">
-        <v>0.1011536916548215</v>
-      </c>
-      <c r="N3">
-        <v>0.1789797946206727</v>
-      </c>
-      <c r="O3">
-        <v>0.1726894573919343</v>
-      </c>
-      <c r="P3">
-        <v>0.1738728165946373</v>
-      </c>
-      <c r="Q3">
-        <v>0.2525142444596454</v>
-      </c>
-      <c r="R3">
-        <v>0.2475249976218991</v>
-      </c>
-      <c r="S3">
-        <v>0.255713639650946</v>
-      </c>
-      <c r="T3">
-        <v>0.2928322070710072</v>
-      </c>
-      <c r="U3">
-        <v>0.2940084387592624</v>
-      </c>
-      <c r="V3">
-        <v>0.3137637401213069</v>
-      </c>
-      <c r="W3">
-        <v>0.001869700701004347</v>
-      </c>
-      <c r="X3">
-        <v>0.3039233660583848</v>
-      </c>
-      <c r="Y3">
-        <v>0.3002289262914682</v>
-      </c>
-      <c r="Z3">
-        <v>0.3078415998742265</v>
-      </c>
-      <c r="AA3">
-        <v>0.4481233899072491</v>
-      </c>
-      <c r="AB3">
-        <v>0.4463180747955694</v>
-      </c>
-      <c r="AC3">
-        <v>0.4585852651378226</v>
-      </c>
-      <c r="AD3">
-        <v>0.4052696777173711</v>
-      </c>
-      <c r="AE3">
-        <v>0.4086558333297102</v>
-      </c>
-      <c r="AF3">
-        <v>0.4067019442358616</v>
-      </c>
-      <c r="AG3">
-        <v>0.985449928045534</v>
-      </c>
-      <c r="AH3">
-        <v>0.1928535557583117</v>
-      </c>
-      <c r="AI3">
-        <v>0.9940083474749077</v>
-      </c>
-      <c r="AJ3">
-        <v>0.9835278215611972</v>
-      </c>
-      <c r="AK3">
-        <v>0.953755380326761</v>
-      </c>
-      <c r="AL3">
-        <v>0.9819740242282641</v>
-      </c>
-      <c r="AM3">
-        <v>0.9788849928641112</v>
-      </c>
-      <c r="AN3">
-        <v>1.10425467251388</v>
-      </c>
-      <c r="AO3">
-        <v>1.098594181794953</v>
-      </c>
-      <c r="AP3">
-        <v>1.096510620778534</v>
-      </c>
-      <c r="AQ3">
-        <v>1.065805080491945</v>
-      </c>
-      <c r="AR3">
-        <v>1.065646616280369</v>
-      </c>
-      <c r="AS3">
-        <v>0.1900194398218211</v>
-      </c>
-      <c r="AT3">
-        <v>1.074111195167979</v>
-      </c>
-      <c r="AU3">
-        <v>1.123957093707858</v>
-      </c>
-      <c r="AV3">
-        <v>1.11245921217335</v>
-      </c>
-      <c r="AW3">
-        <v>1.105008508231081</v>
-      </c>
-      <c r="AX3">
-        <v>1.075295965202646</v>
-      </c>
-      <c r="AY3">
-        <v>1.082903579075164</v>
-      </c>
-      <c r="AZ3">
-        <v>1.083910664160616</v>
-      </c>
-      <c r="BA3">
-        <v>1.156531424687362</v>
-      </c>
-      <c r="BB3">
-        <v>1.153948784082036</v>
-      </c>
-      <c r="BC3">
-        <v>1.174401777410012</v>
-      </c>
-      <c r="BD3">
-        <v>0.1833590955163211</v>
-      </c>
-      <c r="BE3">
-        <v>1.045432144962698</v>
-      </c>
-      <c r="BF3">
-        <v>1.029427607496673</v>
-      </c>
-      <c r="BG3">
-        <v>1.037962699501496</v>
-      </c>
-      <c r="BH3">
-        <v>1.255249383946394</v>
-      </c>
-      <c r="BI3">
-        <v>1.288895485521961</v>
-      </c>
-      <c r="BJ3">
-        <v>1.265233471629128</v>
-      </c>
-      <c r="BK3">
-        <v>1.260028518855096</v>
-      </c>
-      <c r="BL3">
-        <v>1.254994352563541</v>
-      </c>
-      <c r="BM3">
-        <v>1.245648968037489</v>
-      </c>
-      <c r="BN3">
-        <v>2.419851279703033</v>
-      </c>
-      <c r="BO3">
-        <v>0.0320701584753309</v>
-      </c>
-      <c r="BP3">
-        <v>2.389803366704771</v>
-      </c>
-      <c r="BQ3">
-        <v>2.402928895117701</v>
-      </c>
-      <c r="BR3">
-        <v>1.63023505717894</v>
-      </c>
-      <c r="BS3">
-        <v>1.651122404539787</v>
-      </c>
-      <c r="BT3">
-        <v>1.613737177433537</v>
-      </c>
-      <c r="BU3">
-        <v>1.660786902927901</v>
-      </c>
-      <c r="BV3">
-        <v>1.683014039654155</v>
-      </c>
-      <c r="BW3">
-        <v>1.676140434024832</v>
-      </c>
-      <c r="BX3">
-        <v>1.660140996320911</v>
-      </c>
-      <c r="BY3">
-        <v>1.634348831846555</v>
-      </c>
-      <c r="BZ3">
-        <v>0.03093495153954072</v>
-      </c>
-      <c r="CA3">
-        <v>1.628704209351442</v>
-      </c>
-      <c r="CB3">
-        <v>1.876055044353057</v>
-      </c>
-      <c r="CC3">
-        <v>1.868342932769132</v>
-      </c>
-      <c r="CD3">
-        <v>1.875966400268557</v>
-      </c>
-      <c r="CE3">
-        <v>1.860660744604795</v>
-      </c>
-      <c r="CF3">
-        <v>1.860135408236272</v>
-      </c>
-      <c r="CG3">
-        <v>1.8299393991325</v>
-      </c>
-      <c r="CH3">
-        <v>0.03044318140292155</v>
-      </c>
-      <c r="CI3">
-        <v>0.05513501163719099</v>
-      </c>
-    </row>
-    <row r="4" spans="1:87">
-      <c r="A4">
-        <v>0</v>
-      </c>
-      <c r="B4">
-        <v>0.03833920716397395</v>
-      </c>
-      <c r="C4">
-        <v>0.04367385821915429</v>
-      </c>
-      <c r="D4">
-        <v>0.1297175473504567</v>
-      </c>
-      <c r="E4">
-        <v>0.1314549432236708</v>
-      </c>
-      <c r="F4">
-        <v>0.126546191620998</v>
-      </c>
-      <c r="G4">
-        <v>0.1408241820141943</v>
-      </c>
-      <c r="H4">
-        <v>0.14193599480132</v>
-      </c>
-      <c r="I4">
-        <v>0.1469368819771829</v>
-      </c>
-      <c r="J4">
-        <v>0.09187943693942219</v>
-      </c>
-      <c r="K4">
-        <v>0.09279983223092153</v>
-      </c>
-      <c r="L4">
-        <v>-0.001004910967455668</v>
-      </c>
-      <c r="M4">
-        <v>0.1031102377321041</v>
-      </c>
-      <c r="N4">
-        <v>0.1557520307000901</v>
-      </c>
-      <c r="O4">
-        <v>0.1553085342176607</v>
-      </c>
-      <c r="P4">
-        <v>0.1525362433194694</v>
-      </c>
-      <c r="Q4">
-        <v>0.2528441489259688</v>
-      </c>
-      <c r="R4">
-        <v>0.2357826949753737</v>
-      </c>
-      <c r="S4">
-        <v>0.2358582630510093</v>
-      </c>
-      <c r="T4">
-        <v>0.2796335062737026</v>
-      </c>
-      <c r="U4">
-        <v>0.2823934259153261</v>
-      </c>
-      <c r="V4">
-        <v>0.3132074683489514</v>
-      </c>
-      <c r="W4">
-        <v>0.01151183258022224</v>
-      </c>
-      <c r="X4">
-        <v>0.2966779126958042</v>
-      </c>
-      <c r="Y4">
-        <v>0.285126218778282</v>
-      </c>
-      <c r="Z4">
-        <v>0.3017339166970138</v>
-      </c>
-      <c r="AA4">
-        <v>0.4558772986221947</v>
-      </c>
-      <c r="AB4">
-        <v>0.4528359006649535</v>
-      </c>
-      <c r="AC4">
-        <v>0.4573808235033963</v>
-      </c>
-      <c r="AD4">
-        <v>0.4101833791173501</v>
-      </c>
-      <c r="AE4">
-        <v>0.4229486839812581</v>
-      </c>
-      <c r="AF4">
-        <v>0.4091607952057537</v>
-      </c>
-      <c r="AG4">
-        <v>1.024477842413456</v>
-      </c>
-      <c r="AH4">
-        <v>0.188325535155088</v>
-      </c>
-      <c r="AI4">
-        <v>1.004498740112759</v>
-      </c>
-      <c r="AJ4">
-        <v>1.00460740855161</v>
-      </c>
-      <c r="AK4">
-        <v>0.9748877903160449</v>
-      </c>
-      <c r="AL4">
-        <v>0.9741640868250526</v>
-      </c>
-      <c r="AM4">
-        <v>0.9679925760233756</v>
-      </c>
-      <c r="AN4">
-        <v>1.099505350093428</v>
-      </c>
-      <c r="AO4">
-        <v>1.122928633549595</v>
-      </c>
-      <c r="AP4">
-        <v>1.085626175492969</v>
-      </c>
-      <c r="AQ4">
-        <v>1.092988516261982</v>
-      </c>
-      <c r="AR4">
-        <v>1.103531673330121</v>
-      </c>
-      <c r="AS4">
-        <v>0.2014408876085131</v>
-      </c>
-      <c r="AT4">
-        <v>1.103110674663337</v>
-      </c>
-      <c r="AU4">
-        <v>1.172028554412571</v>
-      </c>
-      <c r="AV4">
-        <v>1.167673494442184</v>
-      </c>
-      <c r="AW4">
-        <v>1.168423750731289</v>
-      </c>
-      <c r="AX4">
-        <v>1.125860318784975</v>
-      </c>
-      <c r="AY4">
-        <v>1.106687745906473</v>
-      </c>
-      <c r="AZ4">
-        <v>1.117439128134247</v>
-      </c>
-      <c r="BA4">
-        <v>1.187103285661931</v>
-      </c>
-      <c r="BB4">
-        <v>1.17566789098289</v>
-      </c>
-      <c r="BC4">
-        <v>1.168209155089518</v>
-      </c>
-      <c r="BD4">
-        <v>0.1905223314708753</v>
-      </c>
-      <c r="BE4">
-        <v>1.068966952670205</v>
-      </c>
-      <c r="BF4">
-        <v>1.060162313290766</v>
-      </c>
-      <c r="BG4">
-        <v>1.084601906465271</v>
-      </c>
-      <c r="BH4">
-        <v>1.300468441429387</v>
-      </c>
-      <c r="BI4">
-        <v>1.318199809783778</v>
-      </c>
-      <c r="BJ4">
-        <v>1.31284049392728</v>
-      </c>
-      <c r="BK4">
-        <v>1.317602262333849</v>
-      </c>
-      <c r="BL4">
-        <v>1.282926373557593</v>
-      </c>
-      <c r="BM4">
-        <v>1.320491286496821</v>
-      </c>
-      <c r="BN4">
-        <v>2.636961302139714</v>
-      </c>
-      <c r="BO4">
-        <v>0.02138087320821584</v>
-      </c>
-      <c r="BP4">
-        <v>2.587155235745727</v>
-      </c>
-      <c r="BQ4">
-        <v>2.651770855926393</v>
-      </c>
-      <c r="BR4">
-        <v>1.720932236206869</v>
-      </c>
-      <c r="BS4">
-        <v>1.722383544002407</v>
-      </c>
-      <c r="BT4">
-        <v>1.711706377621188</v>
-      </c>
-      <c r="BU4">
-        <v>1.781260444724237</v>
-      </c>
-      <c r="BV4">
-        <v>1.785818006532374</v>
-      </c>
-      <c r="BW4">
-        <v>1.763899655059693</v>
-      </c>
-      <c r="BX4">
-        <v>1.719517875086779</v>
-      </c>
-      <c r="BY4">
-        <v>1.74203260405706</v>
-      </c>
-      <c r="BZ4">
-        <v>0.01194290195077402</v>
-      </c>
-      <c r="CA4">
-        <v>1.714476042920863</v>
-      </c>
-      <c r="CB4">
-        <v>1.953065676662382</v>
-      </c>
-      <c r="CC4">
-        <v>2.002280908260923</v>
-      </c>
-      <c r="CD4">
-        <v>2.009111662658423</v>
-      </c>
-      <c r="CE4">
-        <v>1.949364643123308</v>
-      </c>
-      <c r="CF4">
-        <v>1.983909284890204</v>
-      </c>
-      <c r="CG4">
-        <v>1.994716192448075</v>
-      </c>
-      <c r="CH4">
-        <v>0.03445170658732304</v>
-      </c>
-      <c r="CI4">
-        <v>0.05372631012837377</v>
-      </c>
-    </row>
-    <row r="5" spans="1:87">
-      <c r="A5">
-        <v>0</v>
-      </c>
-      <c r="B5">
-        <v>0.1881966511082789</v>
-      </c>
-      <c r="C5">
-        <v>0.1750716187995824</v>
-      </c>
-      <c r="D5">
-        <v>0.2890848398746892</v>
-      </c>
-      <c r="E5">
-        <v>0.2744378742829458</v>
-      </c>
-      <c r="F5">
-        <v>0.2684965519858511</v>
-      </c>
-      <c r="G5">
-        <v>0.2684043977114589</v>
-      </c>
-      <c r="H5">
-        <v>0.288873363867502</v>
-      </c>
-      <c r="I5">
-        <v>0.2597976009690804</v>
-      </c>
-      <c r="J5">
-        <v>0.251693458605665</v>
-      </c>
-      <c r="K5">
-        <v>0.2344350474374066</v>
-      </c>
-      <c r="L5">
-        <v>0.01116511243619821</v>
-      </c>
-      <c r="M5">
-        <v>0.2396414284772545</v>
-      </c>
-      <c r="N5">
-        <v>0.290984635207768</v>
-      </c>
-      <c r="O5">
-        <v>0.2970974855986788</v>
-      </c>
-      <c r="P5">
-        <v>0.312706114360255</v>
-      </c>
-      <c r="Q5">
-        <v>0.3780815766488732</v>
-      </c>
-      <c r="R5">
-        <v>0.3880851187727803</v>
-      </c>
-      <c r="S5">
-        <v>0.3838628446330425</v>
-      </c>
-      <c r="T5">
-        <v>0.4585419539298044</v>
-      </c>
-      <c r="U5">
-        <v>0.4502600664085776</v>
-      </c>
-      <c r="V5">
-        <v>0.4242212189429646</v>
-      </c>
-      <c r="W5">
-        <v>0.01402748021711575</v>
-      </c>
-      <c r="X5">
-        <v>0.4657173727026709</v>
-      </c>
-      <c r="Y5">
-        <v>0.4383928731107648</v>
-      </c>
-      <c r="Z5">
-        <v>0.459513729384551</v>
-      </c>
-      <c r="AA5">
-        <v>0.615711562080528</v>
-      </c>
-      <c r="AB5">
-        <v>0.6186077384473645</v>
-      </c>
-      <c r="AC5">
-        <v>0.6116104683614789</v>
-      </c>
-      <c r="AD5">
-        <v>0.5163378661859894</v>
-      </c>
-      <c r="AE5">
-        <v>0.5576603121359391</v>
-      </c>
-      <c r="AF5">
-        <v>0.5445327039376731</v>
-      </c>
-      <c r="AG5">
-        <v>1.156490453635927</v>
-      </c>
-      <c r="AH5">
-        <v>0.2203103574328929</v>
-      </c>
-      <c r="AI5">
-        <v>1.131146284779263</v>
-      </c>
-      <c r="AJ5">
-        <v>1.126423594408779</v>
-      </c>
-      <c r="AK5">
-        <v>1.154344624684555</v>
-      </c>
-      <c r="AL5">
-        <v>1.133051205281654</v>
-      </c>
-      <c r="AM5">
-        <v>1.1398612996056</v>
-      </c>
-      <c r="AN5">
-        <v>1.217134182410509</v>
-      </c>
-      <c r="AO5">
-        <v>1.240710215406989</v>
-      </c>
-      <c r="AP5">
-        <v>1.260666619418507</v>
-      </c>
-      <c r="AQ5">
-        <v>1.256218792504037</v>
-      </c>
-      <c r="AR5">
-        <v>1.236803485493025</v>
-      </c>
-      <c r="AS5">
-        <v>0.2346015030006579</v>
-      </c>
-      <c r="AT5">
-        <v>1.262991623145054</v>
-      </c>
-      <c r="AU5">
-        <v>1.310891289812208</v>
-      </c>
-      <c r="AV5">
-        <v>1.296957326823001</v>
-      </c>
-      <c r="AW5">
-        <v>1.30972061749532</v>
-      </c>
-      <c r="AX5">
-        <v>1.250929662137866</v>
-      </c>
-      <c r="AY5">
-        <v>1.247777798863432</v>
-      </c>
-      <c r="AZ5">
-        <v>1.240194597507536</v>
-      </c>
-      <c r="BA5">
-        <v>1.319130365972271</v>
-      </c>
-      <c r="BB5">
-        <v>1.280903502793044</v>
-      </c>
-      <c r="BC5">
-        <v>1.296603695419857</v>
-      </c>
-      <c r="BD5">
-        <v>0.2429821024350673</v>
-      </c>
-      <c r="BE5">
-        <v>1.205024395054442</v>
-      </c>
-      <c r="BF5">
-        <v>1.215268634878065</v>
-      </c>
-      <c r="BG5">
-        <v>1.176498204519787</v>
-      </c>
-      <c r="BH5">
-        <v>1.442777376863091</v>
-      </c>
-      <c r="BI5">
-        <v>1.414179171950821</v>
-      </c>
-      <c r="BJ5">
-        <v>1.430777682913397</v>
-      </c>
-      <c r="BK5">
-        <v>1.4128790881607</v>
-      </c>
-      <c r="BL5">
-        <v>1.443968741246742</v>
-      </c>
-      <c r="BM5">
-        <v>1.420988286948955</v>
-      </c>
-      <c r="BN5">
-        <v>2.760139961080261</v>
-      </c>
-      <c r="BO5">
-        <v>0.1666897062290194</v>
-      </c>
-      <c r="BP5">
-        <v>2.813553185329114</v>
-      </c>
-      <c r="BQ5">
-        <v>2.811651848682326</v>
-      </c>
-      <c r="BR5">
-        <v>1.872951504573724</v>
-      </c>
-      <c r="BS5">
-        <v>1.803617547774103</v>
-      </c>
-      <c r="BT5">
-        <v>1.80425787564384</v>
-      </c>
-      <c r="BU5">
-        <v>1.873694755090048</v>
-      </c>
-      <c r="BV5">
-        <v>1.933464435466854</v>
-      </c>
-      <c r="BW5">
-        <v>1.888959187164408</v>
-      </c>
-      <c r="BX5">
-        <v>1.886639177835629</v>
-      </c>
-      <c r="BY5">
-        <v>1.887277238153974</v>
-      </c>
-      <c r="BZ5">
-        <v>0.1579967294129387</v>
-      </c>
-      <c r="CA5">
-        <v>1.858323361054042</v>
-      </c>
-      <c r="CB5">
-        <v>2.108191897831868</v>
-      </c>
-      <c r="CC5">
-        <v>2.138341436207218</v>
-      </c>
-      <c r="CD5">
-        <v>2.137896413905129</v>
-      </c>
-      <c r="CE5">
-        <v>2.08964915364912</v>
-      </c>
-      <c r="CF5">
-        <v>2.157898578671151</v>
-      </c>
-      <c r="CG5">
-        <v>2.093914529399436</v>
-      </c>
-      <c r="CH5">
-        <v>0.1788430909872715</v>
-      </c>
-      <c r="CI5">
-        <v>0.1850127532138407</v>
-      </c>
-    </row>
-    <row r="6" spans="1:87">
-      <c r="A6">
-        <v>0</v>
-      </c>
-      <c r="B6">
-        <v>0.04618049010047671</v>
-      </c>
-      <c r="C6">
-        <v>0.05660105263717474</v>
-      </c>
-      <c r="D6">
-        <v>0.1404435861315483</v>
-      </c>
-      <c r="E6">
-        <v>0.1129972831565304</v>
-      </c>
-      <c r="F6">
-        <v>0.1453107775944028</v>
-      </c>
-      <c r="G6">
-        <v>0.1334810937770101</v>
-      </c>
-      <c r="H6">
-        <v>0.1566303143704205</v>
-      </c>
-      <c r="I6">
-        <v>0.1355295441204163</v>
-      </c>
-      <c r="J6">
-        <v>0.1241187209410544</v>
-      </c>
-      <c r="K6">
-        <v>0.1276196893336042</v>
-      </c>
-      <c r="L6">
-        <v>-0.003840402552067633</v>
-      </c>
-      <c r="M6">
-        <v>0.1004957451604708</v>
-      </c>
-      <c r="N6">
-        <v>0.1720559465402511</v>
-      </c>
-      <c r="O6">
-        <v>0.1928764199905353</v>
-      </c>
-      <c r="P6">
-        <v>0.1727895077115985</v>
-      </c>
-      <c r="Q6">
-        <v>0.2238226611154495</v>
-      </c>
-      <c r="R6">
-        <v>0.2231275742656919</v>
-      </c>
-      <c r="S6">
-        <v>0.2389180156830674</v>
-      </c>
-      <c r="T6">
-        <v>0.2865781466545998</v>
-      </c>
-      <c r="U6">
-        <v>0.295858746089077</v>
-      </c>
-      <c r="V6">
-        <v>0.3009615773636864</v>
-      </c>
-      <c r="W6">
-        <v>0.007001353599929366</v>
-      </c>
-      <c r="X6">
-        <v>0.326475918346098</v>
-      </c>
-      <c r="Y6">
-        <v>0.3104874623196898</v>
-      </c>
-      <c r="Z6">
-        <v>0.341622288261455</v>
-      </c>
-      <c r="AA6">
-        <v>0.4215945782691212</v>
-      </c>
-      <c r="AB6">
-        <v>0.4294688744584179</v>
-      </c>
-      <c r="AC6">
-        <v>0.4548608398447015</v>
-      </c>
-      <c r="AD6">
-        <v>0.4107678897983407</v>
-      </c>
-      <c r="AE6">
-        <v>0.4202462873998518</v>
-      </c>
-      <c r="AF6">
-        <v>0.4400534671698642</v>
-      </c>
-      <c r="AG6">
-        <v>0.9965589039232278</v>
-      </c>
-      <c r="AH6">
-        <v>0.2085729231489898</v>
-      </c>
-      <c r="AI6">
-        <v>0.9775627895942107</v>
-      </c>
-      <c r="AJ6">
-        <v>0.9392526006422522</v>
-      </c>
-      <c r="AK6">
-        <v>0.9384632591771854</v>
-      </c>
-      <c r="AL6">
-        <v>0.9400950463767029</v>
-      </c>
-      <c r="AM6">
-        <v>0.9405674968129348</v>
-      </c>
-      <c r="AN6">
-        <v>1.011214820888098</v>
-      </c>
-      <c r="AO6">
-        <v>1.016319263455206</v>
-      </c>
-      <c r="AP6">
-        <v>1.045572195712293</v>
-      </c>
-      <c r="AQ6">
-        <v>1.016489194633488</v>
-      </c>
-      <c r="AR6">
-        <v>1.025402628562557</v>
-      </c>
-      <c r="AS6">
-        <v>0.2107291892734859</v>
-      </c>
-      <c r="AT6">
-        <v>1.015296954046005</v>
-      </c>
-      <c r="AU6">
-        <v>1.08998575457769</v>
-      </c>
-      <c r="AV6">
-        <v>1.076187666963908</v>
-      </c>
-      <c r="AW6">
-        <v>1.070350577039326</v>
-      </c>
-      <c r="AX6">
-        <v>1.01762947982831</v>
-      </c>
-      <c r="AY6">
-        <v>1.030289597858286</v>
-      </c>
-      <c r="AZ6">
-        <v>1.024942126674597</v>
-      </c>
-      <c r="BA6">
-        <v>1.050383162557839</v>
-      </c>
-      <c r="BB6">
-        <v>1.092254933154031</v>
-      </c>
-      <c r="BC6">
-        <v>1.09822167779114</v>
-      </c>
-      <c r="BD6">
-        <v>0.2359426421017406</v>
-      </c>
-      <c r="BE6">
-        <v>0.9523925047341975</v>
-      </c>
-      <c r="BF6">
-        <v>1.035088531458818</v>
-      </c>
-      <c r="BG6">
-        <v>0.9807408297827257</v>
-      </c>
-      <c r="BH6">
-        <v>1.191356993940401</v>
-      </c>
-      <c r="BI6">
-        <v>1.201910560472023</v>
-      </c>
-      <c r="BJ6">
-        <v>1.2184766318359</v>
-      </c>
-      <c r="BK6">
-        <v>1.186423776242012</v>
-      </c>
-      <c r="BL6">
-        <v>1.304553440054293</v>
-      </c>
-      <c r="BM6">
-        <v>1.222382950648558</v>
-      </c>
-      <c r="BN6">
-        <v>2.242925312456034</v>
-      </c>
-      <c r="BO6">
-        <v>0.07211756104950118</v>
-      </c>
-      <c r="BP6">
-        <v>2.173834750663177</v>
-      </c>
-      <c r="BQ6">
-        <v>2.252674025538894</v>
-      </c>
-      <c r="BR6">
-        <v>1.489589958837439</v>
-      </c>
-      <c r="BS6">
-        <v>1.512023919696251</v>
-      </c>
-      <c r="BT6">
-        <v>1.552012845938398</v>
-      </c>
-      <c r="BU6">
-        <v>1.670492050770646</v>
-      </c>
-      <c r="BV6">
-        <v>1.625057732931408</v>
-      </c>
-      <c r="BW6">
-        <v>1.675864123836584</v>
-      </c>
-      <c r="BX6">
-        <v>1.56561358516818</v>
-      </c>
-      <c r="BY6">
-        <v>1.649281507369268</v>
-      </c>
-      <c r="BZ6">
-        <v>0.03431128333213561</v>
-      </c>
-      <c r="CA6">
-        <v>1.612388089464998</v>
-      </c>
-      <c r="CB6">
-        <v>1.801793873707485</v>
-      </c>
-      <c r="CC6">
-        <v>1.881591187463184</v>
-      </c>
-      <c r="CD6">
-        <v>1.769034225942265</v>
-      </c>
-      <c r="CE6">
-        <v>1.820545299080496</v>
-      </c>
-      <c r="CF6">
-        <v>1.752036053586298</v>
-      </c>
-      <c r="CG6">
-        <v>1.790508605933244</v>
-      </c>
-      <c r="CH6">
-        <v>0.05008895685144273</v>
-      </c>
-      <c r="CI6">
-        <v>0.06627287461984564</v>
-      </c>
-    </row>
-    <row r="7" spans="1:87">
-      <c r="A7">
-        <v>0</v>
-      </c>
-      <c r="B7">
-        <v>0.08139561075577238</v>
-      </c>
-      <c r="C7">
-        <v>0.08580789983117487</v>
-      </c>
-      <c r="D7">
-        <v>0.2188236736177796</v>
-      </c>
-      <c r="E7">
-        <v>0.2033783344532896</v>
-      </c>
-      <c r="F7">
-        <v>0.1814783696929212</v>
-      </c>
-      <c r="G7">
-        <v>0.1877154390448533</v>
-      </c>
-      <c r="H7">
-        <v>0.2104282265880995</v>
-      </c>
-      <c r="I7">
-        <v>0.1921159350891234</v>
-      </c>
-      <c r="J7">
-        <v>0.1624031750507396</v>
-      </c>
-      <c r="K7">
-        <v>0.1358949407699438</v>
-      </c>
-      <c r="L7">
-        <v>0.01233184694713855</v>
-      </c>
-      <c r="M7">
-        <v>0.1938904951474605</v>
-      </c>
-      <c r="N7">
-        <v>0.2463740684337486</v>
-      </c>
-      <c r="O7">
-        <v>0.2174215592437918</v>
-      </c>
-      <c r="P7">
-        <v>0.2132178736942696</v>
-      </c>
-      <c r="Q7">
-        <v>0.3349426784622033</v>
-      </c>
-      <c r="R7">
-        <v>0.3668434489370849</v>
-      </c>
-      <c r="S7">
-        <v>0.2760251502098539</v>
-      </c>
-      <c r="T7">
-        <v>0.3640708838821</v>
-      </c>
-      <c r="U7">
-        <v>0.342690909572162</v>
-      </c>
-      <c r="V7">
-        <v>0.4456181228603575</v>
-      </c>
-      <c r="W7">
-        <v>0.03589530866177911</v>
-      </c>
-      <c r="X7">
-        <v>0.3575320177480512</v>
-      </c>
-      <c r="Y7">
-        <v>0.3617844519202073</v>
-      </c>
-      <c r="Z7">
-        <v>0.4090053258879582</v>
-      </c>
-      <c r="AA7">
-        <v>0.6120020618939226</v>
-      </c>
-      <c r="AB7">
-        <v>0.614626782827309</v>
-      </c>
-      <c r="AC7">
-        <v>0.5791489688119996</v>
-      </c>
-      <c r="AD7">
-        <v>0.5017647710425769</v>
-      </c>
-      <c r="AE7">
-        <v>0.489678767677242</v>
-      </c>
-      <c r="AF7">
-        <v>0.4631440780117863</v>
-      </c>
-      <c r="AG7">
-        <v>1.23091731600297</v>
-      </c>
-      <c r="AH7">
-        <v>0.2217959432978147</v>
-      </c>
-      <c r="AI7">
-        <v>1.389517363312149</v>
-      </c>
-      <c r="AJ7">
-        <v>1.380500487476161</v>
-      </c>
-      <c r="AK7">
-        <v>1.292199369509935</v>
-      </c>
-      <c r="AL7">
-        <v>1.117573344985812</v>
-      </c>
-      <c r="AM7">
-        <v>1.305691723231708</v>
-      </c>
-      <c r="AN7">
-        <v>1.602930376760634</v>
-      </c>
-      <c r="AO7">
-        <v>1.403550978622442</v>
-      </c>
-      <c r="AP7">
-        <v>1.525600570811129</v>
-      </c>
-      <c r="AQ7">
-        <v>1.484894420512529</v>
-      </c>
-      <c r="AR7">
-        <v>1.525600570811129</v>
-      </c>
-      <c r="AS7">
-        <v>0.2699811624978711</v>
-      </c>
-      <c r="AT7">
-        <v>1.516983793421944</v>
-      </c>
-      <c r="AU7">
-        <v>1.601896105798979</v>
-      </c>
-      <c r="AV7">
-        <v>1.407989077527697</v>
-      </c>
-      <c r="AW7">
-        <v>1.596922238622056</v>
-      </c>
-      <c r="AX7">
-        <v>1.550518291839777</v>
-      </c>
-      <c r="AY7">
-        <v>1.38199278486653</v>
-      </c>
-      <c r="AZ7">
-        <v>1.382500478386768</v>
-      </c>
-      <c r="BA7">
-        <v>1.473513180848214</v>
-      </c>
-      <c r="BB7">
-        <v>1.607102640956338</v>
-      </c>
-      <c r="BC7">
-        <v>1.556055712444142</v>
-      </c>
-      <c r="BD7">
-        <v>0.2710764792454293</v>
-      </c>
-      <c r="BE7">
-        <v>1.37983795834449</v>
-      </c>
-      <c r="BF7">
-        <v>1.416399336047944</v>
-      </c>
-      <c r="BG7">
-        <v>1.44083032705779</v>
-      </c>
-      <c r="BH7">
-        <v>1.658911452186672</v>
-      </c>
-      <c r="BI7">
-        <v>1.773067063912149</v>
-      </c>
-      <c r="BJ7">
-        <v>1.926080660151839</v>
-      </c>
-      <c r="BK7">
-        <v>1.680002939679785</v>
-      </c>
-      <c r="BL7">
-        <v>1.888063179885118</v>
-      </c>
-      <c r="BM7">
-        <v>1.789964692695393</v>
-      </c>
-      <c r="BO7">
-        <v>0.1062020160298224</v>
-      </c>
-      <c r="BR7">
-        <v>2.684462882471138</v>
-      </c>
-      <c r="BS7">
-        <v>2.498777989999738</v>
-      </c>
-      <c r="BT7">
-        <v>2.275318400961112</v>
-      </c>
-      <c r="BU7">
-        <v>2.714938376468172</v>
-      </c>
-      <c r="BV7">
-        <v>2.790374078712237</v>
-      </c>
-      <c r="BW7">
-        <v>2.889090844672491</v>
-      </c>
-      <c r="BX7">
-        <v>3.031002863128569</v>
-      </c>
-      <c r="BY7">
-        <v>2.858717110926029</v>
-      </c>
-      <c r="BZ7">
-        <v>0.0715543656274555</v>
-      </c>
-      <c r="CA7">
-        <v>2.892091199905992</v>
-      </c>
-      <c r="CB7">
-        <v>3.346224959460505</v>
-      </c>
-      <c r="CC7">
-        <v>3.748771574773756</v>
-      </c>
-      <c r="CD7">
-        <v>3.826215663449488</v>
-      </c>
-      <c r="CE7">
-        <v>3.670235156945154</v>
-      </c>
-      <c r="CF7">
-        <v>3.877437932587533</v>
-      </c>
-      <c r="CG7">
-        <v>3.69005895255929</v>
-      </c>
-      <c r="CH7">
-        <v>0.1090431169904558</v>
-      </c>
-      <c r="CI7">
-        <v>0.08244096957791737</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed data handling issues, added filter to remove negative values from initial dataset, added function to bark out negative data values in absorbance calculations.
</commit_message>
<xml_diff>
--- a/combined_dataframes.xlsx
+++ b/combined_dataframes.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="92">
   <si>
     <t>Wavelength</t>
   </si>
@@ -291,6 +291,9 @@
   </si>
   <si>
     <t>STDMaterial_18</t>
+  </si>
+  <si>
+    <t>inf</t>
   </si>
 </sst>
 </file>
@@ -718,58 +721,58 @@
         <v>630.188</v>
       </c>
       <c r="B2">
-        <v>13969.45642333333</v>
+        <v>41886.28602333333</v>
       </c>
       <c r="C2">
-        <v>19.02787666666667</v>
+        <v>30123.27569</v>
       </c>
       <c r="D2">
-        <v>1.9357</v>
+        <v>20.811775</v>
       </c>
       <c r="E2">
-        <v>13975.28592333333</v>
+        <v>18.441265</v>
       </c>
       <c r="F2">
-        <v>16.1025</v>
+        <v>38.112315</v>
       </c>
       <c r="G2">
-        <v>76.70576666666666</v>
+        <v>50.4082</v>
       </c>
       <c r="H2">
-        <v>105.6347533333333</v>
+        <v>12.82031</v>
       </c>
       <c r="I2">
-        <v>15585.20577</v>
+        <v>34.89241666666667</v>
       </c>
       <c r="J2">
-        <v>4280.827903333334</v>
+        <v>102.29485</v>
       </c>
       <c r="K2">
-        <v>6491.428146666666</v>
+        <v>113.24899</v>
       </c>
       <c r="L2">
-        <v>11985.06718</v>
+        <v>4680.075023333334</v>
       </c>
       <c r="M2">
-        <v>18041.65933</v>
+        <v>3604.433183333333</v>
       </c>
       <c r="N2">
+        <v>12221.5875</v>
+      </c>
+      <c r="O2">
+        <v>11771.46911</v>
+      </c>
+      <c r="P2">
         <v>20515.28316333333</v>
       </c>
-      <c r="O2">
+      <c r="Q2">
         <v>20102.13738666667</v>
       </c>
-      <c r="P2">
-        <v>26449.27023</v>
-      </c>
-      <c r="Q2">
-        <v>22493.71921</v>
-      </c>
       <c r="R2">
-        <v>17384.64073</v>
+        <v>24659.36187</v>
       </c>
       <c r="S2">
-        <v>7.201156666666667</v>
+        <v>21672.70910666667</v>
       </c>
     </row>
     <row r="3" spans="1:19">
@@ -777,58 +780,58 @@
         <v>710.104</v>
       </c>
       <c r="B3">
-        <v>12552.49591333333</v>
+        <v>36795.61794333334</v>
       </c>
       <c r="C3">
-        <v>-27.32914666666666</v>
+        <v>26599.52937</v>
       </c>
       <c r="D3">
+        <v>34.514585</v>
+      </c>
+      <c r="E3">
+        <v>27.98452333333333</v>
+      </c>
+      <c r="F3">
+        <v>33.36978</v>
+      </c>
+      <c r="G3">
         <v>23.70994666666667</v>
       </c>
-      <c r="E3">
-        <v>12095.73364333333</v>
-      </c>
-      <c r="F3">
-        <v>0.6442500000000001</v>
-      </c>
-      <c r="G3">
-        <v>123.8023133333333</v>
-      </c>
       <c r="H3">
-        <v>242.73299</v>
+        <v>8.07855</v>
       </c>
       <c r="I3">
-        <v>14170.36128666667</v>
+        <v>14.489295</v>
       </c>
       <c r="J3">
-        <v>5503.121763333334</v>
+        <v>200.01529</v>
       </c>
       <c r="K3">
-        <v>7479.256183333334</v>
+        <v>226.4408066666666</v>
       </c>
       <c r="L3">
-        <v>12234.60357666667</v>
+        <v>5869.553856666666</v>
       </c>
       <c r="M3">
-        <v>16713.60751333333</v>
+        <v>4908.467036666667</v>
       </c>
       <c r="N3">
+        <v>12434.50541</v>
+      </c>
+      <c r="O3">
+        <v>11854.02763666667</v>
+      </c>
+      <c r="P3">
         <v>19356.84124333333</v>
       </c>
-      <c r="O3">
+      <c r="Q3">
         <v>19671.82022</v>
       </c>
-      <c r="P3">
-        <v>24196.13092666666</v>
-      </c>
-      <c r="Q3">
-        <v>21074.1171</v>
-      </c>
       <c r="R3">
-        <v>15849.14506333333</v>
+        <v>22936.02401333333</v>
       </c>
       <c r="S3">
-        <v>33.19843</v>
+        <v>20403.25568666667</v>
       </c>
     </row>
     <row r="4" spans="1:19">
@@ -836,58 +839,58 @@
         <v>800.131</v>
       </c>
       <c r="B4">
-        <v>6932.285936666666</v>
+        <v>20554.8369</v>
       </c>
       <c r="C4">
-        <v>-8.370313333333334</v>
+        <v>14848.4749</v>
       </c>
       <c r="D4">
-        <v>26.52627666666666</v>
+        <v>14.92804</v>
       </c>
       <c r="E4">
-        <v>6795.605430000001</v>
+        <v>5.619759999999999</v>
       </c>
       <c r="F4">
-        <v>53.33856</v>
+        <v>8.25407</v>
       </c>
       <c r="G4">
-        <v>80.91987</v>
+        <v>56.734655</v>
       </c>
       <c r="H4">
-        <v>141.4823333333333</v>
+        <v>43.38448333333333</v>
       </c>
       <c r="I4">
-        <v>7957.620139999999</v>
+        <v>36.29832333333334</v>
       </c>
       <c r="J4">
-        <v>3077.371226666667</v>
+        <v>115.6491033333333</v>
       </c>
       <c r="K4">
-        <v>4145.92234</v>
+        <v>134.3358933333333</v>
       </c>
       <c r="L4">
-        <v>7273.76042</v>
+        <v>3299.528983333334</v>
       </c>
       <c r="M4">
-        <v>9614.88789</v>
+        <v>2581.32409</v>
       </c>
       <c r="N4">
+        <v>7316.216723333334</v>
+      </c>
+      <c r="O4">
+        <v>6990.159266666667</v>
+      </c>
+      <c r="P4">
         <v>11214.71510666666</v>
       </c>
-      <c r="O4">
+      <c r="Q4">
         <v>11253.09757333333</v>
       </c>
-      <c r="P4">
-        <v>13577.53117333333</v>
-      </c>
-      <c r="Q4">
-        <v>12441.78536333333</v>
-      </c>
       <c r="R4">
-        <v>9035.658949999999</v>
+        <v>13030.57828333333</v>
       </c>
       <c r="S4">
-        <v>-19.49027333333333</v>
+        <v>12165.85010333333</v>
       </c>
     </row>
     <row r="5" spans="1:19">
@@ -895,58 +898,58 @@
         <v>905.029</v>
       </c>
       <c r="B5">
-        <v>3095.688013333334</v>
+        <v>9177.530586666668</v>
       </c>
       <c r="C5">
-        <v>-4.855340000000001</v>
+        <v>5975.128903333333</v>
       </c>
       <c r="D5">
-        <v>-21.94467333333334</v>
+        <v>41.33446333333333</v>
       </c>
       <c r="E5">
-        <v>3074.815486666667</v>
+        <v>45.843405</v>
       </c>
       <c r="F5">
-        <v>12.58806333333333</v>
+        <v>18.17754</v>
       </c>
       <c r="G5">
-        <v>40.86438666666667</v>
+        <v>10.18604</v>
       </c>
       <c r="H5">
-        <v>76.11745333333333</v>
+        <v>10.36183</v>
       </c>
       <c r="I5">
-        <v>3223.61855</v>
+        <v>35.56543</v>
       </c>
       <c r="J5">
-        <v>541.7520733333333</v>
+        <v>65.75201</v>
       </c>
       <c r="K5">
-        <v>998.6890166666666</v>
+        <v>61.565015</v>
       </c>
       <c r="L5">
-        <v>1984.38306</v>
+        <v>579.0114566666667</v>
       </c>
       <c r="M5">
-        <v>3203.457866666667</v>
+        <v>471.6415233333334</v>
       </c>
       <c r="N5">
+        <v>2070.12945</v>
+      </c>
+      <c r="O5">
+        <v>1819.580843333333</v>
+      </c>
+      <c r="P5">
         <v>3664.984486666667</v>
       </c>
-      <c r="O5">
+      <c r="Q5">
         <v>3816.84904</v>
       </c>
-      <c r="P5">
-        <v>4980.962733333333</v>
-      </c>
-      <c r="Q5">
-        <v>4137.550749999999</v>
-      </c>
       <c r="R5">
-        <v>3347.038946666667</v>
+        <v>4457.43869</v>
       </c>
       <c r="S5">
-        <v>27.57530666666667</v>
+        <v>4007.866093333334</v>
       </c>
     </row>
     <row r="6" spans="1:19">
@@ -954,58 +957,58 @@
         <v>940.061</v>
       </c>
       <c r="B6">
-        <v>332.25372</v>
+        <v>1032.1978</v>
       </c>
       <c r="C6">
-        <v>-19.60666666666667</v>
+        <v>473.6399866666666</v>
       </c>
       <c r="D6">
-        <v>-12.81786666666667</v>
+        <v>34.95126</v>
       </c>
       <c r="E6">
-        <v>353.1356033333333</v>
+        <v>50.58386</v>
       </c>
       <c r="F6">
-        <v>-9.891603333333334</v>
+        <v>16.50851</v>
       </c>
       <c r="G6">
-        <v>-17.43703</v>
+        <v>16.33288</v>
       </c>
       <c r="H6">
-        <v>78.22518666666666</v>
+        <v>10.36155</v>
       </c>
       <c r="I6">
-        <v>402.96002</v>
+        <v>17.38667</v>
       </c>
       <c r="J6">
-        <v>31.79190666666666</v>
+        <v>37.146265</v>
       </c>
       <c r="K6">
-        <v>75.53742666666666</v>
+        <v>95.67583333333333</v>
       </c>
       <c r="L6">
-        <v>123.7908633333333</v>
+        <v>43.67735666666667</v>
       </c>
       <c r="M6">
-        <v>206.3967533333333</v>
+        <v>64.46751</v>
       </c>
       <c r="N6">
+        <v>121.4478733333333</v>
+      </c>
+      <c r="O6">
+        <v>102.8225566666667</v>
+      </c>
+      <c r="P6">
         <v>227.02584</v>
       </c>
-      <c r="O6">
+      <c r="Q6">
         <v>223.2759233333333</v>
       </c>
-      <c r="P6">
-        <v>381.7327366666667</v>
-      </c>
-      <c r="Q6">
-        <v>295.8948766666667</v>
-      </c>
       <c r="R6">
-        <v>277.1073966666667</v>
+        <v>333.41682</v>
       </c>
       <c r="S6">
-        <v>-7.549576666666666</v>
+        <v>275.8496933333333</v>
       </c>
     </row>
     <row r="7" spans="1:19">
@@ -1013,58 +1016,58 @@
         <v>1000.111</v>
       </c>
       <c r="B7">
-        <v>17.6243</v>
+        <v>68.44456666666666</v>
       </c>
       <c r="C7">
+        <v>42.50425</v>
+      </c>
+      <c r="D7">
+        <v>57.08346</v>
+      </c>
+      <c r="E7">
+        <v>44.26014</v>
+      </c>
+      <c r="F7">
         <v>30.97146333333333</v>
       </c>
-      <c r="D7">
-        <v>-9.300673333333334</v>
-      </c>
-      <c r="E7">
-        <v>23.65732333333333</v>
-      </c>
-      <c r="F7">
-        <v>-9.188706666666667</v>
-      </c>
       <c r="G7">
-        <v>50.70141333333333</v>
+        <v>52.86748</v>
       </c>
       <c r="H7">
-        <v>-2.57548</v>
+        <v>27.57355</v>
       </c>
       <c r="I7">
-        <v>22.89632666666666</v>
+        <v>29.94484</v>
       </c>
       <c r="J7">
-        <v>-15.27766</v>
+        <v>57.610755</v>
       </c>
       <c r="K7">
-        <v>0.3514033333333335</v>
+        <v>8.605320000000001</v>
       </c>
       <c r="L7">
-        <v>47.19506666666667</v>
+        <v>24.93896</v>
       </c>
       <c r="M7">
-        <v>30.61949333333333</v>
+        <v>9.48343</v>
       </c>
       <c r="N7">
+        <v>13.611025</v>
+      </c>
+      <c r="O7">
+        <v>51.52733666666666</v>
+      </c>
+      <c r="P7">
         <v>59.72284</v>
       </c>
-      <c r="O7">
+      <c r="Q7">
         <v>66.51241</v>
       </c>
-      <c r="P7">
-        <v>61.77090333333333</v>
-      </c>
-      <c r="Q7">
-        <v>23.12794</v>
-      </c>
       <c r="R7">
-        <v>0.7653099999999995</v>
+        <v>82.38233</v>
       </c>
       <c r="S7">
-        <v>-13.16375333333333</v>
+        <v>31.20573333333333</v>
       </c>
     </row>
   </sheetData>
@@ -1255,163 +1258,142 @@
         <v>41905.55299</v>
       </c>
       <c r="C2">
-        <v>-33.01256</v>
+        <v>41946.92794</v>
       </c>
       <c r="D2">
+        <v>41806.37714</v>
+      </c>
+      <c r="E2">
+        <v>30393.86229</v>
+      </c>
+      <c r="F2">
+        <v>29988.32273</v>
+      </c>
+      <c r="G2">
+        <v>29987.64205</v>
+      </c>
+      <c r="H2">
+        <v>10.7128</v>
+      </c>
+      <c r="I2">
+        <v>30.91075</v>
+      </c>
+      <c r="K2">
+        <v>1.05369</v>
+      </c>
+      <c r="M2">
         <v>35.82884</v>
       </c>
-      <c r="E2">
-        <v>-19.141</v>
-      </c>
-      <c r="F2">
+      <c r="O2">
         <v>34.42366</v>
       </c>
-      <c r="G2">
+      <c r="P2">
         <v>41.80097</v>
       </c>
-      <c r="H2">
+      <c r="Q2">
         <v>50.4082</v>
       </c>
-      <c r="I2">
-        <v>-1.93175</v>
-      </c>
-      <c r="J2">
-        <v>-42.66935</v>
-      </c>
-      <c r="K2">
+      <c r="T2">
         <v>12.82031</v>
       </c>
-      <c r="L2">
-        <v>-33.89048</v>
-      </c>
-      <c r="M2">
-        <v>41946.92794</v>
-      </c>
-      <c r="N2">
-        <v>-36.3486</v>
-      </c>
-      <c r="O2">
+      <c r="W2">
         <v>49.00291</v>
       </c>
-      <c r="P2">
+      <c r="X2">
         <v>35.65319</v>
       </c>
-      <c r="Q2">
+      <c r="Y2">
         <v>20.02115</v>
       </c>
-      <c r="R2">
+      <c r="Z2">
         <v>129.2961</v>
       </c>
-      <c r="S2">
+      <c r="AA2">
         <v>80.80005</v>
       </c>
-      <c r="T2">
+      <c r="AB2">
         <v>96.7884</v>
       </c>
-      <c r="U2">
+      <c r="AC2">
         <v>147.7487</v>
       </c>
-      <c r="V2">
+      <c r="AD2">
         <v>72.36716</v>
       </c>
-      <c r="W2">
+      <c r="AE2">
         <v>119.63111</v>
       </c>
-      <c r="X2">
-        <v>41806.37714</v>
-      </c>
-      <c r="Y2">
+      <c r="AF2">
         <v>4829.60906</v>
       </c>
-      <c r="Z2">
+      <c r="AG2">
         <v>4667.25919</v>
       </c>
-      <c r="AA2">
+      <c r="AH2">
         <v>4543.35682</v>
       </c>
-      <c r="AB2">
+      <c r="AI2">
         <v>3631.8677</v>
       </c>
-      <c r="AC2">
+      <c r="AJ2">
         <v>3458.41838</v>
       </c>
-      <c r="AD2">
+      <c r="AK2">
         <v>3723.01347</v>
       </c>
-      <c r="AE2">
+      <c r="AL2">
         <v>12292.85259</v>
       </c>
-      <c r="AF2">
+      <c r="AM2">
         <v>12218.66083</v>
       </c>
-      <c r="AG2">
+      <c r="AN2">
         <v>12153.24908</v>
       </c>
-      <c r="AH2">
+      <c r="AO2">
         <v>11583.29163</v>
       </c>
-      <c r="AI2">
-        <v>30393.86229</v>
-      </c>
-      <c r="AJ2">
+      <c r="AP2">
         <v>11930.24861</v>
       </c>
-      <c r="AK2">
+      <c r="AQ2">
         <v>11800.86709</v>
       </c>
-      <c r="AL2">
+      <c r="AR2">
         <v>20460.76736</v>
       </c>
-      <c r="AM2">
+      <c r="AS2">
         <v>20339.58929</v>
       </c>
-      <c r="AN2">
+      <c r="AT2">
         <v>20745.49284</v>
       </c>
-      <c r="AO2">
+      <c r="AU2">
         <v>19917.27543</v>
       </c>
-      <c r="AP2">
+      <c r="AV2">
         <v>20233.65534</v>
       </c>
-      <c r="AQ2">
+      <c r="AW2">
         <v>20155.48139</v>
       </c>
-      <c r="AR2">
+      <c r="AX2">
         <v>24687.38741</v>
       </c>
-      <c r="AS2">
+      <c r="AY2">
         <v>24672.10055</v>
       </c>
-      <c r="AT2">
-        <v>29988.32273</v>
-      </c>
-      <c r="AU2">
+      <c r="AZ2">
         <v>24618.59765</v>
       </c>
-      <c r="AV2">
+      <c r="BA2">
         <v>21113.79306</v>
       </c>
-      <c r="AW2">
+      <c r="BB2">
         <v>21748.76692</v>
       </c>
-      <c r="AX2">
+      <c r="BC2">
         <v>22155.56734</v>
-      </c>
-      <c r="AY2">
-        <v>29987.64205</v>
-      </c>
-      <c r="AZ2">
-        <v>10.7128</v>
-      </c>
-      <c r="BA2">
-        <v>30.91075</v>
-      </c>
-      <c r="BB2">
-        <v>-10.36097</v>
-      </c>
-      <c r="BC2">
-        <v>1.05369</v>
       </c>
     </row>
     <row r="3" spans="1:55">
@@ -1422,163 +1404,148 @@
         <v>37627.27997</v>
       </c>
       <c r="C3">
+        <v>36323.02239</v>
+      </c>
+      <c r="D3">
+        <v>36436.55147</v>
+      </c>
+      <c r="E3">
+        <v>26458.42355</v>
+      </c>
+      <c r="F3">
+        <v>26722.44636</v>
+      </c>
+      <c r="G3">
+        <v>26617.7182</v>
+      </c>
+      <c r="H3">
+        <v>0.17561</v>
+      </c>
+      <c r="I3">
+        <v>68.85356</v>
+      </c>
+      <c r="K3">
+        <v>53.7458</v>
+      </c>
+      <c r="L3">
         <v>2.80986</v>
       </c>
-      <c r="D3">
+      <c r="M3">
         <v>27.39791</v>
       </c>
-      <c r="E3">
-        <v>-33.89048</v>
-      </c>
-      <c r="F3">
-        <v>-81.46674</v>
-      </c>
-      <c r="G3">
+      <c r="P3">
         <v>33.36978</v>
       </c>
-      <c r="H3">
+      <c r="Q3">
         <v>41.97663</v>
       </c>
-      <c r="I3">
+      <c r="R3">
         <v>17.0354</v>
       </c>
-      <c r="J3">
+      <c r="S3">
         <v>12.11781</v>
       </c>
-      <c r="K3">
-        <v>-37.75323</v>
-      </c>
-      <c r="L3">
+      <c r="U3">
         <v>1.93177</v>
       </c>
-      <c r="M3">
-        <v>36323.02239</v>
-      </c>
-      <c r="N3">
+      <c r="V3">
         <v>14.22533</v>
       </c>
-      <c r="O3">
+      <c r="W3">
         <v>0.52684</v>
       </c>
-      <c r="P3">
-        <v>-12.81942</v>
-      </c>
-      <c r="Q3">
+      <c r="Y3">
         <v>28.45175</v>
       </c>
-      <c r="R3">
+      <c r="Z3">
         <v>144.05805</v>
       </c>
-      <c r="S3">
+      <c r="AA3">
         <v>198.89714</v>
       </c>
-      <c r="T3">
+      <c r="AB3">
         <v>257.09068</v>
       </c>
-      <c r="U3">
+      <c r="AC3">
         <v>204.69824</v>
       </c>
-      <c r="V3">
+      <c r="AD3">
         <v>266.41005</v>
       </c>
-      <c r="W3">
+      <c r="AE3">
         <v>208.21413</v>
       </c>
-      <c r="X3">
-        <v>36436.55147</v>
-      </c>
-      <c r="Y3">
+      <c r="AF3">
         <v>5866.31826</v>
       </c>
-      <c r="Z3">
+      <c r="AG3">
         <v>5865.10487</v>
       </c>
-      <c r="AA3">
+      <c r="AH3">
         <v>5877.23844</v>
       </c>
-      <c r="AB3">
+      <c r="AI3">
         <v>4767.02198</v>
       </c>
-      <c r="AC3">
+      <c r="AJ3">
         <v>5023.34223</v>
       </c>
-      <c r="AD3">
+      <c r="AK3">
         <v>4935.0369</v>
       </c>
-      <c r="AE3">
+      <c r="AL3">
         <v>12479.38942</v>
       </c>
-      <c r="AF3">
+      <c r="AM3">
         <v>12429.55047</v>
       </c>
-      <c r="AG3">
+      <c r="AN3">
         <v>12394.57634</v>
       </c>
-      <c r="AH3">
+      <c r="AO3">
         <v>11879.68392</v>
       </c>
-      <c r="AI3">
-        <v>26458.42355</v>
-      </c>
-      <c r="AJ3">
+      <c r="AP3">
         <v>11753.67232</v>
       </c>
-      <c r="AK3">
+      <c r="AQ3">
         <v>11928.72667</v>
       </c>
-      <c r="AL3">
+      <c r="AR3">
         <v>19285.49722</v>
       </c>
-      <c r="AM3">
+      <c r="AS3">
         <v>19428.18697</v>
       </c>
-      <c r="AN3">
+      <c r="AT3">
         <v>19356.83954</v>
       </c>
-      <c r="AO3">
+      <c r="AU3">
         <v>19801.57694</v>
       </c>
-      <c r="AP3">
+      <c r="AV3">
         <v>19831.6843</v>
       </c>
-      <c r="AQ3">
+      <c r="AW3">
         <v>19382.19942</v>
       </c>
-      <c r="AR3">
+      <c r="AX3">
         <v>22788.94463</v>
       </c>
-      <c r="AS3">
+      <c r="AY3">
         <v>23077.00179</v>
       </c>
-      <c r="AT3">
-        <v>26722.44636</v>
-      </c>
-      <c r="AU3">
+      <c r="AZ3">
         <v>22942.12562</v>
       </c>
-      <c r="AV3">
+      <c r="BA3">
         <v>19903.23526</v>
       </c>
-      <c r="AW3">
+      <c r="BB3">
         <v>20376.99042</v>
       </c>
-      <c r="AX3">
+      <c r="BC3">
         <v>20929.54138</v>
-      </c>
-      <c r="AY3">
-        <v>26617.7182</v>
-      </c>
-      <c r="AZ3">
-        <v>0.17561</v>
-      </c>
-      <c r="BA3">
-        <v>68.85356</v>
-      </c>
-      <c r="BB3">
-        <v>-23.00407</v>
-      </c>
-      <c r="BC3">
-        <v>53.7458</v>
       </c>
     </row>
     <row r="4" spans="1:55">
@@ -1589,163 +1556,148 @@
         <v>20785.61829</v>
       </c>
       <c r="C4">
+        <v>20344.66628</v>
+      </c>
+      <c r="D4">
+        <v>20534.22613</v>
+      </c>
+      <c r="E4">
+        <v>14993.14162</v>
+      </c>
+      <c r="F4">
+        <v>14817.95728</v>
+      </c>
+      <c r="G4">
+        <v>14734.3258</v>
+      </c>
+      <c r="H4">
+        <v>23.35822</v>
+      </c>
+      <c r="J4">
+        <v>6.49786</v>
+      </c>
+      <c r="L4">
         <v>4.91728</v>
       </c>
-      <c r="D4">
+      <c r="M4">
         <v>6.32224</v>
       </c>
-      <c r="E4">
+      <c r="N4">
         <v>8.25407</v>
       </c>
-      <c r="F4">
-        <v>-9.834160000000001</v>
-      </c>
-      <c r="G4">
-        <v>-23.53085</v>
-      </c>
-      <c r="H4">
-        <v>-33.89048</v>
-      </c>
-      <c r="I4">
+      <c r="R4">
         <v>25.46587</v>
       </c>
-      <c r="J4">
+      <c r="S4">
         <v>88.00344</v>
       </c>
-      <c r="K4">
+      <c r="T4">
         <v>25.46587</v>
       </c>
-      <c r="L4">
+      <c r="U4">
         <v>16.68414</v>
       </c>
-      <c r="M4">
-        <v>20344.66628</v>
-      </c>
-      <c r="N4">
+      <c r="V4">
         <v>88.00344</v>
       </c>
-      <c r="O4">
+      <c r="W4">
         <v>11.06405</v>
       </c>
-      <c r="P4">
+      <c r="X4">
         <v>60.94819</v>
       </c>
-      <c r="Q4">
+      <c r="Y4">
         <v>36.88273</v>
       </c>
-      <c r="R4">
+      <c r="Z4">
         <v>114.5352</v>
       </c>
-      <c r="S4">
+      <c r="AA4">
         <v>91.34168</v>
       </c>
-      <c r="T4">
+      <c r="AB4">
         <v>141.07043</v>
       </c>
-      <c r="U4">
+      <c r="AC4">
         <v>107.68229</v>
       </c>
-      <c r="V4">
+      <c r="AD4">
         <v>175.69428</v>
       </c>
-      <c r="W4">
+      <c r="AE4">
         <v>119.63111</v>
       </c>
-      <c r="X4">
-        <v>20534.22613</v>
-      </c>
-      <c r="Y4">
+      <c r="AF4">
         <v>3219.00318</v>
       </c>
-      <c r="Z4">
+      <c r="AG4">
         <v>3339.96741</v>
       </c>
-      <c r="AA4">
+      <c r="AH4">
         <v>3339.61636</v>
       </c>
-      <c r="AB4">
+      <c r="AI4">
         <v>2552.52991</v>
       </c>
-      <c r="AC4">
+      <c r="AJ4">
         <v>2680.44637</v>
       </c>
-      <c r="AD4">
+      <c r="AK4">
         <v>2510.99599</v>
       </c>
-      <c r="AE4">
+      <c r="AL4">
         <v>7246.32466</v>
       </c>
-      <c r="AF4">
+      <c r="AM4">
         <v>7399.91635</v>
       </c>
-      <c r="AG4">
+      <c r="AN4">
         <v>7302.40916</v>
       </c>
-      <c r="AH4">
+      <c r="AO4">
         <v>7118.95575</v>
       </c>
-      <c r="AI4">
-        <v>14993.14162</v>
-      </c>
-      <c r="AJ4">
+      <c r="AP4">
         <v>6930.67306</v>
       </c>
-      <c r="AK4">
+      <c r="AQ4">
         <v>6920.84899</v>
       </c>
-      <c r="AL4">
+      <c r="AR4">
         <v>11267.90452</v>
       </c>
-      <c r="AM4">
+      <c r="AS4">
         <v>11278.74303</v>
       </c>
-      <c r="AN4">
+      <c r="AT4">
         <v>11097.49777</v>
       </c>
-      <c r="AO4">
+      <c r="AU4">
         <v>11091.73719</v>
       </c>
-      <c r="AP4">
+      <c r="AV4">
         <v>11343.42938</v>
       </c>
-      <c r="AQ4">
+      <c r="AW4">
         <v>11324.12615</v>
       </c>
-      <c r="AR4">
+      <c r="AX4">
         <v>12972.00585</v>
       </c>
-      <c r="AS4">
+      <c r="AY4">
         <v>12942.63039</v>
       </c>
-      <c r="AT4">
-        <v>14817.95728</v>
-      </c>
-      <c r="AU4">
+      <c r="AZ4">
         <v>13177.09861</v>
       </c>
-      <c r="AV4">
+      <c r="BA4">
         <v>11985.54266</v>
       </c>
-      <c r="AW4">
+      <c r="BB4">
         <v>12162.71482</v>
       </c>
-      <c r="AX4">
+      <c r="BC4">
         <v>12349.29283</v>
-      </c>
-      <c r="AY4">
-        <v>14734.3258</v>
-      </c>
-      <c r="AZ4">
-        <v>23.35822</v>
-      </c>
-      <c r="BA4">
-        <v>-55.48573</v>
-      </c>
-      <c r="BB4">
-        <v>6.49786</v>
-      </c>
-      <c r="BC4">
-        <v>-9.482950000000001</v>
       </c>
     </row>
     <row r="5" spans="1:55">
@@ -1756,163 +1708,145 @@
         <v>9223.12463</v>
       </c>
       <c r="C5">
-        <v>-11.94141</v>
+        <v>9243.41185</v>
       </c>
       <c r="D5">
+        <v>9066.05528</v>
+      </c>
+      <c r="E5">
+        <v>5981.72723</v>
+      </c>
+      <c r="F5">
+        <v>6063.64777</v>
+      </c>
+      <c r="G5">
+        <v>5880.01171</v>
+      </c>
+      <c r="H5">
+        <v>57.08346</v>
+      </c>
+      <c r="I5">
+        <v>3.51233</v>
+      </c>
+      <c r="J5">
+        <v>63.4076</v>
+      </c>
+      <c r="K5">
+        <v>15.80599</v>
+      </c>
+      <c r="M5">
         <v>75.88082</v>
       </c>
-      <c r="E5">
+      <c r="N5">
         <v>4.03918</v>
       </c>
-      <c r="F5">
+      <c r="O5">
         <v>32.3159</v>
       </c>
-      <c r="G5">
-        <v>-50.9211</v>
-      </c>
-      <c r="H5">
+      <c r="Q5">
         <v>16.68414</v>
       </c>
-      <c r="I5">
-        <v>-86.20610000000001</v>
-      </c>
-      <c r="J5">
+      <c r="S5">
         <v>3.68794</v>
       </c>
-      <c r="K5">
+      <c r="T5">
         <v>0.17561</v>
       </c>
-      <c r="L5">
-        <v>-19.141</v>
-      </c>
-      <c r="M5">
-        <v>9243.41185</v>
-      </c>
-      <c r="N5">
+      <c r="V5">
         <v>20.54805</v>
       </c>
-      <c r="O5">
+      <c r="W5">
         <v>40.5714</v>
       </c>
-      <c r="P5">
-        <v>-23.35526</v>
-      </c>
-      <c r="Q5">
+      <c r="Y5">
         <v>30.55946</v>
       </c>
-      <c r="R5">
+      <c r="Z5">
         <v>53.39447</v>
       </c>
-      <c r="S5">
+      <c r="AA5">
         <v>38.63923</v>
       </c>
-      <c r="T5">
+      <c r="AB5">
         <v>105.22233</v>
       </c>
-      <c r="U5">
+      <c r="AC5">
         <v>33.89672</v>
       </c>
-      <c r="V5">
+      <c r="AD5">
         <v>89.23331</v>
       </c>
-      <c r="W5">
-        <v>-13.17063</v>
-      </c>
-      <c r="X5">
-        <v>9066.05528</v>
-      </c>
-      <c r="Y5">
+      <c r="AF5">
         <v>617.971</v>
       </c>
-      <c r="Z5">
+      <c r="AG5">
         <v>492.11332</v>
       </c>
-      <c r="AA5">
+      <c r="AH5">
         <v>626.95005</v>
       </c>
-      <c r="AB5">
+      <c r="AI5">
         <v>506.19285</v>
       </c>
-      <c r="AC5">
+      <c r="AJ5">
         <v>452.5182</v>
       </c>
-      <c r="AD5">
+      <c r="AK5">
         <v>456.21352</v>
       </c>
-      <c r="AE5">
+      <c r="AL5">
         <v>2087.33533</v>
       </c>
-      <c r="AF5">
+      <c r="AM5">
         <v>2024.79597</v>
       </c>
-      <c r="AG5">
+      <c r="AN5">
         <v>2098.25705</v>
       </c>
-      <c r="AH5">
+      <c r="AO5">
         <v>1830.09616</v>
       </c>
-      <c r="AI5">
-        <v>5981.72723</v>
-      </c>
-      <c r="AJ5">
+      <c r="AP5">
         <v>1863.75345</v>
       </c>
-      <c r="AK5">
+      <c r="AQ5">
         <v>1764.89292</v>
       </c>
-      <c r="AL5">
+      <c r="AR5">
         <v>3549.63081</v>
       </c>
-      <c r="AM5">
+      <c r="AS5">
         <v>3750.17494</v>
       </c>
-      <c r="AN5">
+      <c r="AT5">
         <v>3695.14771</v>
       </c>
-      <c r="AO5">
+      <c r="AU5">
         <v>3935.13612</v>
       </c>
-      <c r="AP5">
+      <c r="AV5">
         <v>3800.28372</v>
       </c>
-      <c r="AQ5">
+      <c r="AW5">
         <v>3715.12728</v>
       </c>
-      <c r="AR5">
+      <c r="AX5">
         <v>4523.97912</v>
       </c>
-      <c r="AS5">
+      <c r="AY5">
         <v>4355.26131</v>
       </c>
-      <c r="AT5">
-        <v>6063.64777</v>
-      </c>
-      <c r="AU5">
+      <c r="AZ5">
         <v>4493.07564</v>
       </c>
-      <c r="AV5">
+      <c r="BA5">
         <v>3840.74805</v>
       </c>
-      <c r="AW5">
+      <c r="BB5">
         <v>4078.82856</v>
       </c>
-      <c r="AX5">
+      <c r="BC5">
         <v>4104.02167</v>
-      </c>
-      <c r="AY5">
-        <v>5880.01171</v>
-      </c>
-      <c r="AZ5">
-        <v>57.08346</v>
-      </c>
-      <c r="BA5">
-        <v>3.51233</v>
-      </c>
-      <c r="BB5">
-        <v>63.4076</v>
-      </c>
-      <c r="BC5">
-        <v>15.80599</v>
       </c>
     </row>
     <row r="6" spans="1:55">
@@ -1923,163 +1857,124 @@
         <v>970.7617</v>
       </c>
       <c r="C6">
-        <v>-24.5844</v>
+        <v>1063.6207</v>
       </c>
       <c r="D6">
+        <v>1062.211</v>
+      </c>
+      <c r="E6">
+        <v>435.274</v>
+      </c>
+      <c r="F6">
+        <v>434.04231</v>
+      </c>
+      <c r="G6">
+        <v>551.60365</v>
+      </c>
+      <c r="H6">
+        <v>50.75953</v>
+      </c>
+      <c r="J6">
+        <v>19.14299</v>
+      </c>
+      <c r="M6">
         <v>50.58386</v>
       </c>
-      <c r="E6">
-        <v>-17.03383</v>
-      </c>
-      <c r="F6">
-        <v>-58.29468</v>
-      </c>
-      <c r="G6">
+      <c r="P6">
         <v>16.50851</v>
       </c>
-      <c r="H6">
-        <v>-12.81942</v>
-      </c>
-      <c r="I6">
-        <v>-41.96706</v>
-      </c>
-      <c r="J6">
+      <c r="S6">
         <v>16.33288</v>
       </c>
-      <c r="K6">
-        <v>-14.57544</v>
-      </c>
-      <c r="L6">
+      <c r="U6">
         <v>10.36155</v>
       </c>
-      <c r="M6">
-        <v>1063.6207</v>
-      </c>
-      <c r="N6">
-        <v>-17.38502</v>
-      </c>
-      <c r="O6">
+      <c r="W6">
         <v>17.38667</v>
       </c>
-      <c r="P6">
-        <v>-29.67646</v>
-      </c>
-      <c r="Q6">
-        <v>-83.22208000000001</v>
-      </c>
-      <c r="R6">
-        <v>-1.40491</v>
-      </c>
-      <c r="S6">
+      <c r="AA6">
         <v>32.3159</v>
       </c>
-      <c r="T6">
+      <c r="AB6">
         <v>41.97663</v>
       </c>
-      <c r="U6">
+      <c r="AC6">
         <v>107.68229</v>
       </c>
-      <c r="V6">
+      <c r="AD6">
         <v>85.01664</v>
       </c>
-      <c r="W6">
+      <c r="AE6">
         <v>94.32857</v>
       </c>
-      <c r="X6">
-        <v>1062.211</v>
-      </c>
-      <c r="Y6">
+      <c r="AF6">
         <v>52.34049</v>
       </c>
-      <c r="Z6">
+      <c r="AG6">
         <v>0.52684</v>
       </c>
-      <c r="AA6">
+      <c r="AH6">
         <v>78.16473999999999</v>
       </c>
-      <c r="AB6">
+      <c r="AI6">
         <v>16.68414</v>
       </c>
-      <c r="AC6">
-        <v>-3.16104</v>
-      </c>
-      <c r="AD6">
+      <c r="AK6">
         <v>112.25088</v>
       </c>
-      <c r="AE6">
+      <c r="AL6">
         <v>117.52244</v>
       </c>
-      <c r="AF6">
+      <c r="AM6">
         <v>99.42397</v>
       </c>
-      <c r="AG6">
+      <c r="AN6">
         <v>147.39721</v>
       </c>
-      <c r="AH6">
+      <c r="AO6">
         <v>124.55141</v>
       </c>
-      <c r="AI6">
-        <v>435.274</v>
-      </c>
-      <c r="AJ6">
+      <c r="AP6">
         <v>67.44814</v>
       </c>
-      <c r="AK6">
+      <c r="AQ6">
         <v>116.46812</v>
       </c>
-      <c r="AL6">
+      <c r="AR6">
         <v>216.8283</v>
       </c>
-      <c r="AM6">
+      <c r="AS6">
         <v>211.20268</v>
       </c>
-      <c r="AN6">
+      <c r="AT6">
         <v>253.04654</v>
       </c>
-      <c r="AO6">
+      <c r="AU6">
         <v>251.28824</v>
       </c>
-      <c r="AP6">
+      <c r="AV6">
         <v>189.75633</v>
       </c>
-      <c r="AQ6">
+      <c r="AW6">
         <v>228.7832</v>
       </c>
-      <c r="AR6">
+      <c r="AX6">
         <v>341.32972</v>
       </c>
-      <c r="AS6">
+      <c r="AY6">
         <v>369.82618</v>
       </c>
-      <c r="AT6">
-        <v>434.04231</v>
-      </c>
-      <c r="AU6">
+      <c r="AZ6">
         <v>289.09456</v>
       </c>
-      <c r="AV6">
+      <c r="BA6">
         <v>283.11549</v>
       </c>
-      <c r="AW6">
+      <c r="BB6">
         <v>315.47458</v>
       </c>
-      <c r="AX6">
+      <c r="BC6">
         <v>228.95901</v>
-      </c>
-      <c r="AY6">
-        <v>551.60365</v>
-      </c>
-      <c r="AZ6">
-        <v>50.75953</v>
-      </c>
-      <c r="BA6">
-        <v>-40.73804</v>
-      </c>
-      <c r="BB6">
-        <v>19.14299</v>
-      </c>
-      <c r="BC6">
-        <v>-1.05368</v>
       </c>
     </row>
     <row r="7" spans="1:55">
@@ -2090,163 +1985,109 @@
         <v>41.62532</v>
       </c>
       <c r="C7">
-        <v>-33.01256</v>
+        <v>81.50281</v>
       </c>
       <c r="D7">
+        <v>82.20556999999999</v>
+      </c>
+      <c r="E7">
+        <v>57.61047</v>
+      </c>
+      <c r="F7">
+        <v>20.54805</v>
+      </c>
+      <c r="G7">
+        <v>49.35423</v>
+      </c>
+      <c r="J7">
+        <v>57.08346</v>
+      </c>
+      <c r="M7">
         <v>44.26014</v>
       </c>
-      <c r="E7">
+      <c r="N7">
         <v>71.48875</v>
       </c>
-      <c r="F7">
+      <c r="O7">
         <v>13.34719</v>
       </c>
-      <c r="G7">
+      <c r="P7">
         <v>8.07845</v>
       </c>
-      <c r="H7">
-        <v>-12.81942</v>
-      </c>
-      <c r="I7">
+      <c r="R7">
         <v>52.86748</v>
       </c>
-      <c r="J7">
-        <v>-67.95008</v>
-      </c>
-      <c r="K7">
+      <c r="T7">
         <v>27.57355</v>
       </c>
-      <c r="L7">
-        <v>-38.10439</v>
-      </c>
-      <c r="M7">
-        <v>81.50281</v>
-      </c>
-      <c r="N7">
-        <v>-34.24164</v>
-      </c>
-      <c r="O7">
-        <v>-16.33143</v>
-      </c>
-      <c r="P7">
+      <c r="X7">
         <v>23.00695</v>
       </c>
-      <c r="Q7">
+      <c r="Y7">
         <v>36.88273</v>
       </c>
-      <c r="R7">
+      <c r="Z7">
         <v>68.15085000000001</v>
       </c>
-      <c r="S7">
+      <c r="AA7">
         <v>47.07066</v>
       </c>
-      <c r="T7">
-        <v>-10.71218</v>
-      </c>
-      <c r="U7">
+      <c r="AC7">
         <v>8.605320000000001</v>
       </c>
-      <c r="V7">
-        <v>-5.61958</v>
-      </c>
-      <c r="W7">
-        <v>-38.45555</v>
-      </c>
-      <c r="X7">
-        <v>82.20556999999999</v>
-      </c>
-      <c r="Y7">
+      <c r="AF7">
         <v>24.93896</v>
       </c>
-      <c r="Z7">
-        <v>-5.79519</v>
-      </c>
-      <c r="AA7">
-        <v>-14.57544</v>
-      </c>
-      <c r="AB7">
-        <v>-25.46235</v>
-      </c>
-      <c r="AC7">
+      <c r="AJ7">
         <v>9.48343</v>
       </c>
-      <c r="AD7">
-        <v>-10.00976</v>
-      </c>
-      <c r="AE7">
+      <c r="AL7">
         <v>1.58054</v>
       </c>
-      <c r="AF7">
+      <c r="AM7">
         <v>25.64151</v>
       </c>
-      <c r="AG7">
-        <v>-4.39031</v>
-      </c>
-      <c r="AH7">
+      <c r="AO7">
         <v>120.334</v>
       </c>
-      <c r="AI7">
-        <v>57.61047</v>
-      </c>
-      <c r="AJ7">
+      <c r="AP7">
         <v>0</v>
       </c>
-      <c r="AK7">
+      <c r="AQ7">
         <v>34.24801</v>
       </c>
-      <c r="AL7">
+      <c r="AR7">
         <v>5.97099</v>
       </c>
-      <c r="AM7">
+      <c r="AS7">
         <v>67.79949000000001</v>
       </c>
-      <c r="AN7">
+      <c r="AT7">
         <v>105.39804</v>
       </c>
-      <c r="AO7">
+      <c r="AU7">
         <v>97.31551</v>
       </c>
-      <c r="AP7">
+      <c r="AV7">
         <v>52.69182</v>
       </c>
-      <c r="AQ7">
+      <c r="AW7">
         <v>49.5299</v>
       </c>
-      <c r="AR7">
+      <c r="AX7">
         <v>102.93811</v>
       </c>
-      <c r="AS7">
+      <c r="AY7">
         <v>61.82655</v>
       </c>
-      <c r="AT7">
-        <v>20.54805</v>
-      </c>
-      <c r="AU7">
-        <v>-23.00407</v>
-      </c>
-      <c r="AV7">
+      <c r="BA7">
         <v>21.60186</v>
       </c>
-      <c r="AW7">
+      <c r="BB7">
         <v>70.78603</v>
       </c>
-      <c r="AX7">
+      <c r="BC7">
         <v>1.22931</v>
-      </c>
-      <c r="AY7">
-        <v>49.35423</v>
-      </c>
-      <c r="AZ7">
-        <v>-48.28761</v>
-      </c>
-      <c r="BA7">
-        <v>-57.59244</v>
-      </c>
-      <c r="BB7">
-        <v>57.08346</v>
-      </c>
-      <c r="BC7">
-        <v>-38.98228</v>
       </c>
     </row>
   </sheetData>
@@ -2326,55 +2167,52 @@
         <v>630.188</v>
       </c>
       <c r="B2">
-        <v>4.995299620221993</v>
+        <v>0.001724963836062461</v>
       </c>
       <c r="C2">
+        <v>0.007761891073783482</v>
+      </c>
+      <c r="D2">
+        <v>0.7492961175287587</v>
+      </c>
+      <c r="E2">
+        <v>2.493580149634246</v>
+      </c>
+      <c r="F2">
         <v>0.1373027607088225</v>
       </c>
-      <c r="E2">
-        <v>5.722706994833109</v>
-      </c>
-      <c r="F2">
-        <v>0.2248889903485518</v>
-      </c>
-      <c r="G2">
-        <v>0.9701352075957687</v>
-      </c>
-      <c r="H2">
-        <v>0.3589151342952568</v>
-      </c>
       <c r="I2">
-        <v>2.96174237543613</v>
+        <v>0.4537479264930682</v>
       </c>
       <c r="J2">
-        <v>0.1377055136405786</v>
+        <v>0.2371614956299856</v>
       </c>
       <c r="K2">
-        <v>0.7118726997008468</v>
+        <v>0.3666706687878193</v>
       </c>
       <c r="L2">
-        <v>0.02940408630086061</v>
+        <v>0.03062204961686835</v>
       </c>
       <c r="M2">
-        <v>0.543092063647444</v>
+        <v>0.03751444978560724</v>
       </c>
       <c r="N2">
+        <v>0.005714158463767701</v>
+      </c>
+      <c r="O2">
+        <v>0.01492339326305733</v>
+      </c>
+      <c r="P2">
         <v>0.01013837546677909</v>
       </c>
-      <c r="O2">
+      <c r="Q2">
         <v>0.008212814642403124</v>
       </c>
-      <c r="P2">
-        <v>0.1124828577445869</v>
-      </c>
-      <c r="Q2">
-        <v>0.08147170337382224</v>
-      </c>
       <c r="R2">
-        <v>4.497653829707875</v>
+        <v>0.001465289159804688</v>
       </c>
       <c r="S2">
-        <v>2.389176444441049</v>
+        <v>0.0242933467258729</v>
       </c>
     </row>
     <row r="3" spans="1:19">
@@ -2382,55 +2220,55 @@
         <v>710.104</v>
       </c>
       <c r="B3">
-        <v>4.961212533967454</v>
+        <v>0.01952907923740375</v>
+      </c>
+      <c r="C3">
+        <v>0.005000690228146048</v>
       </c>
       <c r="D3">
+        <v>4.222468049465279</v>
+      </c>
+      <c r="E3">
+        <v>1.5464701506389</v>
+      </c>
+      <c r="G3">
         <v>0.6419952810963966</v>
       </c>
-      <c r="E3">
-        <v>6.959182563089944</v>
-      </c>
-      <c r="F3">
-        <v>2.330540908303858</v>
-      </c>
-      <c r="G3">
-        <v>1.042140595617285</v>
-      </c>
       <c r="H3">
-        <v>0.1429654927510638</v>
+        <v>1.411800558539723</v>
       </c>
       <c r="I3">
-        <v>2.619010873400925</v>
+        <v>2.820697070152297</v>
       </c>
       <c r="J3">
-        <v>0.1202849132683757</v>
+        <v>0.2902309780989877</v>
       </c>
       <c r="K3">
-        <v>0.530572759271272</v>
+        <v>0.1474615416379214</v>
       </c>
       <c r="L3">
-        <v>0.02534915275716958</v>
+        <v>0.001138166409084474</v>
       </c>
       <c r="M3">
-        <v>0.4642582614033626</v>
+        <v>0.02663757977267676</v>
       </c>
       <c r="N3">
+        <v>0.003426812157935884</v>
+      </c>
+      <c r="O3">
+        <v>0.007629469904159279</v>
+      </c>
+      <c r="P3">
         <v>0.003685789063810974</v>
       </c>
-      <c r="O3">
+      <c r="Q3">
         <v>0.01282015160987156</v>
       </c>
-      <c r="P3">
-        <v>0.08852755607780817</v>
-      </c>
-      <c r="Q3">
-        <v>0.076160053919179</v>
-      </c>
       <c r="R3">
-        <v>6.818766289144904</v>
+        <v>0.006285148498897456</v>
       </c>
       <c r="S3">
-        <v>0.1751619505126095</v>
+        <v>0.0251569636654362</v>
       </c>
     </row>
     <row r="4" spans="1:19">
@@ -2438,52 +2276,55 @@
         <v>800.131</v>
       </c>
       <c r="B4">
-        <v>4.749561423667795</v>
+        <v>0.0107537697827067</v>
+      </c>
+      <c r="C4">
+        <v>0.008882406404589462</v>
       </c>
       <c r="D4">
+        <v>0.9047262015756741</v>
+      </c>
+      <c r="E4">
+        <v>0.1777086928942029</v>
+      </c>
+      <c r="G4">
         <v>0.8768384162925928</v>
       </c>
-      <c r="E4">
-        <v>3.986254183380136</v>
-      </c>
-      <c r="F4">
-        <v>1.106542119991522</v>
-      </c>
-      <c r="G4">
-        <v>0.5996673779892893</v>
-      </c>
       <c r="H4">
-        <v>0.2452153856524817</v>
+        <v>0.8642736113531588</v>
       </c>
       <c r="I4">
-        <v>2.606056542008332</v>
+        <v>0.8768829408699463</v>
       </c>
       <c r="J4">
-        <v>0.1552053318019095</v>
+        <v>0.2173874418753982</v>
       </c>
       <c r="K4">
-        <v>0.5939310416617086</v>
+        <v>0.2576993286455241</v>
       </c>
       <c r="L4">
-        <v>0.01967055912201143</v>
+        <v>0.02126777453491441</v>
       </c>
       <c r="M4">
-        <v>0.4459142624125887</v>
+        <v>0.03397249450790905</v>
       </c>
       <c r="N4">
+        <v>0.01060902024779602</v>
+      </c>
+      <c r="O4">
+        <v>0.01590067164540986</v>
+      </c>
+      <c r="P4">
         <v>0.009088342074837686</v>
       </c>
-      <c r="O4">
+      <c r="Q4">
         <v>0.01249211973890599</v>
       </c>
-      <c r="P4">
-        <v>0.07747696896596436</v>
-      </c>
-      <c r="Q4">
-        <v>0.05101515963165079</v>
-      </c>
       <c r="R4">
-        <v>3.67225616663221</v>
+        <v>0.009777124905127877</v>
+      </c>
+      <c r="S4">
+        <v>0.01494967008100202</v>
       </c>
     </row>
     <row r="5" spans="1:19">
@@ -2491,58 +2332,58 @@
         <v>905.029</v>
       </c>
       <c r="B5">
-        <v>3.394328361906694</v>
+        <v>0.01060824267020598</v>
       </c>
       <c r="C5">
+        <v>0.01541048549459068</v>
+      </c>
+      <c r="D5">
+        <v>1.64096015005667</v>
+      </c>
+      <c r="E5">
+        <v>1.109291419042228</v>
+      </c>
+      <c r="F5">
         <v>1.47044104470758</v>
       </c>
-      <c r="D5">
+      <c r="G5">
         <v>1.067300279922528</v>
       </c>
-      <c r="E5">
-        <v>7.687068124186458</v>
-      </c>
-      <c r="F5">
-        <v>0.4810428615956892</v>
-      </c>
-      <c r="G5">
-        <v>0.2801927318624694</v>
-      </c>
       <c r="H5">
-        <v>0.6119920286217797</v>
+        <v>3.367423297604404</v>
       </c>
       <c r="I5">
-        <v>1.899183454083217</v>
+        <v>0.2003863478862582</v>
       </c>
       <c r="J5">
-        <v>0.1324200371744105</v>
+        <v>0.5112753114437442</v>
       </c>
       <c r="K5">
-        <v>0.8803236986232265</v>
+        <v>0.6844342124707929</v>
       </c>
       <c r="L5">
-        <v>0.07093282060830981</v>
+        <v>0.1358372905100923</v>
       </c>
       <c r="M5">
-        <v>0.68953012569829</v>
+        <v>0.06249968861821361</v>
       </c>
       <c r="N5">
+        <v>0.01924684005848419</v>
+      </c>
+      <c r="O5">
+        <v>0.02774513187590493</v>
+      </c>
+      <c r="P5">
         <v>0.02844049743334633</v>
       </c>
-      <c r="O5">
+      <c r="Q5">
         <v>0.02898129780539387</v>
       </c>
-      <c r="P5">
-        <v>0.1810888854672414</v>
-      </c>
-      <c r="Q5">
-        <v>0.07914298463203463</v>
-      </c>
       <c r="R5">
-        <v>2.578374138105477</v>
+        <v>0.02025685679291453</v>
       </c>
       <c r="S5">
-        <v>1.447032339310716</v>
+        <v>0.03663053919915115</v>
       </c>
     </row>
     <row r="6" spans="1:19">
@@ -2550,43 +2391,43 @@
         <v>940.061</v>
       </c>
       <c r="B6">
-        <v>2.089110546386839</v>
-      </c>
-      <c r="E6">
-        <v>3.27484646241964</v>
-      </c>
-      <c r="H6">
-        <v>0.4901387526781569</v>
-      </c>
-      <c r="I6">
-        <v>1.595403737920094</v>
+        <v>0.05236407850460666</v>
+      </c>
+      <c r="C6">
+        <v>0.1375730616527762</v>
+      </c>
+      <c r="D6">
+        <v>0.6895442232484918</v>
       </c>
       <c r="J6">
-        <v>2.559981566258668</v>
+        <v>0.1849463706449851</v>
       </c>
       <c r="K6">
-        <v>0.03245120048290794</v>
+        <v>0.11845439687007</v>
       </c>
       <c r="L6">
-        <v>0.1975532595488047</v>
+        <v>2.778038745182362</v>
       </c>
       <c r="M6">
-        <v>0.9585807285128292</v>
+        <v>1.347941958259772</v>
       </c>
       <c r="N6">
+        <v>0.1976109045819472</v>
+      </c>
+      <c r="O6">
+        <v>0.3364300133841509</v>
+      </c>
+      <c r="P6">
         <v>0.09765903269132591</v>
       </c>
-      <c r="O6">
+      <c r="Q6">
         <v>0.1429844332320555</v>
       </c>
-      <c r="P6">
-        <v>0.1223418246211045</v>
-      </c>
-      <c r="Q6">
-        <v>0.05740870400691337</v>
-      </c>
       <c r="R6">
-        <v>1.206525798489109</v>
+        <v>0.125612213006786</v>
+      </c>
+      <c r="S6">
+        <v>0.1630599946910611</v>
       </c>
     </row>
     <row r="7" spans="1:19">
@@ -2594,43 +2435,34 @@
         <v>1000.111</v>
       </c>
       <c r="B7">
-        <v>0.04339928807014247</v>
+        <v>0.3904403477507102</v>
       </c>
       <c r="C7">
+        <v>0.5559656730549188</v>
+      </c>
+      <c r="F7">
         <v>1.141816039754351</v>
       </c>
-      <c r="E7">
-        <v>0.7663485537973792</v>
-      </c>
-      <c r="G7">
-        <v>0.3091430742427847</v>
-      </c>
       <c r="I7">
-        <v>0.8434311858951723</v>
-      </c>
-      <c r="K7">
-        <v>1.26697943793387</v>
-      </c>
-      <c r="L7">
-        <v>1.093228581790163</v>
-      </c>
-      <c r="M7">
-        <v>0.3677491681763419</v>
+        <v>0.3337169775271709</v>
+      </c>
+      <c r="J7">
+        <v>0.2616816606866113</v>
       </c>
       <c r="N7">
+        <v>1.970314835051048</v>
+      </c>
+      <c r="P7">
         <v>1.545934469471649</v>
       </c>
-      <c r="O7">
+      <c r="Q7">
         <v>0.3733519843742963</v>
       </c>
-      <c r="P7">
-        <v>0.8235924988780805</v>
-      </c>
-      <c r="Q7">
-        <v>0.8392524823199595</v>
-      </c>
       <c r="R7">
-        <v>2.611041598220012</v>
+        <v>0.3604795368623867</v>
+      </c>
+      <c r="S7">
+        <v>2.083787280955262</v>
       </c>
     </row>
   </sheetData>
@@ -2814,143 +2646,143 @@
       <c r="A2">
         <v>0</v>
       </c>
+      <c r="B2">
+        <v>-0.0009868510245363523</v>
+      </c>
       <c r="C2">
+        <v>0.002369456689062963</v>
+      </c>
+      <c r="D2">
+        <v>0.321177658068397</v>
+      </c>
+      <c r="E2">
+        <v>0.334610284186732</v>
+      </c>
+      <c r="F2">
+        <v>0.3346329826127608</v>
+      </c>
+      <c r="G2">
+        <v>8.271734338524011</v>
+      </c>
+      <c r="H2">
+        <v>7.212069606881336</v>
+      </c>
+      <c r="J2">
+        <v>10.5908753375122</v>
+      </c>
+      <c r="L2">
         <v>7.064420471035114</v>
       </c>
-      <c r="E2">
+      <c r="N2">
         <v>7.104429508065826</v>
       </c>
-      <c r="F2">
+      <c r="O2">
         <v>6.910254081720142</v>
       </c>
-      <c r="G2">
+      <c r="P2">
         <v>6.72301976646716</v>
       </c>
-      <c r="J2">
+      <c r="S2">
         <v>8.092142994555823</v>
       </c>
-      <c r="L2">
-        <v>-0.0009868510245363523</v>
-      </c>
-      <c r="N2">
+      <c r="V2">
         <v>6.751293942620885</v>
       </c>
-      <c r="O2">
+      <c r="W2">
         <v>7.069335002800199</v>
       </c>
-      <c r="P2">
+      <c r="X2">
         <v>7.646384411928474</v>
       </c>
-      <c r="Q2">
+      <c r="Y2">
         <v>5.781068503813306</v>
       </c>
-      <c r="R2">
+      <c r="Z2">
         <v>6.251196042384491</v>
       </c>
-      <c r="S2">
+      <c r="AA2">
         <v>6.070646474332196</v>
       </c>
-      <c r="T2">
+      <c r="AB2">
         <v>5.647660769122093</v>
       </c>
-      <c r="U2">
+      <c r="AC2">
         <v>6.36142102139537</v>
       </c>
-      <c r="V2">
+      <c r="AD2">
         <v>5.858760701974419</v>
       </c>
-      <c r="W2">
-        <v>0.002369456689062963</v>
-      </c>
-      <c r="X2">
+      <c r="AE2">
         <v>2.160652823311019</v>
       </c>
-      <c r="Y2">
+      <c r="AF2">
         <v>2.194846345568148</v>
       </c>
-      <c r="Z2">
+      <c r="AG2">
         <v>2.221752221235033</v>
       </c>
-      <c r="AA2">
+      <c r="AH2">
         <v>2.445671313876951</v>
       </c>
-      <c r="AB2">
+      <c r="AI2">
         <v>2.494606978787585</v>
       </c>
-      <c r="AC2">
+      <c r="AJ2">
         <v>2.420884934807099</v>
       </c>
-      <c r="AD2">
+      <c r="AK2">
         <v>1.226400344504993</v>
       </c>
-      <c r="AE2">
+      <c r="AL2">
         <v>1.232453988382594</v>
       </c>
-      <c r="AF2">
+      <c r="AM2">
         <v>1.237821799711515</v>
       </c>
-      <c r="AG2">
+      <c r="AN2">
         <v>1.285854664692653</v>
       </c>
-      <c r="AH2">
-        <v>0.321177658068397</v>
-      </c>
-      <c r="AI2">
+      <c r="AO2">
         <v>1.256341272787208</v>
       </c>
-      <c r="AJ2">
+      <c r="AP2">
         <v>1.267245336765769</v>
       </c>
-      <c r="AK2">
+      <c r="AQ2">
         <v>0.7169090825445777</v>
       </c>
-      <c r="AL2">
+      <c r="AR2">
         <v>0.7228491495566002</v>
       </c>
-      <c r="AM2">
+      <c r="AS2">
         <v>0.7030893371885647</v>
       </c>
-      <c r="AN2">
+      <c r="AT2">
         <v>0.7438308805416863</v>
       </c>
-      <c r="AO2">
+      <c r="AU2">
         <v>0.7280710238081137</v>
       </c>
-      <c r="AP2">
+      <c r="AV2">
         <v>0.7319420670612602</v>
       </c>
-      <c r="AQ2">
+      <c r="AW2">
         <v>0.5291258656977472</v>
       </c>
-      <c r="AR2">
+      <c r="AX2">
         <v>0.5297452748983102</v>
       </c>
-      <c r="AS2">
-        <v>0.334610284186732</v>
-      </c>
-      <c r="AT2">
+      <c r="AY2">
         <v>0.5319161883958456</v>
       </c>
-      <c r="AU2">
+      <c r="AZ2">
         <v>0.6854918213014732</v>
       </c>
-      <c r="AV2">
+      <c r="BA2">
         <v>0.6558612851468613</v>
       </c>
-      <c r="AW2">
+      <c r="BB2">
         <v>0.6373295356540289</v>
-      </c>
-      <c r="AX2">
-        <v>0.3346329826127608</v>
-      </c>
-      <c r="AY2">
-        <v>8.271734338524011</v>
-      </c>
-      <c r="AZ2">
-        <v>7.212069606881336</v>
-      </c>
-      <c r="BB2">
-        <v>10.5908753375122</v>
       </c>
     </row>
     <row r="3" spans="1:54">
@@ -2958,148 +2790,148 @@
         <v>0</v>
       </c>
       <c r="B3">
+        <v>0.03527755258783717</v>
+      </c>
+      <c r="C3">
+        <v>0.03215688636863803</v>
+      </c>
+      <c r="D3">
+        <v>0.3521547401396932</v>
+      </c>
+      <c r="E3">
+        <v>0.3422254185756777</v>
+      </c>
+      <c r="F3">
+        <v>0.3461522266550301</v>
+      </c>
+      <c r="G3">
+        <v>12.27497424921892</v>
+      </c>
+      <c r="H3">
+        <v>6.30350266697805</v>
+      </c>
+      <c r="J3">
+        <v>6.551219073004707</v>
+      </c>
+      <c r="K3">
         <v>9.502349937384105</v>
       </c>
-      <c r="C3">
+      <c r="L3">
         <v>7.225017864312048</v>
       </c>
-      <c r="F3">
+      <c r="O3">
         <v>7.02783389743097</v>
       </c>
-      <c r="G3">
+      <c r="P3">
         <v>6.79837156257643</v>
       </c>
-      <c r="H3">
+      <c r="Q3">
         <v>7.7001910655189</v>
       </c>
-      <c r="I3">
+      <c r="R3">
         <v>8.04080832617964</v>
       </c>
-      <c r="K3">
+      <c r="T3">
         <v>9.877047916339993</v>
       </c>
-      <c r="L3">
-        <v>0.03527755258783717</v>
-      </c>
-      <c r="M3">
+      <c r="U3">
         <v>7.880460419087207</v>
       </c>
-      <c r="N3">
+      <c r="V3">
         <v>11.17634297927583</v>
       </c>
-      <c r="P3">
+      <c r="X3">
         <v>7.187274927320402</v>
       </c>
-      <c r="Q3">
+      <c r="Y3">
         <v>5.565268254081594</v>
       </c>
-      <c r="R3">
+      <c r="Z3">
         <v>5.242696790752963</v>
       </c>
-      <c r="S3">
+      <c r="AA3">
         <v>4.986055734295956</v>
       </c>
-      <c r="T3">
+      <c r="AB3">
         <v>5.213947702742479</v>
       </c>
-      <c r="U3">
+      <c r="AC3">
         <v>4.950447934244662</v>
       </c>
-      <c r="V3">
+      <c r="AD3">
         <v>5.196917576111406</v>
       </c>
-      <c r="W3">
-        <v>0.03215688636863803</v>
-      </c>
-      <c r="X3">
+      <c r="AE3">
         <v>1.858502094329916</v>
       </c>
-      <c r="Y3">
+      <c r="AF3">
         <v>1.858708955848912</v>
       </c>
-      <c r="Z3">
+      <c r="AG3">
         <v>1.856642319914637</v>
       </c>
-      <c r="AA3">
+      <c r="AH3">
         <v>2.066007531363974</v>
       </c>
-      <c r="AB3">
+      <c r="AI3">
         <v>2.013633823405331</v>
       </c>
-      <c r="AC3">
+      <c r="AJ3">
         <v>2.031369168381267</v>
       </c>
-      <c r="AD3">
+      <c r="AK3">
         <v>1.103650881377462</v>
       </c>
-      <c r="AE3">
+      <c r="AL3">
         <v>1.107652578497324</v>
       </c>
-      <c r="AF3">
+      <c r="AM3">
         <v>1.110470333450653</v>
       </c>
-      <c r="AG3">
+      <c r="AN3">
         <v>1.15289961092246</v>
       </c>
-      <c r="AH3">
-        <v>0.3521547401396932</v>
-      </c>
-      <c r="AI3">
+      <c r="AO3">
         <v>1.163563588809684</v>
       </c>
-      <c r="AJ3">
+      <c r="AP3">
         <v>1.148779821474097</v>
       </c>
-      <c r="AK3">
+      <c r="AQ3">
         <v>0.6683759443818894</v>
       </c>
-      <c r="AL3">
+      <c r="AR3">
         <v>0.6610043702662816</v>
       </c>
-      <c r="AM3">
+      <c r="AS3">
         <v>0.6646834968210266</v>
       </c>
-      <c r="AN3">
+      <c r="AT3">
         <v>0.6419677404789425</v>
       </c>
-      <c r="AO3">
+      <c r="AU3">
         <v>0.6404484425534448</v>
       </c>
-      <c r="AP3">
+      <c r="AV3">
         <v>0.6633742292551066</v>
       </c>
-      <c r="AQ3">
+      <c r="AW3">
         <v>0.5014537847257093</v>
       </c>
-      <c r="AR3">
+      <c r="AX3">
         <v>0.4888927903535583</v>
       </c>
-      <c r="AS3">
-        <v>0.3422254185756777</v>
-      </c>
-      <c r="AT3">
+      <c r="AY3">
         <v>0.4947545510512887</v>
       </c>
-      <c r="AU3">
+      <c r="AZ3">
         <v>0.6368470240465879</v>
       </c>
-      <c r="AV3">
+      <c r="BA3">
         <v>0.6133229747616171</v>
       </c>
-      <c r="AW3">
+      <c r="BB3">
         <v>0.5865676943124826</v>
-      </c>
-      <c r="AX3">
-        <v>0.3461522266550301</v>
-      </c>
-      <c r="AY3">
-        <v>12.27497424921892</v>
-      </c>
-      <c r="AZ3">
-        <v>6.30350266697805</v>
-      </c>
-      <c r="BB3">
-        <v>6.551219073004707</v>
       </c>
     </row>
     <row r="4" spans="1:54">
@@ -3107,526 +2939,529 @@
         <v>0</v>
       </c>
       <c r="B4">
+        <v>0.02144254092336376</v>
+      </c>
+      <c r="C4">
+        <v>0.01216825791178978</v>
+      </c>
+      <c r="D4">
+        <v>0.3266684479855524</v>
+      </c>
+      <c r="E4">
+        <v>0.3384215441849036</v>
+      </c>
+      <c r="F4">
+        <v>0.3440814590572777</v>
+      </c>
+      <c r="G4">
+        <v>6.791067641750565</v>
+      </c>
+      <c r="I4">
+        <v>8.070543706253178</v>
+      </c>
+      <c r="K4">
         <v>8.349261066076865</v>
       </c>
-      <c r="C4">
+      <c r="L4">
         <v>8.097943022434288</v>
       </c>
-      <c r="D4">
+      <c r="M4">
         <v>7.831310186146149</v>
       </c>
-      <c r="H4">
+      <c r="Q4">
         <v>6.704677473884654</v>
       </c>
-      <c r="I4">
+      <c r="R4">
         <v>5.464640693553923</v>
       </c>
-      <c r="J4">
+      <c r="S4">
         <v>6.704677473884654</v>
       </c>
-      <c r="K4">
+      <c r="T4">
         <v>7.127558030604622</v>
       </c>
-      <c r="L4">
-        <v>0.02144254092336376</v>
-      </c>
-      <c r="M4">
+      <c r="U4">
         <v>5.464640693553923</v>
       </c>
-      <c r="N4">
+      <c r="V4">
         <v>7.538315484663701</v>
       </c>
-      <c r="O4">
+      <c r="W4">
         <v>5.831992439163377</v>
       </c>
-      <c r="P4">
+      <c r="X4">
         <v>6.334273178367257</v>
       </c>
-      <c r="Q4">
+      <c r="Y4">
         <v>5.201134398847057</v>
       </c>
-      <c r="R4">
+      <c r="Z4">
         <v>5.427409397771441</v>
       </c>
-      <c r="S4">
+      <c r="AA4">
         <v>4.992757328963292</v>
       </c>
-      <c r="T4">
+      <c r="AB4">
         <v>5.26283146579071</v>
       </c>
-      <c r="U4">
+      <c r="AC4">
         <v>4.773271159006398</v>
       </c>
-      <c r="V4">
+      <c r="AD4">
         <v>5.15760367342838</v>
       </c>
-      <c r="W4">
-        <v>0.01216825791178978</v>
-      </c>
-      <c r="X4">
+      <c r="AE4">
         <v>1.865189578994434</v>
       </c>
-      <c r="Y4">
+      <c r="AF4">
         <v>1.828300269739079</v>
       </c>
-      <c r="Z4">
+      <c r="AG4">
         <v>1.82840538107907</v>
       </c>
-      <c r="AA4">
+      <c r="AH4">
         <v>2.09717633028342</v>
       </c>
-      <c r="AB4">
+      <c r="AI4">
         <v>2.048277982571045</v>
       </c>
-      <c r="AC4">
+      <c r="AJ4">
         <v>2.113581835994198</v>
       </c>
-      <c r="AD4">
+      <c r="AK4">
         <v>1.053766922316019</v>
       </c>
-      <c r="AE4">
+      <c r="AL4">
         <v>1.032792623102875</v>
       </c>
-      <c r="AF4">
+      <c r="AM4">
         <v>1.046057003568155</v>
       </c>
-      <c r="AG4">
+      <c r="AN4">
         <v>1.071500268853276</v>
       </c>
-      <c r="AH4">
-        <v>0.3266684479855524</v>
-      </c>
-      <c r="AI4">
+      <c r="AO4">
         <v>1.098304388054219</v>
       </c>
-      <c r="AJ4">
+      <c r="AP4">
         <v>1.099722870674653</v>
       </c>
-      <c r="AK4">
+      <c r="AQ4">
         <v>0.612302942770254</v>
       </c>
-      <c r="AL4">
+      <c r="AR4">
         <v>0.6113415128449541</v>
       </c>
-      <c r="AM4">
+      <c r="AS4">
         <v>0.6275416624151797</v>
       </c>
-      <c r="AN4">
+      <c r="AT4">
         <v>0.6280608853753045</v>
       </c>
-      <c r="AO4">
+      <c r="AU4">
         <v>0.6056226521514031</v>
       </c>
-      <c r="AP4">
+      <c r="AV4">
         <v>0.6073258119509334</v>
       </c>
-      <c r="AQ4">
+      <c r="AW4">
         <v>0.4714676797787611</v>
       </c>
-      <c r="AR4">
+      <c r="AX4">
         <v>0.473734774891326</v>
       </c>
-      <c r="AS4">
-        <v>0.3384215441849036</v>
-      </c>
-      <c r="AT4">
+      <c r="AY4">
         <v>0.4557809501659731</v>
       </c>
-      <c r="AU4">
+      <c r="AZ4">
         <v>0.5505601740692386</v>
       </c>
-      <c r="AV4">
+      <c r="BA4">
         <v>0.5358862093517571</v>
       </c>
-      <c r="AW4">
+      <c r="BB4">
         <v>0.5206625184892706</v>
-      </c>
-      <c r="AX4">
-        <v>0.3440814590572777</v>
-      </c>
-      <c r="AY4">
-        <v>6.791067641750565</v>
-      </c>
-      <c r="BA4">
-        <v>8.070543706253178</v>
       </c>
     </row>
     <row r="5" spans="1:54">
       <c r="A5">
         <v>0</v>
       </c>
+      <c r="B5">
+        <v>-0.002197188214864343</v>
+      </c>
       <c r="C5">
+        <v>0.01717662711178382</v>
+      </c>
+      <c r="D5">
+        <v>0.4330045164129592</v>
+      </c>
+      <c r="E5">
+        <v>0.4194023158881378</v>
+      </c>
+      <c r="F5">
+        <v>0.4501551237138702</v>
+      </c>
+      <c r="G5">
+        <v>5.084954748651293</v>
+      </c>
+      <c r="H5">
+        <v>7.873189521189055</v>
+      </c>
+      <c r="I5">
+        <v>4.979885428025235</v>
+      </c>
+      <c r="J5">
+        <v>6.369080173989713</v>
+      </c>
+      <c r="L5">
         <v>4.800305204556098</v>
       </c>
-      <c r="D5">
+      <c r="M5">
         <v>7.733427455026388</v>
       </c>
-      <c r="E5">
+      <c r="N5">
         <v>5.653909786930866</v>
       </c>
-      <c r="G5">
+      <c r="P5">
         <v>6.31501058852859</v>
       </c>
-      <c r="I5">
+      <c r="R5">
         <v>7.82440111951963</v>
       </c>
-      <c r="J5">
+      <c r="S5">
         <v>10.86895880789553</v>
       </c>
-      <c r="L5">
-        <v>-0.002197188214864343</v>
-      </c>
-      <c r="M5">
+      <c r="U5">
         <v>6.106703110172253</v>
       </c>
-      <c r="N5">
+      <c r="V5">
         <v>5.426405771220866</v>
       </c>
-      <c r="P5">
+      <c r="X5">
         <v>5.709794862116025</v>
       </c>
-      <c r="Q5">
+      <c r="Y5">
         <v>5.151761973549949</v>
       </c>
-      <c r="R5">
+      <c r="Z5">
         <v>5.475201074491629</v>
       </c>
-      <c r="S5">
+      <c r="AA5">
         <v>4.473393615964602</v>
       </c>
-      <c r="T5">
+      <c r="AB5">
         <v>5.606150901558078</v>
       </c>
-      <c r="U5">
+      <c r="AC5">
         <v>4.638214755729734</v>
       </c>
-      <c r="W5">
-        <v>0.01717662711178382</v>
-      </c>
-      <c r="X5">
+      <c r="AE5">
         <v>2.703027625310849</v>
       </c>
-      <c r="Y5">
+      <c r="AF5">
         <v>2.930760140926376</v>
       </c>
-      <c r="Z5">
+      <c r="AG5">
         <v>2.688602283713438</v>
       </c>
-      <c r="AA5">
+      <c r="AH5">
         <v>2.902551432941729</v>
       </c>
-      <c r="AB5">
+      <c r="AI5">
         <v>3.014641172775545</v>
       </c>
-      <c r="AC5">
+      <c r="AJ5">
         <v>3.006508210565505</v>
       </c>
-      <c r="AD5">
+      <c r="AK5">
         <v>1.485825586319976</v>
       </c>
-      <c r="AE5">
+      <c r="AL5">
         <v>1.516244937192256</v>
       </c>
-      <c r="AF5">
+      <c r="AM5">
         <v>1.480606853201056</v>
       </c>
-      <c r="AG5">
+      <c r="AN5">
         <v>1.61734536519812</v>
       </c>
-      <c r="AH5">
-        <v>0.4330045164129592</v>
-      </c>
-      <c r="AI5">
+      <c r="AO5">
         <v>1.599121438917284</v>
       </c>
-      <c r="AJ5">
+      <c r="AP5">
         <v>1.653623857129413</v>
       </c>
-      <c r="AK5">
+      <c r="AQ5">
         <v>0.9548702762228773</v>
       </c>
-      <c r="AL5">
+      <c r="AR5">
         <v>0.8999113875581437</v>
       </c>
-      <c r="AM5">
+      <c r="AS5">
         <v>0.9146933478751004</v>
       </c>
-      <c r="AN5">
+      <c r="AT5">
         <v>0.8517684037259662</v>
       </c>
-      <c r="AO5">
+      <c r="AU5">
         <v>0.8866381500159414</v>
       </c>
-      <c r="AP5">
+      <c r="AV5">
         <v>0.909300938432563</v>
       </c>
-      <c r="AQ5">
+      <c r="AW5">
         <v>0.7123219342604135</v>
       </c>
-      <c r="AR5">
+      <c r="AX5">
         <v>0.7503292663184096</v>
       </c>
-      <c r="AS5">
-        <v>0.4194023158881378</v>
-      </c>
-      <c r="AT5">
+      <c r="AY5">
         <v>0.7191764120959206</v>
       </c>
-      <c r="AU5">
+      <c r="AZ5">
         <v>0.876046724803855</v>
       </c>
-      <c r="AV5">
+      <c r="BA5">
         <v>0.8159040475761727</v>
       </c>
-      <c r="AW5">
+      <c r="BB5">
         <v>0.8097464890500682</v>
-      </c>
-      <c r="AX5">
-        <v>0.4501551237138702</v>
-      </c>
-      <c r="AY5">
-        <v>5.084954748651293</v>
-      </c>
-      <c r="AZ5">
-        <v>7.873189521189055</v>
-      </c>
-      <c r="BA5">
-        <v>4.979885428025235</v>
-      </c>
-      <c r="BB5">
-        <v>6.369080173989713</v>
       </c>
     </row>
     <row r="6" spans="1:54">
       <c r="A6">
         <v>0</v>
       </c>
+      <c r="B6">
+        <v>-0.09135310030747056</v>
+      </c>
       <c r="C6">
+        <v>-0.09002684272401879</v>
+      </c>
+      <c r="D6">
+        <v>0.8021053032240173</v>
+      </c>
+      <c r="E6">
+        <v>0.8049390032478694</v>
+      </c>
+      <c r="F6">
+        <v>0.5652512580647395</v>
+      </c>
+      <c r="G6">
+        <v>2.950981637531783</v>
+      </c>
+      <c r="I6">
+        <v>3.926144429905822</v>
+      </c>
+      <c r="L6">
         <v>2.954448467996935</v>
       </c>
-      <c r="F6">
+      <c r="O6">
         <v>4.074205015550776</v>
       </c>
-      <c r="I6">
+      <c r="R6">
         <v>4.084900767120548</v>
       </c>
-      <c r="K6">
+      <c r="T6">
         <v>4.539979181535936</v>
       </c>
-      <c r="L6">
-        <v>-0.09135310030747056</v>
-      </c>
-      <c r="N6">
+      <c r="V6">
         <v>4.022377200407783</v>
       </c>
-      <c r="R6">
+      <c r="Z6">
         <v>3.402521651905551</v>
       </c>
-      <c r="S6">
+      <c r="AA6">
         <v>3.140967986227732</v>
       </c>
-      <c r="T6">
+      <c r="AB6">
         <v>2.198895888689364</v>
       </c>
-      <c r="U6">
+      <c r="AC6">
         <v>2.435234019039055</v>
       </c>
-      <c r="V6">
+      <c r="AD6">
         <v>2.331296908075263</v>
       </c>
-      <c r="W6">
-        <v>-0.09002684272401879</v>
-      </c>
-      <c r="X6">
+      <c r="AE6">
         <v>2.920310762152936</v>
       </c>
-      <c r="Y6">
+      <c r="AF6">
         <v>7.518939402927136</v>
       </c>
-      <c r="Z6">
+      <c r="AG6">
         <v>2.519262370349024</v>
       </c>
-      <c r="AA6">
+      <c r="AH6">
         <v>4.063622453503275</v>
       </c>
-      <c r="AC6">
+      <c r="AJ6">
         <v>2.157344654840557</v>
       </c>
-      <c r="AD6">
+      <c r="AK6">
         <v>2.111451727002341</v>
       </c>
-      <c r="AE6">
+      <c r="AL6">
         <v>2.278687789603264</v>
       </c>
-      <c r="AF6">
+      <c r="AM6">
         <v>1.884949969586585</v>
       </c>
-      <c r="AG6">
+      <c r="AN6">
         <v>2.053362458677017</v>
       </c>
-      <c r="AH6">
-        <v>0.8021053032240173</v>
-      </c>
-      <c r="AI6">
+      <c r="AO6">
         <v>2.666722014784512</v>
       </c>
-      <c r="AJ6">
+      <c r="AP6">
         <v>2.120463433587223</v>
       </c>
-      <c r="AK6">
+      <c r="AQ6">
         <v>1.498975224973961</v>
       </c>
-      <c r="AL6">
+      <c r="AR6">
         <v>1.525262779930308</v>
       </c>
-      <c r="AM6">
+      <c r="AS6">
         <v>1.344507596696353</v>
       </c>
-      <c r="AN6">
+      <c r="AT6">
         <v>1.351480374278677</v>
       </c>
-      <c r="AO6">
+      <c r="AU6">
         <v>1.632340245672732</v>
       </c>
-      <c r="AP6">
+      <c r="AV6">
         <v>1.44530619083949</v>
       </c>
-      <c r="AQ6">
+      <c r="AW6">
         <v>1.045232090138032</v>
       </c>
-      <c r="AR6">
+      <c r="AX6">
         <v>0.9650479096043314</v>
       </c>
-      <c r="AS6">
-        <v>0.8049390032478694</v>
-      </c>
-      <c r="AT6">
+      <c r="AY6">
         <v>1.211327189248919</v>
       </c>
-      <c r="AU6">
+      <c r="AZ6">
         <v>1.232226114806656</v>
       </c>
-      <c r="AV6">
+      <c r="BA6">
         <v>1.124002912863534</v>
       </c>
-      <c r="AW6">
+      <c r="BB6">
         <v>1.444538029176422</v>
-      </c>
-      <c r="AX6">
-        <v>0.5652512580647395</v>
-      </c>
-      <c r="AY6">
-        <v>2.950981637531783</v>
-      </c>
-      <c r="BA6">
-        <v>3.926144429905822</v>
       </c>
     </row>
     <row r="7" spans="1:54">
       <c r="A7">
         <v>0</v>
       </c>
+      <c r="B7">
+        <v>-0.671928862221308</v>
+      </c>
       <c r="C7">
+        <v>-0.6805144253648557</v>
+      </c>
+      <c r="D7">
+        <v>-0.3249956860581171</v>
+      </c>
+      <c r="E7">
+        <v>0.7059425900298402</v>
+      </c>
+      <c r="F7">
+        <v>-0.1703148405331999</v>
+      </c>
+      <c r="I7">
+        <v>-0.3158057714911197</v>
+      </c>
+      <c r="L7">
         <v>-0.06137586178613235</v>
       </c>
-      <c r="D7">
+      <c r="M7">
         <v>-0.5408314587042193</v>
       </c>
-      <c r="E7">
+      <c r="N7">
         <v>1.137402760159347</v>
       </c>
-      <c r="F7">
+      <c r="O7">
         <v>1.63950861351096</v>
       </c>
-      <c r="H7">
+      <c r="Q7">
         <v>-0.2390797690709351</v>
       </c>
-      <c r="J7">
+      <c r="S7">
         <v>0.4118516560639531</v>
       </c>
-      <c r="L7">
-        <v>-0.671928862221308</v>
-      </c>
-      <c r="O7">
+      <c r="W7">
         <v>0.5929122917618943</v>
       </c>
-      <c r="P7">
+      <c r="X7">
         <v>0.1209652161488118</v>
       </c>
-      <c r="Q7">
+      <c r="Y7">
         <v>-0.493014994593176</v>
       </c>
-      <c r="R7">
+      <c r="Z7">
         <v>-0.122941241025856</v>
       </c>
-      <c r="T7">
+      <c r="AB7">
         <v>1.576328019305107</v>
       </c>
-      <c r="W7">
-        <v>-0.6805144253648557</v>
-      </c>
-      <c r="X7">
+      <c r="AE7">
         <v>0.5122773966565201</v>
       </c>
-      <c r="AB7">
+      <c r="AI7">
         <v>1.47916257078485</v>
       </c>
-      <c r="AD7">
+      <c r="AK7">
         <v>3.270942075158769</v>
       </c>
-      <c r="AE7">
+      <c r="AL7">
         <v>0.4844961132846687</v>
       </c>
-      <c r="AG7">
+      <c r="AN7">
         <v>-1.061562573856884</v>
       </c>
-      <c r="AH7">
-        <v>-0.3249956860581171</v>
-      </c>
-      <c r="AJ7">
+      <c r="AO7" t="s">
+        <v>91</v>
+      </c>
+      <c r="AP7">
         <v>0.1950801751282898</v>
       </c>
-      <c r="AK7">
+      <c r="AQ7">
         <v>1.941795893156639</v>
       </c>
-      <c r="AL7">
+      <c r="AR7">
         <v>-0.4878460368354194</v>
       </c>
-      <c r="AM7">
+      <c r="AS7">
         <v>-0.929035404150185</v>
       </c>
-      <c r="AN7">
+      <c r="AT7">
         <v>-0.8492497444352084</v>
       </c>
-      <c r="AO7">
+      <c r="AU7">
         <v>-0.2357515893246583</v>
       </c>
-      <c r="AP7">
+      <c r="AV7">
         <v>-0.1738678916609658</v>
       </c>
-      <c r="AQ7">
+      <c r="AW7">
         <v>-0.9054192978874812</v>
       </c>
-      <c r="AR7">
+      <c r="AX7">
         <v>-0.3956242478987219</v>
       </c>
-      <c r="AS7">
-        <v>0.7059425900298402</v>
-      </c>
-      <c r="AU7">
+      <c r="AZ7">
         <v>0.6559292138648641</v>
       </c>
-      <c r="AV7">
+      <c r="BA7">
         <v>-0.5309530288873089</v>
       </c>
-      <c r="AW7">
+      <c r="BB7">
         <v>3.522255599589863</v>
-      </c>
-      <c r="AX7">
-        <v>-0.1703148405331999</v>
-      </c>
-      <c r="BA7">
-        <v>-0.3158057714911197</v>
       </c>
     </row>
   </sheetData>
@@ -3703,249 +3538,279 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>6.598723444337138</v>
+        <v>0.3296603191407701</v>
       </c>
       <c r="C2">
-        <v>8.884159523040678</v>
+        <v>7.607194817490235</v>
       </c>
       <c r="D2">
-        <v>-0.0004172162342559312</v>
+        <v>7.728122933146121</v>
       </c>
       <c r="E2">
-        <v>6.765654001771132</v>
+        <v>7.002176291537233</v>
       </c>
       <c r="F2">
-        <v>5.204651650960755</v>
+        <v>6.722559889533247</v>
       </c>
       <c r="G2">
-        <v>4.884641120545216</v>
+        <v>8.091683117621908</v>
       </c>
       <c r="H2">
-        <v>-0.1094488539841212</v>
+        <v>7.090444231679342</v>
       </c>
       <c r="I2">
-        <v>1.182726835982149</v>
+        <v>6.014854420229931</v>
       </c>
       <c r="J2">
-        <v>0.7663907023045956</v>
+        <v>5.913124903788237</v>
       </c>
       <c r="K2">
-        <v>0.1532117890172575</v>
+        <v>2.191644330379332</v>
       </c>
       <c r="L2">
-        <v>-0.2558102287752875</v>
+        <v>2.452793943130414</v>
       </c>
       <c r="M2">
-        <v>-0.3842968663169468</v>
+        <v>1.231754615517668</v>
       </c>
       <c r="N2">
-        <v>-0.3639528848287876</v>
+        <v>1.269279739142317</v>
       </c>
       <c r="O2">
-        <v>-0.6383553051475742</v>
+        <v>0.7137883422623288</v>
       </c>
       <c r="P2">
-        <v>-0.4763628617916895</v>
+        <v>0.734132323750488</v>
       </c>
       <c r="Q2">
-        <v>-0.2187138375021365</v>
+        <v>0.5298018505347537</v>
       </c>
       <c r="R2">
-        <v>7.570386879942415</v>
+        <v>0.6589046466138117</v>
       </c>
     </row>
     <row r="3" spans="1:18">
       <c r="A3">
         <v>0</v>
       </c>
+      <c r="B3">
+        <v>0.3244852376837802</v>
+      </c>
       <c r="C3">
-        <v>6.271780151670569</v>
+        <v>6.971752051114541</v>
       </c>
       <c r="D3">
-        <v>0.03706672439305822</v>
+        <v>7.181482420175956</v>
       </c>
       <c r="E3">
-        <v>9.877343231792514</v>
+        <v>7.005483339446334</v>
       </c>
       <c r="F3">
-        <v>4.618988756214164</v>
+        <v>7.347239388767625</v>
       </c>
       <c r="G3">
-        <v>3.945712769717209</v>
+        <v>8.423921638456504</v>
       </c>
       <c r="H3">
-        <v>-0.1212330266058801</v>
+        <v>7.839723938535279</v>
       </c>
       <c r="I3">
-        <v>0.8246039988091252</v>
+        <v>5.214740225814023</v>
       </c>
       <c r="J3">
-        <v>0.5177861770497234</v>
+        <v>5.090650467891878</v>
       </c>
       <c r="K3">
-        <v>0.02565122775383427</v>
+        <v>1.835600133481228</v>
       </c>
       <c r="L3">
-        <v>-0.2863036854331391</v>
+        <v>2.014417079891322</v>
       </c>
       <c r="M3">
-        <v>-0.4331263862571195</v>
+        <v>1.084903458018339</v>
       </c>
       <c r="N3">
-        <v>-0.4492676426338248</v>
+        <v>1.132711065673662</v>
       </c>
       <c r="O3">
-        <v>-0.6562732179565456</v>
+        <v>0.6423328508399366</v>
       </c>
       <c r="P3">
-        <v>-0.5181260864112246</v>
+        <v>0.6261915944632312</v>
       </c>
       <c r="Q3">
-        <v>-0.2331960362859314</v>
+        <v>0.4726699849059673</v>
       </c>
       <c r="R3">
-        <v>5.935172216695203</v>
+        <v>0.5896842798574651</v>
       </c>
     </row>
     <row r="4" spans="1:18">
       <c r="A4">
         <v>0</v>
       </c>
+      <c r="B4">
+        <v>0.3251991258713444</v>
+      </c>
       <c r="C4">
-        <v>5.565809084746518</v>
+        <v>7.227610240861648</v>
       </c>
       <c r="D4">
-        <v>0.01991347682875193</v>
+        <v>8.204562606124053</v>
       </c>
       <c r="E4">
-        <v>4.867285377018603</v>
+        <v>7.820145152460407</v>
       </c>
       <c r="F4">
-        <v>4.450485493009343</v>
+        <v>5.892466341169427</v>
       </c>
       <c r="G4">
-        <v>3.89177004226206</v>
+        <v>6.160749714194783</v>
       </c>
       <c r="H4">
-        <v>-0.1379403579662106</v>
+        <v>6.339080013451767</v>
       </c>
       <c r="I4">
-        <v>0.8121138850871681</v>
+        <v>5.180290929122628</v>
       </c>
       <c r="J4">
-        <v>0.5140643372696264</v>
+        <v>5.030508234322499</v>
       </c>
       <c r="K4">
-        <v>-0.04808378973576734</v>
+        <v>1.829316559547337</v>
       </c>
       <c r="L4">
-        <v>-0.3271230992658724</v>
+        <v>2.074793805046334</v>
       </c>
       <c r="M4">
-        <v>-0.4810371449659721</v>
+        <v>1.033002932219159</v>
       </c>
       <c r="N4">
-        <v>-0.4844538108027234</v>
+        <v>1.078592944592312</v>
       </c>
       <c r="O4">
-        <v>-0.6722266870790489</v>
+        <v>0.6058695207428427</v>
       </c>
       <c r="P4">
-        <v>-0.5848709751656606</v>
+        <v>0.6024528549060915</v>
       </c>
       <c r="Q4">
-        <v>-0.2649892346223947</v>
+        <v>0.4557975144415266</v>
+      </c>
+      <c r="R4">
+        <v>0.524463430635795</v>
       </c>
     </row>
     <row r="5" spans="1:18">
       <c r="A5">
         <v>0</v>
       </c>
+      <c r="B5">
+        <v>0.4291524978073202</v>
+      </c>
+      <c r="C5">
+        <v>5.40281683288105</v>
+      </c>
       <c r="D5">
-        <v>0.006765284640481984</v>
+        <v>5.299282098401393</v>
       </c>
       <c r="E5">
-        <v>5.505016448308531</v>
+        <v>6.22432668209168</v>
       </c>
       <c r="F5">
-        <v>4.327506516657974</v>
+        <v>6.803495292740686</v>
       </c>
       <c r="G5">
-        <v>3.705487872823189</v>
+        <v>6.786384585995152</v>
       </c>
       <c r="H5">
-        <v>-0.04049432212510903</v>
+        <v>5.553139349503119</v>
       </c>
       <c r="I5">
-        <v>1.742956991232057</v>
+        <v>4.938623207221142</v>
       </c>
       <c r="J5">
-        <v>1.131322023186363</v>
+        <v>5.004419677264226</v>
       </c>
       <c r="K5">
-        <v>0.4447021149396336</v>
+        <v>2.763191183787661</v>
       </c>
       <c r="L5">
-        <v>-0.03422062996650074</v>
+        <v>2.968294235586116</v>
       </c>
       <c r="M5">
-        <v>-0.1688139227339628</v>
+        <v>1.489147027617968</v>
       </c>
       <c r="N5">
-        <v>-0.2094150438340742</v>
+        <v>1.618152000468391</v>
       </c>
       <c r="O5">
-        <v>-0.4756130125365335</v>
+        <v>0.9179340666752709</v>
       </c>
       <c r="P5">
-        <v>-0.2900938267263956</v>
+        <v>0.8773329455751595</v>
       </c>
       <c r="Q5">
-        <v>-0.07806587869010696</v>
+        <v>0.7221838528578617</v>
       </c>
       <c r="R5">
-        <v>4.720844772482351</v>
+        <v>0.8284992157943516</v>
       </c>
     </row>
     <row r="6" spans="1:18">
       <c r="A6">
         <v>0</v>
       </c>
+      <c r="B6">
+        <v>0.7789980830304857</v>
+      </c>
+      <c r="C6">
+        <v>3.385491074810341</v>
+      </c>
       <c r="D6">
-        <v>-0.06095323466960551</v>
+        <v>3.015813041263556</v>
+      </c>
+      <c r="E6">
+        <v>4.135569588817398</v>
+      </c>
+      <c r="F6">
+        <v>4.14626534038717</v>
       </c>
       <c r="G6">
-        <v>1.446307218087942</v>
+        <v>4.601343754802558</v>
       </c>
       <c r="H6">
-        <v>-0.1929384571511742</v>
+        <v>4.083741773674405</v>
       </c>
       <c r="I6">
-        <v>2.346687143862821</v>
+        <v>3.324582366591025</v>
       </c>
       <c r="J6">
-        <v>1.481270643051965</v>
+        <v>2.378479853025953</v>
       </c>
       <c r="K6">
-        <v>0.9873053382228408</v>
+        <v>3.162615780609991</v>
       </c>
       <c r="L6">
-        <v>0.4760985904094073</v>
+        <v>2.773284218380979</v>
       </c>
       <c r="M6">
-        <v>0.3808350503168544</v>
+        <v>2.139960449682975</v>
       </c>
       <c r="N6">
-        <v>0.3974905629490362</v>
+        <v>2.306440842563572</v>
       </c>
       <c r="O6">
-        <v>-0.138821827589935</v>
+        <v>1.514381750740383</v>
       </c>
       <c r="P6">
-        <v>0.1158946490706902</v>
+        <v>1.531037263372565</v>
       </c>
       <c r="Q6">
-        <v>0.1814937492750197</v>
+        <v>1.130052175388308</v>
+      </c>
+      <c r="R6">
+        <v>1.319589466339948</v>
       </c>
     </row>
     <row r="7" spans="1:18">
@@ -3953,40 +3818,55 @@
         <v>0</v>
       </c>
       <c r="B7">
-        <v>-0.5637876112982098</v>
+        <v>0.4764201009792872</v>
+      </c>
+      <c r="C7">
+        <v>0.1815097644601263</v>
       </c>
       <c r="D7">
-        <v>-0.2943940900936612</v>
+        <v>0.4359396741651137</v>
+      </c>
+      <c r="E7">
+        <v>0.7929579290142199</v>
       </c>
       <c r="F7">
-        <v>-1.056675155008143</v>
+        <v>0.2582357668803111</v>
+      </c>
+      <c r="G7">
+        <v>0.9091671920151991</v>
       </c>
       <c r="H7">
-        <v>-0.2616978585268205</v>
+        <v>0.8266671493369104</v>
+      </c>
+      <c r="I7">
+        <v>0.1723149028879223</v>
       </c>
       <c r="J7">
-        <v>3.915099249005633</v>
+        <v>2.073643555256353</v>
       </c>
       <c r="K7">
-        <v>-0.9850107357573641</v>
+        <v>1.009592932607766</v>
       </c>
       <c r="L7">
-        <v>-0.552358211575849</v>
+        <v>1.976478106736096</v>
       </c>
       <c r="M7">
-        <v>-1.220435895200582</v>
+        <v>1.615144045812054</v>
       </c>
       <c r="N7">
-        <v>-1.328109915194899</v>
+        <v>0.2839116960081089</v>
       </c>
       <c r="O7">
-        <v>-1.254153802146641</v>
+        <v>0.1363096451118474</v>
       </c>
       <c r="P7">
-        <v>-0.2717627788550755</v>
+        <v>0.02863562511753045</v>
       </c>
       <c r="Q7">
-        <v>3.136752930077993</v>
+        <v>-0.1853468002619424</v>
+      </c>
+      <c r="R7">
+        <v>0.7854223332927206</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed wavelengths not appearing on absorbance worksheets & data frames.
</commit_message>
<xml_diff>
--- a/combined_dataframes.xlsx
+++ b/combined_dataframes.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="91">
   <si>
     <t>Wavelength</t>
   </si>
@@ -291,9 +291,6 @@
   </si>
   <si>
     <t>STDMaterial_18</t>
-  </si>
-  <si>
-    <t>inf</t>
   </si>
 </sst>
 </file>
@@ -651,7 +648,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S7"/>
+  <dimension ref="A1:S6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1011,65 +1008,6 @@
         <v>275.8496933333333</v>
       </c>
     </row>
-    <row r="7" spans="1:19">
-      <c r="A7">
-        <v>1000.111</v>
-      </c>
-      <c r="B7">
-        <v>68.44456666666666</v>
-      </c>
-      <c r="C7">
-        <v>42.50425</v>
-      </c>
-      <c r="D7">
-        <v>57.08346</v>
-      </c>
-      <c r="E7">
-        <v>44.26014</v>
-      </c>
-      <c r="F7">
-        <v>30.97146333333333</v>
-      </c>
-      <c r="G7">
-        <v>52.86748</v>
-      </c>
-      <c r="H7">
-        <v>27.57355</v>
-      </c>
-      <c r="I7">
-        <v>29.94484</v>
-      </c>
-      <c r="J7">
-        <v>57.610755</v>
-      </c>
-      <c r="K7">
-        <v>8.605320000000001</v>
-      </c>
-      <c r="L7">
-        <v>24.93896</v>
-      </c>
-      <c r="M7">
-        <v>9.48343</v>
-      </c>
-      <c r="N7">
-        <v>13.611025</v>
-      </c>
-      <c r="O7">
-        <v>51.52733666666666</v>
-      </c>
-      <c r="P7">
-        <v>59.72284</v>
-      </c>
-      <c r="Q7">
-        <v>66.51241</v>
-      </c>
-      <c r="R7">
-        <v>82.38233</v>
-      </c>
-      <c r="S7">
-        <v>31.20573333333333</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1077,7 +1015,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BC7"/>
+  <dimension ref="A1:BC6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1977,119 +1915,6 @@
         <v>228.95901</v>
       </c>
     </row>
-    <row r="7" spans="1:55">
-      <c r="A7">
-        <v>1000.111</v>
-      </c>
-      <c r="B7">
-        <v>41.62532</v>
-      </c>
-      <c r="C7">
-        <v>81.50281</v>
-      </c>
-      <c r="D7">
-        <v>82.20556999999999</v>
-      </c>
-      <c r="E7">
-        <v>57.61047</v>
-      </c>
-      <c r="F7">
-        <v>20.54805</v>
-      </c>
-      <c r="G7">
-        <v>49.35423</v>
-      </c>
-      <c r="J7">
-        <v>57.08346</v>
-      </c>
-      <c r="M7">
-        <v>44.26014</v>
-      </c>
-      <c r="N7">
-        <v>71.48875</v>
-      </c>
-      <c r="O7">
-        <v>13.34719</v>
-      </c>
-      <c r="P7">
-        <v>8.07845</v>
-      </c>
-      <c r="R7">
-        <v>52.86748</v>
-      </c>
-      <c r="T7">
-        <v>27.57355</v>
-      </c>
-      <c r="X7">
-        <v>23.00695</v>
-      </c>
-      <c r="Y7">
-        <v>36.88273</v>
-      </c>
-      <c r="Z7">
-        <v>68.15085000000001</v>
-      </c>
-      <c r="AA7">
-        <v>47.07066</v>
-      </c>
-      <c r="AC7">
-        <v>8.605320000000001</v>
-      </c>
-      <c r="AF7">
-        <v>24.93896</v>
-      </c>
-      <c r="AJ7">
-        <v>9.48343</v>
-      </c>
-      <c r="AL7">
-        <v>1.58054</v>
-      </c>
-      <c r="AM7">
-        <v>25.64151</v>
-      </c>
-      <c r="AO7">
-        <v>120.334</v>
-      </c>
-      <c r="AP7">
-        <v>0</v>
-      </c>
-      <c r="AQ7">
-        <v>34.24801</v>
-      </c>
-      <c r="AR7">
-        <v>5.97099</v>
-      </c>
-      <c r="AS7">
-        <v>67.79949000000001</v>
-      </c>
-      <c r="AT7">
-        <v>105.39804</v>
-      </c>
-      <c r="AU7">
-        <v>97.31551</v>
-      </c>
-      <c r="AV7">
-        <v>52.69182</v>
-      </c>
-      <c r="AW7">
-        <v>49.5299</v>
-      </c>
-      <c r="AX7">
-        <v>102.93811</v>
-      </c>
-      <c r="AY7">
-        <v>61.82655</v>
-      </c>
-      <c r="BA7">
-        <v>21.60186</v>
-      </c>
-      <c r="BB7">
-        <v>70.78603</v>
-      </c>
-      <c r="BC7">
-        <v>1.22931</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2097,7 +1922,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S7"/>
+  <dimension ref="A1:S6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2164,7 +1989,7 @@
     </row>
     <row r="2" spans="1:19">
       <c r="A2">
-        <v>630.188</v>
+        <v>0</v>
       </c>
       <c r="B2">
         <v>0.001724963836062461</v>
@@ -2217,7 +2042,7 @@
     </row>
     <row r="3" spans="1:19">
       <c r="A3">
-        <v>710.104</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>0.01952907923740375</v>
@@ -2273,7 +2098,7 @@
     </row>
     <row r="4" spans="1:19">
       <c r="A4">
-        <v>800.131</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>0.0107537697827067</v>
@@ -2329,7 +2154,7 @@
     </row>
     <row r="5" spans="1:19">
       <c r="A5">
-        <v>905.029</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>0.01060824267020598</v>
@@ -2388,7 +2213,7 @@
     </row>
     <row r="6" spans="1:19">
       <c r="A6">
-        <v>940.061</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>0.05236407850460666</v>
@@ -2428,41 +2253,6 @@
       </c>
       <c r="S6">
         <v>0.1630599946910611</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19">
-      <c r="A7">
-        <v>1000.111</v>
-      </c>
-      <c r="B7">
-        <v>0.3904403477507102</v>
-      </c>
-      <c r="C7">
-        <v>0.5559656730549188</v>
-      </c>
-      <c r="F7">
-        <v>1.141816039754351</v>
-      </c>
-      <c r="I7">
-        <v>0.3337169775271709</v>
-      </c>
-      <c r="J7">
-        <v>0.2616816606866113</v>
-      </c>
-      <c r="N7">
-        <v>1.970314835051048</v>
-      </c>
-      <c r="P7">
-        <v>1.545934469471649</v>
-      </c>
-      <c r="Q7">
-        <v>0.3733519843742963</v>
-      </c>
-      <c r="R7">
-        <v>0.3604795368623867</v>
-      </c>
-      <c r="S7">
-        <v>2.083787280955262</v>
       </c>
     </row>
   </sheetData>
@@ -2472,996 +2262,904 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BB7"/>
+  <dimension ref="A1:BC6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:54">
+    <row r="1" spans="1:55">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AR1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="AR1" s="1" t="s">
+      <c r="AS1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="AS1" s="1" t="s">
+      <c r="AT1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="AT1" s="1" t="s">
+      <c r="AU1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="AU1" s="1" t="s">
+      <c r="AV1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="AV1" s="1" t="s">
+      <c r="AW1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="AW1" s="1" t="s">
+      <c r="AX1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="AX1" s="1" t="s">
+      <c r="AY1" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="AY1" s="1" t="s">
+      <c r="AZ1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="AZ1" s="1" t="s">
+      <c r="BA1" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="BA1" s="1" t="s">
+      <c r="BB1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="BB1" s="1" t="s">
+      <c r="BC1" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:54">
+    <row r="2" spans="1:55">
       <c r="A2">
+        <v>630.188</v>
+      </c>
+      <c r="B2">
         <v>0</v>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>-0.0009868510245363523</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>0.002369456689062963</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>0.321177658068397</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>0.334610284186732</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>0.3346329826127608</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>8.271734338524011</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>7.212069606881336</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>10.5908753375122</v>
       </c>
-      <c r="L2">
+      <c r="M2">
         <v>7.064420471035114</v>
       </c>
-      <c r="N2">
+      <c r="O2">
         <v>7.104429508065826</v>
       </c>
-      <c r="O2">
+      <c r="P2">
         <v>6.910254081720142</v>
       </c>
-      <c r="P2">
+      <c r="Q2">
         <v>6.72301976646716</v>
       </c>
-      <c r="S2">
+      <c r="T2">
         <v>8.092142994555823</v>
       </c>
-      <c r="V2">
+      <c r="W2">
         <v>6.751293942620885</v>
       </c>
-      <c r="W2">
+      <c r="X2">
         <v>7.069335002800199</v>
       </c>
-      <c r="X2">
+      <c r="Y2">
         <v>7.646384411928474</v>
       </c>
-      <c r="Y2">
+      <c r="Z2">
         <v>5.781068503813306</v>
       </c>
-      <c r="Z2">
+      <c r="AA2">
         <v>6.251196042384491</v>
       </c>
-      <c r="AA2">
+      <c r="AB2">
         <v>6.070646474332196</v>
       </c>
-      <c r="AB2">
+      <c r="AC2">
         <v>5.647660769122093</v>
       </c>
-      <c r="AC2">
+      <c r="AD2">
         <v>6.36142102139537</v>
       </c>
-      <c r="AD2">
+      <c r="AE2">
         <v>5.858760701974419</v>
       </c>
-      <c r="AE2">
+      <c r="AF2">
         <v>2.160652823311019</v>
       </c>
-      <c r="AF2">
+      <c r="AG2">
         <v>2.194846345568148</v>
       </c>
-      <c r="AG2">
+      <c r="AH2">
         <v>2.221752221235033</v>
       </c>
-      <c r="AH2">
+      <c r="AI2">
         <v>2.445671313876951</v>
       </c>
-      <c r="AI2">
+      <c r="AJ2">
         <v>2.494606978787585</v>
       </c>
-      <c r="AJ2">
+      <c r="AK2">
         <v>2.420884934807099</v>
       </c>
-      <c r="AK2">
+      <c r="AL2">
         <v>1.226400344504993</v>
       </c>
-      <c r="AL2">
+      <c r="AM2">
         <v>1.232453988382594</v>
       </c>
-      <c r="AM2">
+      <c r="AN2">
         <v>1.237821799711515</v>
       </c>
-      <c r="AN2">
+      <c r="AO2">
         <v>1.285854664692653</v>
       </c>
-      <c r="AO2">
+      <c r="AP2">
         <v>1.256341272787208</v>
       </c>
-      <c r="AP2">
+      <c r="AQ2">
         <v>1.267245336765769</v>
       </c>
-      <c r="AQ2">
+      <c r="AR2">
         <v>0.7169090825445777</v>
       </c>
-      <c r="AR2">
+      <c r="AS2">
         <v>0.7228491495566002</v>
       </c>
-      <c r="AS2">
+      <c r="AT2">
         <v>0.7030893371885647</v>
       </c>
-      <c r="AT2">
+      <c r="AU2">
         <v>0.7438308805416863</v>
       </c>
-      <c r="AU2">
+      <c r="AV2">
         <v>0.7280710238081137</v>
       </c>
-      <c r="AV2">
+      <c r="AW2">
         <v>0.7319420670612602</v>
       </c>
-      <c r="AW2">
+      <c r="AX2">
         <v>0.5291258656977472</v>
       </c>
-      <c r="AX2">
+      <c r="AY2">
         <v>0.5297452748983102</v>
       </c>
-      <c r="AY2">
+      <c r="AZ2">
         <v>0.5319161883958456</v>
       </c>
-      <c r="AZ2">
+      <c r="BA2">
         <v>0.6854918213014732</v>
       </c>
-      <c r="BA2">
+      <c r="BB2">
         <v>0.6558612851468613</v>
       </c>
-      <c r="BB2">
+      <c r="BC2">
         <v>0.6373295356540289</v>
       </c>
     </row>
-    <row r="3" spans="1:54">
+    <row r="3" spans="1:55">
       <c r="A3">
+        <v>710.104</v>
+      </c>
+      <c r="B3">
         <v>0</v>
       </c>
-      <c r="B3">
+      <c r="C3">
         <v>0.03527755258783717</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>0.03215688636863803</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>0.3521547401396932</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>0.3422254185756777</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>0.3461522266550301</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>12.27497424921892</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>6.30350266697805</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>6.551219073004707</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <v>9.502349937384105</v>
       </c>
-      <c r="L3">
+      <c r="M3">
         <v>7.225017864312048</v>
       </c>
-      <c r="O3">
+      <c r="P3">
         <v>7.02783389743097</v>
       </c>
-      <c r="P3">
+      <c r="Q3">
         <v>6.79837156257643</v>
       </c>
-      <c r="Q3">
+      <c r="R3">
         <v>7.7001910655189</v>
       </c>
-      <c r="R3">
+      <c r="S3">
         <v>8.04080832617964</v>
       </c>
-      <c r="T3">
+      <c r="U3">
         <v>9.877047916339993</v>
       </c>
-      <c r="U3">
+      <c r="V3">
         <v>7.880460419087207</v>
       </c>
-      <c r="V3">
+      <c r="W3">
         <v>11.17634297927583</v>
       </c>
-      <c r="X3">
+      <c r="Y3">
         <v>7.187274927320402</v>
       </c>
-      <c r="Y3">
+      <c r="Z3">
         <v>5.565268254081594</v>
       </c>
-      <c r="Z3">
+      <c r="AA3">
         <v>5.242696790752963</v>
       </c>
-      <c r="AA3">
+      <c r="AB3">
         <v>4.986055734295956</v>
       </c>
-      <c r="AB3">
+      <c r="AC3">
         <v>5.213947702742479</v>
       </c>
-      <c r="AC3">
+      <c r="AD3">
         <v>4.950447934244662</v>
       </c>
-      <c r="AD3">
+      <c r="AE3">
         <v>5.196917576111406</v>
       </c>
-      <c r="AE3">
+      <c r="AF3">
         <v>1.858502094329916</v>
       </c>
-      <c r="AF3">
+      <c r="AG3">
         <v>1.858708955848912</v>
       </c>
-      <c r="AG3">
+      <c r="AH3">
         <v>1.856642319914637</v>
       </c>
-      <c r="AH3">
+      <c r="AI3">
         <v>2.066007531363974</v>
       </c>
-      <c r="AI3">
+      <c r="AJ3">
         <v>2.013633823405331</v>
       </c>
-      <c r="AJ3">
+      <c r="AK3">
         <v>2.031369168381267</v>
       </c>
-      <c r="AK3">
+      <c r="AL3">
         <v>1.103650881377462</v>
       </c>
-      <c r="AL3">
+      <c r="AM3">
         <v>1.107652578497324</v>
       </c>
-      <c r="AM3">
+      <c r="AN3">
         <v>1.110470333450653</v>
       </c>
-      <c r="AN3">
+      <c r="AO3">
         <v>1.15289961092246</v>
       </c>
-      <c r="AO3">
+      <c r="AP3">
         <v>1.163563588809684</v>
       </c>
-      <c r="AP3">
+      <c r="AQ3">
         <v>1.148779821474097</v>
       </c>
-      <c r="AQ3">
+      <c r="AR3">
         <v>0.6683759443818894</v>
       </c>
-      <c r="AR3">
+      <c r="AS3">
         <v>0.6610043702662816</v>
       </c>
-      <c r="AS3">
+      <c r="AT3">
         <v>0.6646834968210266</v>
       </c>
-      <c r="AT3">
+      <c r="AU3">
         <v>0.6419677404789425</v>
       </c>
-      <c r="AU3">
+      <c r="AV3">
         <v>0.6404484425534448</v>
       </c>
-      <c r="AV3">
+      <c r="AW3">
         <v>0.6633742292551066</v>
       </c>
-      <c r="AW3">
+      <c r="AX3">
         <v>0.5014537847257093</v>
       </c>
-      <c r="AX3">
+      <c r="AY3">
         <v>0.4888927903535583</v>
       </c>
-      <c r="AY3">
+      <c r="AZ3">
         <v>0.4947545510512887</v>
       </c>
-      <c r="AZ3">
+      <c r="BA3">
         <v>0.6368470240465879</v>
       </c>
-      <c r="BA3">
+      <c r="BB3">
         <v>0.6133229747616171</v>
       </c>
-      <c r="BB3">
+      <c r="BC3">
         <v>0.5865676943124826</v>
       </c>
     </row>
-    <row r="4" spans="1:54">
+    <row r="4" spans="1:55">
       <c r="A4">
+        <v>800.131</v>
+      </c>
+      <c r="B4">
         <v>0</v>
       </c>
-      <c r="B4">
+      <c r="C4">
         <v>0.02144254092336376</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>0.01216825791178978</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>0.3266684479855524</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>0.3384215441849036</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>0.3440814590572777</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>6.791067641750565</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>8.070543706253178</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>8.349261066076865</v>
       </c>
-      <c r="L4">
+      <c r="M4">
         <v>8.097943022434288</v>
       </c>
-      <c r="M4">
+      <c r="N4">
         <v>7.831310186146149</v>
       </c>
-      <c r="Q4">
+      <c r="R4">
         <v>6.704677473884654</v>
       </c>
-      <c r="R4">
+      <c r="S4">
         <v>5.464640693553923</v>
       </c>
-      <c r="S4">
+      <c r="T4">
         <v>6.704677473884654</v>
       </c>
-      <c r="T4">
+      <c r="U4">
         <v>7.127558030604622</v>
       </c>
-      <c r="U4">
+      <c r="V4">
         <v>5.464640693553923</v>
       </c>
-      <c r="V4">
+      <c r="W4">
         <v>7.538315484663701</v>
       </c>
-      <c r="W4">
+      <c r="X4">
         <v>5.831992439163377</v>
       </c>
-      <c r="X4">
+      <c r="Y4">
         <v>6.334273178367257</v>
       </c>
-      <c r="Y4">
+      <c r="Z4">
         <v>5.201134398847057</v>
       </c>
-      <c r="Z4">
+      <c r="AA4">
         <v>5.427409397771441</v>
       </c>
-      <c r="AA4">
+      <c r="AB4">
         <v>4.992757328963292</v>
       </c>
-      <c r="AB4">
+      <c r="AC4">
         <v>5.26283146579071</v>
       </c>
-      <c r="AC4">
+      <c r="AD4">
         <v>4.773271159006398</v>
       </c>
-      <c r="AD4">
+      <c r="AE4">
         <v>5.15760367342838</v>
       </c>
-      <c r="AE4">
+      <c r="AF4">
         <v>1.865189578994434</v>
       </c>
-      <c r="AF4">
+      <c r="AG4">
         <v>1.828300269739079</v>
       </c>
-      <c r="AG4">
+      <c r="AH4">
         <v>1.82840538107907</v>
       </c>
-      <c r="AH4">
+      <c r="AI4">
         <v>2.09717633028342</v>
       </c>
-      <c r="AI4">
+      <c r="AJ4">
         <v>2.048277982571045</v>
       </c>
-      <c r="AJ4">
+      <c r="AK4">
         <v>2.113581835994198</v>
       </c>
-      <c r="AK4">
+      <c r="AL4">
         <v>1.053766922316019</v>
       </c>
-      <c r="AL4">
+      <c r="AM4">
         <v>1.032792623102875</v>
       </c>
-      <c r="AM4">
+      <c r="AN4">
         <v>1.046057003568155</v>
       </c>
-      <c r="AN4">
+      <c r="AO4">
         <v>1.071500268853276</v>
       </c>
-      <c r="AO4">
+      <c r="AP4">
         <v>1.098304388054219</v>
       </c>
-      <c r="AP4">
+      <c r="AQ4">
         <v>1.099722870674653</v>
       </c>
-      <c r="AQ4">
+      <c r="AR4">
         <v>0.612302942770254</v>
       </c>
-      <c r="AR4">
+      <c r="AS4">
         <v>0.6113415128449541</v>
       </c>
-      <c r="AS4">
+      <c r="AT4">
         <v>0.6275416624151797</v>
       </c>
-      <c r="AT4">
+      <c r="AU4">
         <v>0.6280608853753045</v>
       </c>
-      <c r="AU4">
+      <c r="AV4">
         <v>0.6056226521514031</v>
       </c>
-      <c r="AV4">
+      <c r="AW4">
         <v>0.6073258119509334</v>
       </c>
-      <c r="AW4">
+      <c r="AX4">
         <v>0.4714676797787611</v>
       </c>
-      <c r="AX4">
+      <c r="AY4">
         <v>0.473734774891326</v>
       </c>
-      <c r="AY4">
+      <c r="AZ4">
         <v>0.4557809501659731</v>
       </c>
-      <c r="AZ4">
+      <c r="BA4">
         <v>0.5505601740692386</v>
       </c>
-      <c r="BA4">
+      <c r="BB4">
         <v>0.5358862093517571</v>
       </c>
-      <c r="BB4">
+      <c r="BC4">
         <v>0.5206625184892706</v>
       </c>
     </row>
-    <row r="5" spans="1:54">
+    <row r="5" spans="1:55">
       <c r="A5">
+        <v>905.029</v>
+      </c>
+      <c r="B5">
         <v>0</v>
       </c>
-      <c r="B5">
+      <c r="C5">
         <v>-0.002197188214864343</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>0.01717662711178382</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>0.4330045164129592</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>0.4194023158881378</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>0.4501551237138702</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>5.084954748651293</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>7.873189521189055</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>4.979885428025235</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>6.369080173989713</v>
       </c>
-      <c r="L5">
+      <c r="M5">
         <v>4.800305204556098</v>
       </c>
-      <c r="M5">
+      <c r="N5">
         <v>7.733427455026388</v>
       </c>
-      <c r="N5">
+      <c r="O5">
         <v>5.653909786930866</v>
       </c>
-      <c r="P5">
+      <c r="Q5">
         <v>6.31501058852859</v>
       </c>
-      <c r="R5">
+      <c r="S5">
         <v>7.82440111951963</v>
       </c>
-      <c r="S5">
+      <c r="T5">
         <v>10.86895880789553</v>
       </c>
-      <c r="U5">
+      <c r="V5">
         <v>6.106703110172253</v>
       </c>
-      <c r="V5">
+      <c r="W5">
         <v>5.426405771220866</v>
       </c>
-      <c r="X5">
+      <c r="Y5">
         <v>5.709794862116025</v>
       </c>
-      <c r="Y5">
+      <c r="Z5">
         <v>5.151761973549949</v>
       </c>
-      <c r="Z5">
+      <c r="AA5">
         <v>5.475201074491629</v>
       </c>
-      <c r="AA5">
+      <c r="AB5">
         <v>4.473393615964602</v>
       </c>
-      <c r="AB5">
+      <c r="AC5">
         <v>5.606150901558078</v>
       </c>
-      <c r="AC5">
+      <c r="AD5">
         <v>4.638214755729734</v>
       </c>
-      <c r="AE5">
+      <c r="AF5">
         <v>2.703027625310849</v>
       </c>
-      <c r="AF5">
+      <c r="AG5">
         <v>2.930760140926376</v>
       </c>
-      <c r="AG5">
+      <c r="AH5">
         <v>2.688602283713438</v>
       </c>
-      <c r="AH5">
+      <c r="AI5">
         <v>2.902551432941729</v>
       </c>
-      <c r="AI5">
+      <c r="AJ5">
         <v>3.014641172775545</v>
       </c>
-      <c r="AJ5">
+      <c r="AK5">
         <v>3.006508210565505</v>
       </c>
-      <c r="AK5">
+      <c r="AL5">
         <v>1.485825586319976</v>
       </c>
-      <c r="AL5">
+      <c r="AM5">
         <v>1.516244937192256</v>
       </c>
-      <c r="AM5">
+      <c r="AN5">
         <v>1.480606853201056</v>
       </c>
-      <c r="AN5">
+      <c r="AO5">
         <v>1.61734536519812</v>
       </c>
-      <c r="AO5">
+      <c r="AP5">
         <v>1.599121438917284</v>
       </c>
-      <c r="AP5">
+      <c r="AQ5">
         <v>1.653623857129413</v>
       </c>
-      <c r="AQ5">
+      <c r="AR5">
         <v>0.9548702762228773</v>
       </c>
-      <c r="AR5">
+      <c r="AS5">
         <v>0.8999113875581437</v>
       </c>
-      <c r="AS5">
+      <c r="AT5">
         <v>0.9146933478751004</v>
       </c>
-      <c r="AT5">
+      <c r="AU5">
         <v>0.8517684037259662</v>
       </c>
-      <c r="AU5">
+      <c r="AV5">
         <v>0.8866381500159414</v>
       </c>
-      <c r="AV5">
+      <c r="AW5">
         <v>0.909300938432563</v>
       </c>
-      <c r="AW5">
+      <c r="AX5">
         <v>0.7123219342604135</v>
       </c>
-      <c r="AX5">
+      <c r="AY5">
         <v>0.7503292663184096</v>
       </c>
-      <c r="AY5">
+      <c r="AZ5">
         <v>0.7191764120959206</v>
       </c>
-      <c r="AZ5">
+      <c r="BA5">
         <v>0.876046724803855</v>
       </c>
-      <c r="BA5">
+      <c r="BB5">
         <v>0.8159040475761727</v>
       </c>
-      <c r="BB5">
+      <c r="BC5">
         <v>0.8097464890500682</v>
       </c>
     </row>
-    <row r="6" spans="1:54">
+    <row r="6" spans="1:55">
       <c r="A6">
+        <v>940.061</v>
+      </c>
+      <c r="B6">
         <v>0</v>
       </c>
-      <c r="B6">
+      <c r="C6">
         <v>-0.09135310030747056</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>-0.09002684272401879</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>0.8021053032240173</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>0.8049390032478694</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>0.5652512580647395</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>2.950981637531783</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>3.926144429905822</v>
       </c>
-      <c r="L6">
+      <c r="M6">
         <v>2.954448467996935</v>
       </c>
-      <c r="O6">
+      <c r="P6">
         <v>4.074205015550776</v>
       </c>
-      <c r="R6">
+      <c r="S6">
         <v>4.084900767120548</v>
       </c>
-      <c r="T6">
+      <c r="U6">
         <v>4.539979181535936</v>
       </c>
-      <c r="V6">
+      <c r="W6">
         <v>4.022377200407783</v>
       </c>
-      <c r="Z6">
+      <c r="AA6">
         <v>3.402521651905551</v>
       </c>
-      <c r="AA6">
+      <c r="AB6">
         <v>3.140967986227732</v>
       </c>
-      <c r="AB6">
+      <c r="AC6">
         <v>2.198895888689364</v>
       </c>
-      <c r="AC6">
+      <c r="AD6">
         <v>2.435234019039055</v>
       </c>
-      <c r="AD6">
+      <c r="AE6">
         <v>2.331296908075263</v>
       </c>
-      <c r="AE6">
+      <c r="AF6">
         <v>2.920310762152936</v>
       </c>
-      <c r="AF6">
+      <c r="AG6">
         <v>7.518939402927136</v>
       </c>
-      <c r="AG6">
+      <c r="AH6">
         <v>2.519262370349024</v>
       </c>
-      <c r="AH6">
+      <c r="AI6">
         <v>4.063622453503275</v>
       </c>
-      <c r="AJ6">
+      <c r="AK6">
         <v>2.157344654840557</v>
       </c>
-      <c r="AK6">
+      <c r="AL6">
         <v>2.111451727002341</v>
       </c>
-      <c r="AL6">
+      <c r="AM6">
         <v>2.278687789603264</v>
       </c>
-      <c r="AM6">
+      <c r="AN6">
         <v>1.884949969586585</v>
       </c>
-      <c r="AN6">
+      <c r="AO6">
         <v>2.053362458677017</v>
       </c>
-      <c r="AO6">
+      <c r="AP6">
         <v>2.666722014784512</v>
       </c>
-      <c r="AP6">
+      <c r="AQ6">
         <v>2.120463433587223</v>
       </c>
-      <c r="AQ6">
+      <c r="AR6">
         <v>1.498975224973961</v>
       </c>
-      <c r="AR6">
+      <c r="AS6">
         <v>1.525262779930308</v>
       </c>
-      <c r="AS6">
+      <c r="AT6">
         <v>1.344507596696353</v>
       </c>
-      <c r="AT6">
+      <c r="AU6">
         <v>1.351480374278677</v>
       </c>
-      <c r="AU6">
+      <c r="AV6">
         <v>1.632340245672732</v>
       </c>
-      <c r="AV6">
+      <c r="AW6">
         <v>1.44530619083949</v>
       </c>
-      <c r="AW6">
+      <c r="AX6">
         <v>1.045232090138032</v>
       </c>
-      <c r="AX6">
+      <c r="AY6">
         <v>0.9650479096043314</v>
       </c>
-      <c r="AY6">
+      <c r="AZ6">
         <v>1.211327189248919</v>
       </c>
-      <c r="AZ6">
+      <c r="BA6">
         <v>1.232226114806656</v>
       </c>
-      <c r="BA6">
+      <c r="BB6">
         <v>1.124002912863534</v>
       </c>
-      <c r="BB6">
+      <c r="BC6">
         <v>1.444538029176422</v>
-      </c>
-    </row>
-    <row r="7" spans="1:54">
-      <c r="A7">
-        <v>0</v>
-      </c>
-      <c r="B7">
-        <v>-0.671928862221308</v>
-      </c>
-      <c r="C7">
-        <v>-0.6805144253648557</v>
-      </c>
-      <c r="D7">
-        <v>-0.3249956860581171</v>
-      </c>
-      <c r="E7">
-        <v>0.7059425900298402</v>
-      </c>
-      <c r="F7">
-        <v>-0.1703148405331999</v>
-      </c>
-      <c r="I7">
-        <v>-0.3158057714911197</v>
-      </c>
-      <c r="L7">
-        <v>-0.06137586178613235</v>
-      </c>
-      <c r="M7">
-        <v>-0.5408314587042193</v>
-      </c>
-      <c r="N7">
-        <v>1.137402760159347</v>
-      </c>
-      <c r="O7">
-        <v>1.63950861351096</v>
-      </c>
-      <c r="Q7">
-        <v>-0.2390797690709351</v>
-      </c>
-      <c r="S7">
-        <v>0.4118516560639531</v>
-      </c>
-      <c r="W7">
-        <v>0.5929122917618943</v>
-      </c>
-      <c r="X7">
-        <v>0.1209652161488118</v>
-      </c>
-      <c r="Y7">
-        <v>-0.493014994593176</v>
-      </c>
-      <c r="Z7">
-        <v>-0.122941241025856</v>
-      </c>
-      <c r="AB7">
-        <v>1.576328019305107</v>
-      </c>
-      <c r="AE7">
-        <v>0.5122773966565201</v>
-      </c>
-      <c r="AI7">
-        <v>1.47916257078485</v>
-      </c>
-      <c r="AK7">
-        <v>3.270942075158769</v>
-      </c>
-      <c r="AL7">
-        <v>0.4844961132846687</v>
-      </c>
-      <c r="AN7">
-        <v>-1.061562573856884</v>
-      </c>
-      <c r="AO7" t="s">
-        <v>91</v>
-      </c>
-      <c r="AP7">
-        <v>0.1950801751282898</v>
-      </c>
-      <c r="AQ7">
-        <v>1.941795893156639</v>
-      </c>
-      <c r="AR7">
-        <v>-0.4878460368354194</v>
-      </c>
-      <c r="AS7">
-        <v>-0.929035404150185</v>
-      </c>
-      <c r="AT7">
-        <v>-0.8492497444352084</v>
-      </c>
-      <c r="AU7">
-        <v>-0.2357515893246583</v>
-      </c>
-      <c r="AV7">
-        <v>-0.1738678916609658</v>
-      </c>
-      <c r="AW7">
-        <v>-0.9054192978874812</v>
-      </c>
-      <c r="AX7">
-        <v>-0.3956242478987219</v>
-      </c>
-      <c r="AZ7">
-        <v>0.6559292138648641</v>
-      </c>
-      <c r="BA7">
-        <v>-0.5309530288873089</v>
-      </c>
-      <c r="BB7">
-        <v>3.522255599589863</v>
       </c>
     </row>
   </sheetData>
@@ -3471,402 +3169,364 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R7"/>
+  <dimension ref="A1:S6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:19">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:19">
       <c r="A2">
+        <v>630.188</v>
+      </c>
+      <c r="B2">
         <v>0</v>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>0.3296603191407701</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>7.607194817490235</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>7.728122933146121</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>7.002176291537233</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>6.722559889533247</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>8.091683117621908</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>7.090444231679342</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>6.014854420229931</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>5.913124903788237</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <v>2.191644330379332</v>
       </c>
-      <c r="L2">
+      <c r="M2">
         <v>2.452793943130414</v>
       </c>
-      <c r="M2">
+      <c r="N2">
         <v>1.231754615517668</v>
       </c>
-      <c r="N2">
+      <c r="O2">
         <v>1.269279739142317</v>
       </c>
-      <c r="O2">
+      <c r="P2">
         <v>0.7137883422623288</v>
       </c>
-      <c r="P2">
+      <c r="Q2">
         <v>0.734132323750488</v>
       </c>
-      <c r="Q2">
+      <c r="R2">
         <v>0.5298018505347537</v>
       </c>
-      <c r="R2">
+      <c r="S2">
         <v>0.6589046466138117</v>
       </c>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:19">
       <c r="A3">
+        <v>710.104</v>
+      </c>
+      <c r="B3">
         <v>0</v>
       </c>
-      <c r="B3">
+      <c r="C3">
         <v>0.3244852376837802</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>6.971752051114541</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>7.181482420175956</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>7.005483339446334</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>7.347239388767625</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>8.423921638456504</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>7.839723938535279</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>5.214740225814023</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>5.090650467891878</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <v>1.835600133481228</v>
       </c>
-      <c r="L3">
+      <c r="M3">
         <v>2.014417079891322</v>
       </c>
-      <c r="M3">
+      <c r="N3">
         <v>1.084903458018339</v>
       </c>
-      <c r="N3">
+      <c r="O3">
         <v>1.132711065673662</v>
       </c>
-      <c r="O3">
+      <c r="P3">
         <v>0.6423328508399366</v>
       </c>
-      <c r="P3">
+      <c r="Q3">
         <v>0.6261915944632312</v>
       </c>
-      <c r="Q3">
+      <c r="R3">
         <v>0.4726699849059673</v>
       </c>
-      <c r="R3">
+      <c r="S3">
         <v>0.5896842798574651</v>
       </c>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:19">
       <c r="A4">
+        <v>800.131</v>
+      </c>
+      <c r="B4">
         <v>0</v>
       </c>
-      <c r="B4">
+      <c r="C4">
         <v>0.3251991258713444</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>7.227610240861648</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>8.204562606124053</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>7.820145152460407</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>5.892466341169427</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>6.160749714194783</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>6.339080013451767</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>5.180290929122628</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>5.030508234322499</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>1.829316559547337</v>
       </c>
-      <c r="L4">
+      <c r="M4">
         <v>2.074793805046334</v>
       </c>
-      <c r="M4">
+      <c r="N4">
         <v>1.033002932219159</v>
       </c>
-      <c r="N4">
+      <c r="O4">
         <v>1.078592944592312</v>
       </c>
-      <c r="O4">
+      <c r="P4">
         <v>0.6058695207428427</v>
       </c>
-      <c r="P4">
+      <c r="Q4">
         <v>0.6024528549060915</v>
       </c>
-      <c r="Q4">
+      <c r="R4">
         <v>0.4557975144415266</v>
       </c>
-      <c r="R4">
+      <c r="S4">
         <v>0.524463430635795</v>
       </c>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:19">
       <c r="A5">
+        <v>905.029</v>
+      </c>
+      <c r="B5">
         <v>0</v>
       </c>
-      <c r="B5">
+      <c r="C5">
         <v>0.4291524978073202</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>5.40281683288105</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>5.299282098401393</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>6.22432668209168</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>6.803495292740686</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>6.786384585995152</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>5.553139349503119</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>4.938623207221142</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>5.004419677264226</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <v>2.763191183787661</v>
       </c>
-      <c r="L5">
+      <c r="M5">
         <v>2.968294235586116</v>
       </c>
-      <c r="M5">
+      <c r="N5">
         <v>1.489147027617968</v>
       </c>
-      <c r="N5">
+      <c r="O5">
         <v>1.618152000468391</v>
       </c>
-      <c r="O5">
+      <c r="P5">
         <v>0.9179340666752709</v>
       </c>
-      <c r="P5">
+      <c r="Q5">
         <v>0.8773329455751595</v>
       </c>
-      <c r="Q5">
+      <c r="R5">
         <v>0.7221838528578617</v>
       </c>
-      <c r="R5">
+      <c r="S5">
         <v>0.8284992157943516</v>
       </c>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:19">
       <c r="A6">
+        <v>940.061</v>
+      </c>
+      <c r="B6">
         <v>0</v>
       </c>
-      <c r="B6">
+      <c r="C6">
         <v>0.7789980830304857</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>3.385491074810341</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>3.015813041263556</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>4.135569588817398</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>4.14626534038717</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>4.601343754802558</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>4.083741773674405</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>3.324582366591025</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>2.378479853025953</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <v>3.162615780609991</v>
       </c>
-      <c r="L6">
+      <c r="M6">
         <v>2.773284218380979</v>
       </c>
-      <c r="M6">
+      <c r="N6">
         <v>2.139960449682975</v>
       </c>
-      <c r="N6">
+      <c r="O6">
         <v>2.306440842563572</v>
       </c>
-      <c r="O6">
+      <c r="P6">
         <v>1.514381750740383</v>
       </c>
-      <c r="P6">
+      <c r="Q6">
         <v>1.531037263372565</v>
       </c>
-      <c r="Q6">
+      <c r="R6">
         <v>1.130052175388308</v>
       </c>
-      <c r="R6">
+      <c r="S6">
         <v>1.319589466339948</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18">
-      <c r="A7">
-        <v>0</v>
-      </c>
-      <c r="B7">
-        <v>0.4764201009792872</v>
-      </c>
-      <c r="C7">
-        <v>0.1815097644601263</v>
-      </c>
-      <c r="D7">
-        <v>0.4359396741651137</v>
-      </c>
-      <c r="E7">
-        <v>0.7929579290142199</v>
-      </c>
-      <c r="F7">
-        <v>0.2582357668803111</v>
-      </c>
-      <c r="G7">
-        <v>0.9091671920151991</v>
-      </c>
-      <c r="H7">
-        <v>0.8266671493369104</v>
-      </c>
-      <c r="I7">
-        <v>0.1723149028879223</v>
-      </c>
-      <c r="J7">
-        <v>2.073643555256353</v>
-      </c>
-      <c r="K7">
-        <v>1.009592932607766</v>
-      </c>
-      <c r="L7">
-        <v>1.976478106736096</v>
-      </c>
-      <c r="M7">
-        <v>1.615144045812054</v>
-      </c>
-      <c r="N7">
-        <v>0.2839116960081089</v>
-      </c>
-      <c r="O7">
-        <v>0.1363096451118474</v>
-      </c>
-      <c r="P7">
-        <v>0.02863562511753045</v>
-      </c>
-      <c r="Q7">
-        <v>-0.1853468002619424</v>
-      </c>
-      <c r="R7">
-        <v>0.7854223332927206</v>
       </c>
     </row>
   </sheetData>

</xml_diff>